<commit_message>
update shipping instruction template add gross weight and volume column in shipping instruction table populate gross weight and volume in BL show BL with Telex Release document in customer booking view
</commit_message>
<xml_diff>
--- a/public/template/shipping_instruction_template.xlsx
+++ b/public/template/shipping_instruction_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A21BD93-2C40-40CD-A92D-0EFDCF8ADA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE307A1-D81F-4073-B831-E78688DECD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{378D42B6-8EFA-4EF6-9C50-436D539EEED8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{378D42B6-8EFA-4EF6-9C50-436D539EEED8}"/>
   </bookViews>
   <sheets>
     <sheet name="BillOfLading" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
-  <si>
-    <t>MEARSK</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>METAL SCRAP</t>
   </si>
@@ -45,9 +42,6 @@
     <t>SEAL001</t>
   </si>
   <si>
-    <t>20GP</t>
-  </si>
-  <si>
     <t>SEAL002</t>
   </si>
   <si>
@@ -60,21 +54,6 @@
     <t>SEAL005</t>
   </si>
   <si>
-    <t>TEMU1172001</t>
-  </si>
-  <si>
-    <t>TEMU1172002</t>
-  </si>
-  <si>
-    <t>TEMU1172003</t>
-  </si>
-  <si>
-    <t>TEMU1172004</t>
-  </si>
-  <si>
-    <t>TEMU1172005</t>
-  </si>
-  <si>
     <t>BOX OPERATOR</t>
   </si>
   <si>
@@ -151,6 +130,54 @@
   </si>
   <si>
     <t>50350 KUALA LUMPUR,</t>
+  </si>
+  <si>
+    <t>SEAL006</t>
+  </si>
+  <si>
+    <t>SEAL007</t>
+  </si>
+  <si>
+    <t>SEAL008</t>
+  </si>
+  <si>
+    <t>SEAL009</t>
+  </si>
+  <si>
+    <t>TEMU1172101</t>
+  </si>
+  <si>
+    <t>TEMU1172102</t>
+  </si>
+  <si>
+    <t>TEMU1172103</t>
+  </si>
+  <si>
+    <t>TEMU1172104</t>
+  </si>
+  <si>
+    <t>TEMU1172105</t>
+  </si>
+  <si>
+    <t>TEMU1172106</t>
+  </si>
+  <si>
+    <t>TEMU1172107</t>
+  </si>
+  <si>
+    <t>TEMU1172108</t>
+  </si>
+  <si>
+    <t>TEMU1172109</t>
+  </si>
+  <si>
+    <t>40HC</t>
+  </si>
+  <si>
+    <t>EVERGREEN</t>
+  </si>
+  <si>
+    <t>GROSS WEIGHT (KGS)</t>
   </si>
 </sst>
 </file>
@@ -260,7 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -299,16 +326,23 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -339,8 +373,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2600324</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -357,8 +391,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6518274" y="203200"/>
-          <a:ext cx="4324350" cy="1530350"/>
+          <a:off x="6229349" y="209550"/>
+          <a:ext cx="4819651" cy="1581150"/>
           <a:chOff x="6029324" y="276225"/>
           <a:chExt cx="4238625" cy="1390650"/>
         </a:xfrm>
@@ -509,11 +543,75 @@
             </a:r>
           </a:p>
           <a:p>
-            <a:endParaRPr lang="en-MY" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:endParaRPr>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-MY" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>4. </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="0" lang="en-MY" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:prstClr val="white"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:uLnTx/>
+                <a:uFillTx/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Seperate each document by different </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="0" lang="en-MY" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:prstClr val="white"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:uLnTx/>
+                <a:uFillTx/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>BOX OPERATOR</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-MY" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
           <a:p>
             <a:r>
@@ -539,9 +637,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -579,7 +677,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -685,7 +783,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -827,7 +925,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -835,2588 +933,2625 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265EB0DC-959C-45E6-86B4-35F80D54DB28}">
-  <dimension ref="B2:G556"/>
+  <dimension ref="B2:H556"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7265625" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" customWidth="1"/>
-    <col min="3" max="3" width="53.26953125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="53.28515625" customWidth="1"/>
     <col min="4" max="4" width="14" style="6" customWidth="1"/>
-    <col min="5" max="5" width="26.1796875" customWidth="1"/>
-    <col min="6" max="6" width="57.81640625" customWidth="1"/>
-    <col min="7" max="7" width="21.7265625" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="15"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="13" t="s">
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="17" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C7" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C8" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C9" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C15" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C16" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>1</v>
       </c>
       <c r="F19" s="9">
         <v>837800</v>
       </c>
       <c r="G19" s="11">
+        <v>3000</v>
+      </c>
+      <c r="H19" s="11">
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C20" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="18"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="15"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B21" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="9" t="s">
+      <c r="D22" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="15"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B22" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="15"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B23" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="D23" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="15"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="15"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="15"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="15"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="15"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="E23" s="18"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="18"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="18"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="18"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="10"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="10"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
       <c r="D41" s="10"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
       <c r="D42" s="10"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="10"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="10"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
       <c r="D46" s="10"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
       <c r="D47" s="10"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="10"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
       <c r="D49" s="10"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
       <c r="D51" s="10"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
       <c r="D52" s="10"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
       <c r="D53" s="10"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
       <c r="D54" s="10"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="10"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="10"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="10"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="10"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
       <c r="D61" s="10"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
       <c r="D63" s="10"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
       <c r="D64" s="10"/>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
       <c r="D65" s="10"/>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
       <c r="D66" s="10"/>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
       <c r="D67" s="10"/>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
       <c r="D68" s="10"/>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
       <c r="D69" s="10"/>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
       <c r="D70" s="10"/>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
       <c r="D71" s="10"/>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
       <c r="D72" s="10"/>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
       <c r="D73" s="10"/>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
       <c r="D74" s="10"/>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
       <c r="D75" s="10"/>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
       <c r="D76" s="10"/>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
       <c r="D77" s="10"/>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
       <c r="D78" s="10"/>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
       <c r="D79" s="10"/>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
       <c r="D80" s="10"/>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
       <c r="D81" s="10"/>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
       <c r="D82" s="10"/>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
       <c r="D83" s="10"/>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
       <c r="D84" s="10"/>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
       <c r="D85" s="10"/>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
       <c r="D86" s="10"/>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
       <c r="D87" s="10"/>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
       <c r="D88" s="10"/>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
       <c r="D89" s="10"/>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
       <c r="D90" s="10"/>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
       <c r="D91" s="10"/>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
       <c r="D92" s="10"/>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
       <c r="D93" s="10"/>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
       <c r="D94" s="10"/>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
       <c r="D95" s="10"/>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
       <c r="D96" s="10"/>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
       <c r="D97" s="10"/>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
       <c r="D98" s="10"/>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
       <c r="D99" s="10"/>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
       <c r="D101" s="10"/>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
       <c r="D102" s="10"/>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
       <c r="D103" s="10"/>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
       <c r="D104" s="10"/>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
       <c r="D105" s="10"/>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="9"/>
       <c r="C106" s="9"/>
       <c r="D106" s="10"/>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
       <c r="D107" s="10"/>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" s="9"/>
       <c r="C108" s="9"/>
       <c r="D108" s="10"/>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" s="9"/>
       <c r="C109" s="9"/>
       <c r="D109" s="10"/>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" s="9"/>
       <c r="C110" s="9"/>
       <c r="D110" s="10"/>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
       <c r="D111" s="10"/>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" s="9"/>
       <c r="C112" s="9"/>
       <c r="D112" s="10"/>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
       <c r="D113" s="10"/>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="9"/>
       <c r="C114" s="9"/>
       <c r="D114" s="10"/>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="9"/>
       <c r="C115" s="9"/>
       <c r="D115" s="10"/>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="9"/>
       <c r="C116" s="9"/>
       <c r="D116" s="10"/>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="9"/>
       <c r="C117" s="9"/>
       <c r="D117" s="10"/>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="9"/>
       <c r="C118" s="9"/>
       <c r="D118" s="10"/>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" s="9"/>
       <c r="C119" s="9"/>
       <c r="D119" s="10"/>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" s="9"/>
       <c r="C120" s="9"/>
       <c r="D120" s="10"/>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" s="9"/>
       <c r="C121" s="9"/>
       <c r="D121" s="10"/>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" s="9"/>
       <c r="C122" s="9"/>
       <c r="D122" s="10"/>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" s="9"/>
       <c r="C123" s="9"/>
       <c r="D123" s="10"/>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="9"/>
       <c r="C124" s="9"/>
       <c r="D124" s="10"/>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="9"/>
       <c r="C125" s="9"/>
       <c r="D125" s="10"/>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="9"/>
       <c r="C126" s="9"/>
       <c r="D126" s="10"/>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" s="9"/>
       <c r="C127" s="9"/>
       <c r="D127" s="10"/>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" s="9"/>
       <c r="C128" s="9"/>
       <c r="D128" s="10"/>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" s="9"/>
       <c r="C129" s="9"/>
       <c r="D129" s="10"/>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="9"/>
       <c r="C130" s="9"/>
       <c r="D130" s="10"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" s="9"/>
       <c r="C131" s="9"/>
       <c r="D131" s="10"/>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="9"/>
       <c r="C132" s="9"/>
       <c r="D132" s="10"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" s="9"/>
       <c r="C133" s="9"/>
       <c r="D133" s="10"/>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" s="9"/>
       <c r="C134" s="9"/>
       <c r="D134" s="10"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" s="9"/>
       <c r="C135" s="9"/>
       <c r="D135" s="10"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" s="9"/>
       <c r="C136" s="9"/>
       <c r="D136" s="10"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" s="9"/>
       <c r="C137" s="9"/>
       <c r="D137" s="10"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="9"/>
       <c r="C138" s="9"/>
       <c r="D138" s="10"/>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="9"/>
       <c r="C139" s="9"/>
       <c r="D139" s="10"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140" s="9"/>
       <c r="C140" s="9"/>
       <c r="D140" s="10"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B141" s="9"/>
       <c r="C141" s="9"/>
       <c r="D141" s="10"/>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B142" s="9"/>
       <c r="C142" s="9"/>
       <c r="D142" s="10"/>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B143" s="9"/>
       <c r="C143" s="9"/>
       <c r="D143" s="10"/>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" s="9"/>
       <c r="C144" s="9"/>
       <c r="D144" s="10"/>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B145" s="9"/>
       <c r="C145" s="9"/>
       <c r="D145" s="10"/>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B146" s="9"/>
       <c r="C146" s="9"/>
       <c r="D146" s="10"/>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B147" s="9"/>
       <c r="C147" s="9"/>
       <c r="D147" s="10"/>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B148" s="9"/>
       <c r="C148" s="9"/>
       <c r="D148" s="10"/>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B149" s="9"/>
       <c r="C149" s="9"/>
       <c r="D149" s="10"/>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B150" s="9"/>
       <c r="C150" s="9"/>
       <c r="D150" s="10"/>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B151" s="9"/>
       <c r="C151" s="9"/>
       <c r="D151" s="10"/>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B152" s="9"/>
       <c r="C152" s="9"/>
       <c r="D152" s="10"/>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" s="9"/>
       <c r="C153" s="9"/>
       <c r="D153" s="10"/>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B154" s="9"/>
       <c r="C154" s="9"/>
       <c r="D154" s="10"/>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B155" s="9"/>
       <c r="C155" s="9"/>
       <c r="D155" s="10"/>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B156" s="9"/>
       <c r="C156" s="9"/>
       <c r="D156" s="10"/>
     </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B157" s="9"/>
       <c r="C157" s="9"/>
       <c r="D157" s="10"/>
     </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B158" s="9"/>
       <c r="C158" s="9"/>
       <c r="D158" s="10"/>
     </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B159" s="9"/>
       <c r="C159" s="9"/>
       <c r="D159" s="10"/>
     </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B160" s="9"/>
       <c r="C160" s="9"/>
       <c r="D160" s="10"/>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="9"/>
       <c r="C161" s="9"/>
       <c r="D161" s="10"/>
     </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" s="9"/>
       <c r="C162" s="9"/>
       <c r="D162" s="10"/>
     </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="9"/>
       <c r="C163" s="9"/>
       <c r="D163" s="10"/>
     </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="9"/>
       <c r="C164" s="9"/>
       <c r="D164" s="10"/>
     </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="9"/>
       <c r="C165" s="9"/>
       <c r="D165" s="10"/>
     </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="9"/>
       <c r="C166" s="9"/>
       <c r="D166" s="10"/>
     </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" s="9"/>
       <c r="C167" s="9"/>
       <c r="D167" s="10"/>
     </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="9"/>
       <c r="C168" s="9"/>
       <c r="D168" s="10"/>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="9"/>
       <c r="C169" s="9"/>
       <c r="D169" s="10"/>
     </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="9"/>
       <c r="C170" s="9"/>
       <c r="D170" s="10"/>
     </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="9"/>
       <c r="C171" s="9"/>
       <c r="D171" s="10"/>
     </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" s="9"/>
       <c r="C172" s="9"/>
       <c r="D172" s="10"/>
     </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" s="9"/>
       <c r="C173" s="9"/>
       <c r="D173" s="10"/>
     </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="9"/>
       <c r="C174" s="9"/>
       <c r="D174" s="10"/>
     </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" s="9"/>
       <c r="C175" s="9"/>
       <c r="D175" s="10"/>
     </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" s="9"/>
       <c r="C176" s="9"/>
       <c r="D176" s="10"/>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B177" s="9"/>
       <c r="C177" s="9"/>
       <c r="D177" s="10"/>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B178" s="9"/>
       <c r="C178" s="9"/>
       <c r="D178" s="10"/>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B179" s="9"/>
       <c r="C179" s="9"/>
       <c r="D179" s="10"/>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B180" s="9"/>
       <c r="C180" s="9"/>
       <c r="D180" s="10"/>
     </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B181" s="9"/>
       <c r="C181" s="9"/>
       <c r="D181" s="10"/>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B182" s="9"/>
       <c r="C182" s="9"/>
       <c r="D182" s="10"/>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B183" s="9"/>
       <c r="C183" s="9"/>
       <c r="D183" s="10"/>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B184" s="9"/>
       <c r="C184" s="9"/>
       <c r="D184" s="10"/>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" s="9"/>
       <c r="C185" s="9"/>
       <c r="D185" s="10"/>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B186" s="9"/>
       <c r="C186" s="9"/>
       <c r="D186" s="10"/>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B187" s="9"/>
       <c r="C187" s="9"/>
       <c r="D187" s="10"/>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B188" s="9"/>
       <c r="C188" s="9"/>
       <c r="D188" s="10"/>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B189" s="9"/>
       <c r="C189" s="9"/>
       <c r="D189" s="10"/>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B190" s="9"/>
       <c r="C190" s="9"/>
       <c r="D190" s="10"/>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B191" s="9"/>
       <c r="C191" s="9"/>
       <c r="D191" s="10"/>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B192" s="9"/>
       <c r="C192" s="9"/>
       <c r="D192" s="10"/>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" s="9"/>
       <c r="C193" s="9"/>
       <c r="D193" s="10"/>
     </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" s="9"/>
       <c r="C194" s="9"/>
       <c r="D194" s="10"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" s="9"/>
       <c r="C195" s="9"/>
       <c r="D195" s="10"/>
     </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B196" s="9"/>
       <c r="C196" s="9"/>
       <c r="D196" s="10"/>
     </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B197" s="9"/>
       <c r="C197" s="9"/>
       <c r="D197" s="10"/>
     </row>
-    <row r="198" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B198" s="9"/>
       <c r="C198" s="9"/>
       <c r="D198" s="10"/>
     </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" s="9"/>
       <c r="C199" s="9"/>
       <c r="D199" s="10"/>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B200" s="9"/>
       <c r="C200" s="9"/>
       <c r="D200" s="10"/>
     </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B201" s="9"/>
       <c r="C201" s="9"/>
       <c r="D201" s="10"/>
     </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B202" s="9"/>
       <c r="C202" s="9"/>
       <c r="D202" s="10"/>
     </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
       <c r="D203" s="8"/>
     </row>
-    <row r="204" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
       <c r="D204" s="8"/>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
       <c r="D205" s="8"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
       <c r="D206" s="8"/>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
       <c r="D207" s="8"/>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
       <c r="D208" s="8"/>
     </row>
-    <row r="209" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
       <c r="D209" s="8"/>
     </row>
-    <row r="210" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
       <c r="D210" s="8"/>
     </row>
-    <row r="211" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
       <c r="D211" s="8"/>
     </row>
-    <row r="212" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
       <c r="D212" s="8"/>
     </row>
-    <row r="213" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
       <c r="D213" s="8"/>
     </row>
-    <row r="214" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
       <c r="D214" s="8"/>
     </row>
-    <row r="215" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
       <c r="D215" s="8"/>
     </row>
-    <row r="216" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
       <c r="D216" s="8"/>
     </row>
-    <row r="217" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
       <c r="D217" s="8"/>
     </row>
-    <row r="218" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
       <c r="D218" s="8"/>
     </row>
-    <row r="219" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
       <c r="D219" s="8"/>
     </row>
-    <row r="220" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
       <c r="D220" s="8"/>
     </row>
-    <row r="221" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
       <c r="D221" s="8"/>
     </row>
-    <row r="222" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
       <c r="D222" s="8"/>
     </row>
-    <row r="223" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B223" s="2"/>
       <c r="C223" s="2"/>
       <c r="D223" s="8"/>
     </row>
-    <row r="224" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
       <c r="D224" s="8"/>
     </row>
-    <row r="225" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B225" s="2"/>
       <c r="C225" s="2"/>
       <c r="D225" s="8"/>
     </row>
-    <row r="226" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
       <c r="D226" s="8"/>
     </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
       <c r="D227" s="8"/>
     </row>
-    <row r="228" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="228" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
       <c r="D228" s="8"/>
     </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B229" s="2"/>
       <c r="C229" s="2"/>
       <c r="D229" s="8"/>
     </row>
-    <row r="230" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="230" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
       <c r="D230" s="8"/>
     </row>
-    <row r="231" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
       <c r="D231" s="8"/>
     </row>
-    <row r="232" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="232" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B232" s="2"/>
       <c r="C232" s="2"/>
       <c r="D232" s="8"/>
     </row>
-    <row r="233" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="233" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B233" s="2"/>
       <c r="C233" s="2"/>
       <c r="D233" s="8"/>
     </row>
-    <row r="234" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B234" s="2"/>
       <c r="C234" s="2"/>
       <c r="D234" s="8"/>
     </row>
-    <row r="235" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B235" s="2"/>
       <c r="C235" s="2"/>
       <c r="D235" s="8"/>
     </row>
-    <row r="236" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B236" s="2"/>
       <c r="C236" s="2"/>
       <c r="D236" s="8"/>
     </row>
-    <row r="237" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B237" s="2"/>
       <c r="C237" s="2"/>
       <c r="D237" s="8"/>
     </row>
-    <row r="238" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B238" s="2"/>
       <c r="C238" s="2"/>
       <c r="D238" s="8"/>
     </row>
-    <row r="239" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="239" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B239" s="2"/>
       <c r="C239" s="2"/>
       <c r="D239" s="8"/>
     </row>
-    <row r="240" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B240" s="2"/>
       <c r="C240" s="2"/>
       <c r="D240" s="8"/>
     </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="2"/>
       <c r="C241" s="2"/>
       <c r="D241" s="8"/>
     </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="2"/>
       <c r="C242" s="2"/>
       <c r="D242" s="8"/>
     </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="2"/>
       <c r="C243" s="2"/>
       <c r="D243" s="8"/>
     </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
       <c r="D244" s="8"/>
     </row>
-    <row r="245" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="2"/>
       <c r="C245" s="2"/>
       <c r="D245" s="8"/>
     </row>
-    <row r="246" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
       <c r="D246" s="8"/>
     </row>
-    <row r="247" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
       <c r="D247" s="8"/>
     </row>
-    <row r="248" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
       <c r="D248" s="8"/>
     </row>
-    <row r="249" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B249" s="2"/>
       <c r="C249" s="2"/>
       <c r="D249" s="8"/>
     </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
       <c r="D250" s="8"/>
     </row>
-    <row r="251" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
       <c r="D251" s="8"/>
     </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
       <c r="D252" s="8"/>
     </row>
-    <row r="253" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="253" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
       <c r="D253" s="8"/>
     </row>
-    <row r="254" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="254" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
       <c r="D254" s="8"/>
     </row>
-    <row r="255" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="255" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
       <c r="D255" s="8"/>
     </row>
-    <row r="256" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="256" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
       <c r="D256" s="8"/>
     </row>
-    <row r="257" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="257" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
       <c r="D257" s="8"/>
     </row>
-    <row r="258" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="258" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
       <c r="D258" s="8"/>
     </row>
-    <row r="259" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="259" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B259" s="2"/>
       <c r="C259" s="2"/>
       <c r="D259" s="8"/>
     </row>
-    <row r="260" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="260" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
       <c r="D260" s="8"/>
     </row>
-    <row r="261" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="261" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>
       <c r="D261" s="8"/>
     </row>
-    <row r="262" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="262" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B262" s="2"/>
       <c r="C262" s="2"/>
       <c r="D262" s="8"/>
     </row>
-    <row r="263" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="263" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B263" s="2"/>
       <c r="C263" s="2"/>
       <c r="D263" s="8"/>
     </row>
-    <row r="264" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="264" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
       <c r="D264" s="8"/>
     </row>
-    <row r="265" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="265" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B265" s="2"/>
       <c r="C265" s="2"/>
       <c r="D265" s="8"/>
     </row>
-    <row r="266" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="266" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B266" s="2"/>
       <c r="C266" s="2"/>
       <c r="D266" s="8"/>
     </row>
-    <row r="267" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="267" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B267" s="2"/>
       <c r="C267" s="2"/>
       <c r="D267" s="8"/>
     </row>
-    <row r="268" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="268" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B268" s="2"/>
       <c r="C268" s="2"/>
       <c r="D268" s="8"/>
     </row>
-    <row r="269" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="269" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B269" s="2"/>
       <c r="C269" s="2"/>
       <c r="D269" s="8"/>
     </row>
-    <row r="270" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="270" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B270" s="2"/>
       <c r="C270" s="2"/>
       <c r="D270" s="8"/>
     </row>
-    <row r="271" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="271" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B271" s="2"/>
       <c r="C271" s="2"/>
       <c r="D271" s="8"/>
     </row>
-    <row r="272" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="272" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B272" s="2"/>
       <c r="C272" s="2"/>
       <c r="D272" s="8"/>
     </row>
-    <row r="273" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="273" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B273" s="2"/>
       <c r="C273" s="2"/>
       <c r="D273" s="8"/>
     </row>
-    <row r="274" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="274" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B274" s="2"/>
       <c r="C274" s="2"/>
       <c r="D274" s="8"/>
     </row>
-    <row r="275" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="275" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B275" s="2"/>
       <c r="C275" s="2"/>
       <c r="D275" s="8"/>
     </row>
-    <row r="276" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="276" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B276" s="2"/>
       <c r="C276" s="2"/>
       <c r="D276" s="8"/>
     </row>
-    <row r="277" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="277" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B277" s="2"/>
       <c r="C277" s="2"/>
       <c r="D277" s="8"/>
     </row>
-    <row r="278" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="278" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B278" s="2"/>
       <c r="C278" s="2"/>
       <c r="D278" s="8"/>
     </row>
-    <row r="279" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="279" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B279" s="2"/>
       <c r="C279" s="2"/>
       <c r="D279" s="8"/>
     </row>
-    <row r="280" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="280" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B280" s="2"/>
       <c r="C280" s="2"/>
       <c r="D280" s="8"/>
     </row>
-    <row r="281" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="281" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B281" s="2"/>
       <c r="C281" s="2"/>
       <c r="D281" s="8"/>
     </row>
-    <row r="282" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="282" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B282" s="2"/>
       <c r="C282" s="2"/>
       <c r="D282" s="8"/>
     </row>
-    <row r="283" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="283" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B283" s="2"/>
       <c r="C283" s="2"/>
       <c r="D283" s="8"/>
     </row>
-    <row r="284" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="284" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B284" s="2"/>
       <c r="C284" s="2"/>
       <c r="D284" s="8"/>
     </row>
-    <row r="285" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="285" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B285" s="2"/>
       <c r="C285" s="2"/>
       <c r="D285" s="8"/>
     </row>
-    <row r="286" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="286" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B286" s="2"/>
       <c r="C286" s="2"/>
       <c r="D286" s="8"/>
     </row>
-    <row r="287" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="287" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B287" s="2"/>
       <c r="C287" s="2"/>
       <c r="D287" s="8"/>
     </row>
-    <row r="288" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="288" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B288" s="2"/>
       <c r="C288" s="2"/>
       <c r="D288" s="8"/>
     </row>
-    <row r="289" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="289" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B289" s="2"/>
       <c r="C289" s="2"/>
       <c r="D289" s="8"/>
     </row>
-    <row r="290" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="290" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B290" s="2"/>
       <c r="C290" s="2"/>
       <c r="D290" s="8"/>
     </row>
-    <row r="291" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="291" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B291" s="2"/>
       <c r="C291" s="2"/>
       <c r="D291" s="8"/>
     </row>
-    <row r="292" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="292" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B292" s="2"/>
       <c r="C292" s="2"/>
       <c r="D292" s="8"/>
     </row>
-    <row r="293" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="293" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B293" s="2"/>
       <c r="C293" s="2"/>
       <c r="D293" s="8"/>
     </row>
-    <row r="294" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="294" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B294" s="2"/>
       <c r="C294" s="2"/>
       <c r="D294" s="8"/>
     </row>
-    <row r="295" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="295" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B295" s="2"/>
       <c r="C295" s="2"/>
       <c r="D295" s="8"/>
     </row>
-    <row r="296" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="296" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B296" s="2"/>
       <c r="C296" s="2"/>
       <c r="D296" s="8"/>
     </row>
-    <row r="297" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="297" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B297" s="2"/>
       <c r="C297" s="2"/>
       <c r="D297" s="8"/>
     </row>
-    <row r="298" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="298" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B298" s="2"/>
       <c r="C298" s="2"/>
       <c r="D298" s="8"/>
     </row>
-    <row r="299" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="299" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B299" s="2"/>
       <c r="C299" s="2"/>
       <c r="D299" s="8"/>
     </row>
-    <row r="300" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="300" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B300" s="2"/>
       <c r="C300" s="2"/>
       <c r="D300" s="8"/>
     </row>
-    <row r="301" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="301" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B301" s="2"/>
       <c r="C301" s="2"/>
       <c r="D301" s="8"/>
     </row>
-    <row r="302" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="302" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B302" s="2"/>
       <c r="C302" s="2"/>
       <c r="D302" s="8"/>
     </row>
-    <row r="303" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="303" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B303" s="2"/>
       <c r="C303" s="2"/>
       <c r="D303" s="8"/>
     </row>
-    <row r="304" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="304" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B304" s="2"/>
       <c r="C304" s="2"/>
       <c r="D304" s="8"/>
     </row>
-    <row r="305" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="305" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B305" s="2"/>
       <c r="C305" s="2"/>
       <c r="D305" s="8"/>
     </row>
-    <row r="306" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="306" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B306" s="2"/>
       <c r="C306" s="2"/>
       <c r="D306" s="8"/>
     </row>
-    <row r="307" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="307" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B307" s="2"/>
       <c r="C307" s="2"/>
       <c r="D307" s="8"/>
     </row>
-    <row r="308" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="308" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B308" s="2"/>
       <c r="C308" s="2"/>
       <c r="D308" s="8"/>
     </row>
-    <row r="309" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="309" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B309" s="2"/>
       <c r="C309" s="2"/>
       <c r="D309" s="8"/>
     </row>
-    <row r="310" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="310" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B310" s="2"/>
       <c r="C310" s="2"/>
       <c r="D310" s="8"/>
     </row>
-    <row r="311" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="311" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B311" s="2"/>
       <c r="C311" s="2"/>
       <c r="D311" s="8"/>
     </row>
-    <row r="312" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="312" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B312" s="2"/>
       <c r="C312" s="2"/>
       <c r="D312" s="8"/>
     </row>
-    <row r="313" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="313" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B313" s="2"/>
       <c r="C313" s="2"/>
       <c r="D313" s="8"/>
     </row>
-    <row r="314" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="314" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B314" s="2"/>
       <c r="C314" s="2"/>
       <c r="D314" s="8"/>
     </row>
-    <row r="315" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="315" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B315" s="2"/>
       <c r="C315" s="2"/>
       <c r="D315" s="8"/>
     </row>
-    <row r="316" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="316" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B316" s="2"/>
       <c r="C316" s="2"/>
       <c r="D316" s="8"/>
     </row>
-    <row r="317" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="317" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B317" s="2"/>
       <c r="C317" s="2"/>
       <c r="D317" s="8"/>
     </row>
-    <row r="318" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="318" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B318" s="2"/>
       <c r="C318" s="2"/>
       <c r="D318" s="8"/>
     </row>
-    <row r="319" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="319" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B319" s="2"/>
       <c r="C319" s="2"/>
       <c r="D319" s="8"/>
     </row>
-    <row r="320" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="320" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B320" s="2"/>
       <c r="C320" s="2"/>
       <c r="D320" s="8"/>
     </row>
-    <row r="321" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="321" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B321" s="2"/>
       <c r="C321" s="2"/>
       <c r="D321" s="8"/>
     </row>
-    <row r="322" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="322" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B322" s="2"/>
       <c r="C322" s="2"/>
       <c r="D322" s="8"/>
     </row>
-    <row r="323" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="323" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B323" s="2"/>
       <c r="C323" s="2"/>
       <c r="D323" s="8"/>
     </row>
-    <row r="324" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="324" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B324" s="2"/>
       <c r="C324" s="2"/>
       <c r="D324" s="8"/>
     </row>
-    <row r="325" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="325" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B325" s="2"/>
       <c r="C325" s="2"/>
       <c r="D325" s="8"/>
     </row>
-    <row r="326" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="326" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B326" s="2"/>
       <c r="C326" s="2"/>
       <c r="D326" s="8"/>
     </row>
-    <row r="327" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="327" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B327" s="2"/>
       <c r="C327" s="2"/>
       <c r="D327" s="8"/>
     </row>
-    <row r="328" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="328" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B328" s="2"/>
       <c r="C328" s="2"/>
       <c r="D328" s="8"/>
     </row>
-    <row r="329" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="329" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B329" s="2"/>
       <c r="C329" s="2"/>
       <c r="D329" s="8"/>
     </row>
-    <row r="330" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="330" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B330" s="2"/>
       <c r="C330" s="2"/>
       <c r="D330" s="8"/>
     </row>
-    <row r="331" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="331" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B331" s="2"/>
       <c r="C331" s="2"/>
       <c r="D331" s="8"/>
     </row>
-    <row r="332" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="332" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B332" s="2"/>
       <c r="C332" s="2"/>
       <c r="D332" s="8"/>
     </row>
-    <row r="333" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="333" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B333" s="2"/>
       <c r="C333" s="2"/>
       <c r="D333" s="8"/>
     </row>
-    <row r="334" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="334" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B334" s="2"/>
       <c r="C334" s="2"/>
       <c r="D334" s="8"/>
     </row>
-    <row r="335" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="335" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B335" s="2"/>
       <c r="C335" s="2"/>
       <c r="D335" s="8"/>
     </row>
-    <row r="336" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="336" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B336" s="2"/>
       <c r="C336" s="2"/>
       <c r="D336" s="8"/>
     </row>
-    <row r="337" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="337" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B337" s="2"/>
       <c r="C337" s="2"/>
       <c r="D337" s="8"/>
     </row>
-    <row r="338" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="338" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B338" s="2"/>
       <c r="C338" s="2"/>
       <c r="D338" s="8"/>
     </row>
-    <row r="339" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="339" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B339" s="2"/>
       <c r="C339" s="2"/>
       <c r="D339" s="8"/>
     </row>
-    <row r="340" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="340" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B340" s="2"/>
       <c r="C340" s="2"/>
       <c r="D340" s="8"/>
     </row>
-    <row r="341" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="341" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B341" s="2"/>
       <c r="C341" s="2"/>
       <c r="D341" s="8"/>
     </row>
-    <row r="342" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="342" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B342" s="2"/>
       <c r="C342" s="2"/>
       <c r="D342" s="8"/>
     </row>
-    <row r="343" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="343" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B343" s="2"/>
       <c r="C343" s="2"/>
       <c r="D343" s="8"/>
     </row>
-    <row r="344" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="344" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B344" s="2"/>
       <c r="C344" s="2"/>
       <c r="D344" s="8"/>
     </row>
-    <row r="345" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="345" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B345" s="2"/>
       <c r="C345" s="2"/>
       <c r="D345" s="8"/>
     </row>
-    <row r="346" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="346" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B346" s="2"/>
       <c r="C346" s="2"/>
       <c r="D346" s="8"/>
     </row>
-    <row r="347" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="347" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B347" s="2"/>
       <c r="C347" s="2"/>
       <c r="D347" s="8"/>
     </row>
-    <row r="348" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="348" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B348" s="2"/>
       <c r="C348" s="2"/>
       <c r="D348" s="8"/>
     </row>
-    <row r="349" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="349" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B349" s="2"/>
       <c r="C349" s="2"/>
       <c r="D349" s="8"/>
     </row>
-    <row r="350" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="350" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B350" s="2"/>
       <c r="C350" s="2"/>
       <c r="D350" s="8"/>
     </row>
-    <row r="351" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="351" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B351" s="2"/>
       <c r="C351" s="2"/>
       <c r="D351" s="8"/>
     </row>
-    <row r="352" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="352" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B352" s="2"/>
       <c r="C352" s="2"/>
       <c r="D352" s="8"/>
     </row>
-    <row r="353" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="353" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B353" s="2"/>
       <c r="C353" s="2"/>
       <c r="D353" s="8"/>
     </row>
-    <row r="354" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="354" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B354" s="2"/>
       <c r="C354" s="2"/>
       <c r="D354" s="8"/>
     </row>
-    <row r="355" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="355" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B355" s="2"/>
       <c r="C355" s="2"/>
       <c r="D355" s="8"/>
     </row>
-    <row r="356" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="356" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B356" s="2"/>
       <c r="C356" s="2"/>
       <c r="D356" s="8"/>
     </row>
-    <row r="357" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="357" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B357" s="2"/>
       <c r="C357" s="2"/>
       <c r="D357" s="8"/>
     </row>
-    <row r="358" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="358" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B358" s="2"/>
       <c r="C358" s="2"/>
       <c r="D358" s="8"/>
     </row>
-    <row r="359" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="359" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B359" s="2"/>
       <c r="C359" s="2"/>
       <c r="D359" s="8"/>
     </row>
-    <row r="360" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="360" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B360" s="2"/>
       <c r="C360" s="2"/>
       <c r="D360" s="8"/>
     </row>
-    <row r="361" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="361" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B361" s="2"/>
       <c r="C361" s="2"/>
       <c r="D361" s="8"/>
     </row>
-    <row r="362" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="362" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B362" s="2"/>
       <c r="C362" s="2"/>
       <c r="D362" s="8"/>
     </row>
-    <row r="363" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="363" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B363" s="2"/>
       <c r="C363" s="2"/>
       <c r="D363" s="8"/>
     </row>
-    <row r="364" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="364" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B364" s="2"/>
       <c r="C364" s="2"/>
       <c r="D364" s="8"/>
     </row>
-    <row r="365" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="365" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B365" s="2"/>
       <c r="C365" s="2"/>
       <c r="D365" s="8"/>
     </row>
-    <row r="366" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="366" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B366" s="2"/>
       <c r="C366" s="2"/>
       <c r="D366" s="8"/>
     </row>
-    <row r="367" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="367" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B367" s="2"/>
       <c r="C367" s="2"/>
       <c r="D367" s="8"/>
     </row>
-    <row r="368" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="368" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B368" s="2"/>
       <c r="C368" s="2"/>
       <c r="D368" s="8"/>
     </row>
-    <row r="369" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="369" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B369" s="2"/>
       <c r="C369" s="2"/>
       <c r="D369" s="8"/>
     </row>
-    <row r="370" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="370" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B370" s="2"/>
       <c r="C370" s="2"/>
       <c r="D370" s="8"/>
     </row>
-    <row r="371" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="371" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B371" s="2"/>
       <c r="C371" s="2"/>
       <c r="D371" s="8"/>
     </row>
-    <row r="372" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="372" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B372" s="2"/>
       <c r="C372" s="2"/>
       <c r="D372" s="8"/>
     </row>
-    <row r="373" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="373" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B373" s="2"/>
       <c r="C373" s="2"/>
       <c r="D373" s="8"/>
     </row>
-    <row r="374" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="374" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B374" s="2"/>
       <c r="C374" s="2"/>
       <c r="D374" s="8"/>
     </row>
-    <row r="375" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="375" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B375" s="2"/>
       <c r="C375" s="2"/>
       <c r="D375" s="8"/>
     </row>
-    <row r="376" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="376" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B376" s="2"/>
       <c r="C376" s="2"/>
       <c r="D376" s="8"/>
     </row>
-    <row r="377" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="377" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B377" s="2"/>
       <c r="C377" s="2"/>
       <c r="D377" s="8"/>
     </row>
-    <row r="378" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="378" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B378" s="2"/>
       <c r="C378" s="2"/>
       <c r="D378" s="8"/>
     </row>
-    <row r="379" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="379" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B379" s="2"/>
       <c r="C379" s="2"/>
       <c r="D379" s="8"/>
     </row>
-    <row r="380" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="380" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B380" s="2"/>
       <c r="C380" s="2"/>
       <c r="D380" s="8"/>
     </row>
-    <row r="381" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="381" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B381" s="2"/>
       <c r="C381" s="2"/>
       <c r="D381" s="8"/>
     </row>
-    <row r="382" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="382" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B382" s="2"/>
       <c r="C382" s="2"/>
       <c r="D382" s="8"/>
     </row>
-    <row r="383" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="383" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B383" s="2"/>
       <c r="C383" s="2"/>
       <c r="D383" s="8"/>
     </row>
-    <row r="384" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="384" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B384" s="2"/>
       <c r="C384" s="2"/>
       <c r="D384" s="8"/>
     </row>
-    <row r="385" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="385" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B385" s="2"/>
       <c r="C385" s="2"/>
       <c r="D385" s="8"/>
     </row>
-    <row r="386" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="386" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B386" s="2"/>
       <c r="C386" s="2"/>
       <c r="D386" s="8"/>
     </row>
-    <row r="387" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="387" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B387" s="2"/>
       <c r="C387" s="2"/>
       <c r="D387" s="8"/>
     </row>
-    <row r="388" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="388" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B388" s="2"/>
       <c r="C388" s="2"/>
       <c r="D388" s="8"/>
     </row>
-    <row r="389" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="389" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B389" s="2"/>
       <c r="C389" s="2"/>
       <c r="D389" s="8"/>
     </row>
-    <row r="390" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="390" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B390" s="2"/>
       <c r="C390" s="2"/>
       <c r="D390" s="8"/>
     </row>
-    <row r="391" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="391" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B391" s="2"/>
       <c r="C391" s="2"/>
       <c r="D391" s="8"/>
     </row>
-    <row r="392" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="392" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B392" s="2"/>
       <c r="C392" s="2"/>
       <c r="D392" s="8"/>
     </row>
-    <row r="393" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="393" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B393" s="2"/>
       <c r="C393" s="2"/>
       <c r="D393" s="8"/>
     </row>
-    <row r="394" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="394" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B394" s="2"/>
       <c r="C394" s="2"/>
       <c r="D394" s="8"/>
     </row>
-    <row r="395" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="395" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B395" s="2"/>
       <c r="C395" s="2"/>
       <c r="D395" s="8"/>
     </row>
-    <row r="396" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="396" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B396" s="2"/>
       <c r="C396" s="2"/>
       <c r="D396" s="8"/>
     </row>
-    <row r="397" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="397" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B397" s="2"/>
       <c r="C397" s="2"/>
       <c r="D397" s="8"/>
     </row>
-    <row r="398" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="398" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B398" s="2"/>
       <c r="C398" s="2"/>
       <c r="D398" s="8"/>
     </row>
-    <row r="399" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="399" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B399" s="2"/>
       <c r="C399" s="2"/>
       <c r="D399" s="8"/>
     </row>
-    <row r="400" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="400" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B400" s="2"/>
       <c r="C400" s="2"/>
       <c r="D400" s="8"/>
     </row>
-    <row r="401" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="401" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B401" s="2"/>
       <c r="C401" s="2"/>
       <c r="D401" s="8"/>
     </row>
-    <row r="402" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="402" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B402" s="2"/>
       <c r="C402" s="2"/>
       <c r="D402" s="8"/>
     </row>
-    <row r="403" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="403" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B403" s="2"/>
       <c r="C403" s="2"/>
       <c r="D403" s="8"/>
     </row>
-    <row r="404" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="404" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D404" s="8"/>
     </row>
-    <row r="405" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="405" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D405" s="8"/>
     </row>
-    <row r="406" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="406" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D406" s="8"/>
     </row>
-    <row r="407" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="407" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D407" s="8"/>
     </row>
-    <row r="408" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="408" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D408" s="8"/>
     </row>
-    <row r="409" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="409" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D409" s="8"/>
     </row>
-    <row r="410" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="410" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D410" s="8"/>
     </row>
-    <row r="411" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="411" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D411" s="8"/>
     </row>
-    <row r="412" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="412" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D412" s="8"/>
     </row>
-    <row r="413" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="413" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D413" s="8"/>
     </row>
-    <row r="414" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="414" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D414" s="8"/>
     </row>
-    <row r="415" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="415" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D415" s="8"/>
     </row>
-    <row r="416" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="416" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D416" s="8"/>
     </row>
-    <row r="417" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="417" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D417" s="8"/>
     </row>
-    <row r="418" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="418" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D418" s="8"/>
     </row>
-    <row r="419" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="419" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D419" s="8"/>
     </row>
-    <row r="420" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="420" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D420" s="8"/>
     </row>
-    <row r="421" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="421" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D421" s="8"/>
     </row>
-    <row r="422" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="422" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D422" s="8"/>
     </row>
-    <row r="423" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="423" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D423" s="8"/>
     </row>
-    <row r="424" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="424" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D424" s="8"/>
     </row>
-    <row r="425" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="425" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D425" s="8"/>
     </row>
-    <row r="426" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="426" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D426" s="8"/>
     </row>
-    <row r="427" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="427" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D427" s="8"/>
     </row>
-    <row r="428" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="428" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D428" s="8"/>
     </row>
-    <row r="429" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="429" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D429" s="8"/>
     </row>
-    <row r="430" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="430" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D430" s="8"/>
     </row>
-    <row r="431" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="431" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D431" s="8"/>
     </row>
-    <row r="432" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="432" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D432" s="8"/>
     </row>
-    <row r="433" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="433" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D433" s="8"/>
     </row>
-    <row r="434" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="434" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D434" s="8"/>
     </row>
-    <row r="435" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="435" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D435" s="8"/>
     </row>
-    <row r="436" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="436" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D436" s="8"/>
     </row>
-    <row r="437" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="437" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D437" s="8"/>
     </row>
-    <row r="438" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="438" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D438" s="8"/>
     </row>
-    <row r="439" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="439" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D439" s="8"/>
     </row>
-    <row r="440" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="440" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D440" s="8"/>
     </row>
-    <row r="441" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="441" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D441" s="8"/>
     </row>
-    <row r="442" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="442" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D442" s="8"/>
     </row>
-    <row r="443" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="443" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D443" s="8"/>
     </row>
-    <row r="444" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="444" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D444" s="8"/>
     </row>
-    <row r="445" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="445" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D445" s="8"/>
     </row>
-    <row r="446" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="446" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D446" s="8"/>
     </row>
-    <row r="447" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="447" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D447" s="8"/>
     </row>
-    <row r="448" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="448" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D448" s="8"/>
     </row>
-    <row r="449" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="449" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D449" s="8"/>
     </row>
-    <row r="450" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="450" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D450" s="8"/>
     </row>
-    <row r="451" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="451" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D451" s="8"/>
     </row>
-    <row r="452" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="452" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D452" s="8"/>
     </row>
-    <row r="453" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="453" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D453" s="8"/>
     </row>
-    <row r="454" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="454" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D454" s="8"/>
     </row>
-    <row r="455" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="455" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D455" s="8"/>
     </row>
-    <row r="456" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="456" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D456" s="8"/>
     </row>
-    <row r="457" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="457" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D457" s="8"/>
     </row>
-    <row r="458" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="458" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D458" s="8"/>
     </row>
-    <row r="459" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="459" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D459" s="8"/>
     </row>
-    <row r="460" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="460" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D460" s="8"/>
     </row>
-    <row r="461" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="461" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D461" s="8"/>
     </row>
-    <row r="462" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="462" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D462" s="8"/>
     </row>
-    <row r="463" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="463" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D463" s="8"/>
     </row>
-    <row r="464" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="464" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D464" s="8"/>
     </row>
-    <row r="465" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="465" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D465" s="8"/>
     </row>
-    <row r="466" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="466" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D466" s="8"/>
     </row>
-    <row r="467" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="467" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D467" s="8"/>
     </row>
-    <row r="468" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="468" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D468" s="8"/>
     </row>
-    <row r="469" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="469" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D469" s="8"/>
     </row>
-    <row r="470" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="470" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D470" s="8"/>
     </row>
-    <row r="471" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="471" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D471" s="8"/>
     </row>
-    <row r="472" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="472" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D472" s="8"/>
     </row>
-    <row r="473" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="473" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D473" s="8"/>
     </row>
-    <row r="474" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="474" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D474" s="8"/>
     </row>
-    <row r="475" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="475" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D475" s="8"/>
     </row>
-    <row r="476" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="476" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D476" s="8"/>
     </row>
-    <row r="477" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="477" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D477" s="8"/>
     </row>
-    <row r="478" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="478" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D478" s="8"/>
     </row>
-    <row r="479" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="479" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D479" s="8"/>
     </row>
-    <row r="480" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="480" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D480" s="8"/>
     </row>
-    <row r="481" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="481" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D481" s="8"/>
     </row>
-    <row r="482" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="482" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D482" s="8"/>
     </row>
-    <row r="483" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="483" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D483" s="8"/>
     </row>
-    <row r="484" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="484" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D484" s="8"/>
     </row>
-    <row r="485" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="485" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D485" s="8"/>
     </row>
-    <row r="486" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="486" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D486" s="8"/>
     </row>
-    <row r="487" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="487" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D487" s="8"/>
     </row>
-    <row r="488" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="488" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D488" s="8"/>
     </row>
-    <row r="489" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="489" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D489" s="8"/>
     </row>
-    <row r="490" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="490" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D490" s="8"/>
     </row>
-    <row r="491" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="491" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D491" s="8"/>
     </row>
-    <row r="492" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="492" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D492" s="8"/>
     </row>
-    <row r="493" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="493" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D493" s="8"/>
     </row>
-    <row r="494" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="494" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D494" s="8"/>
     </row>
-    <row r="495" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="495" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D495" s="8"/>
     </row>
-    <row r="496" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="496" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D496" s="8"/>
     </row>
-    <row r="497" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="497" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D497" s="8"/>
     </row>
-    <row r="498" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="498" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D498" s="8"/>
     </row>
-    <row r="499" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="499" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D499" s="8"/>
     </row>
-    <row r="500" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="500" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D500" s="8"/>
     </row>
-    <row r="501" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="501" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D501" s="8"/>
     </row>
-    <row r="502" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="502" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D502" s="8"/>
     </row>
-    <row r="503" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="503" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D503" s="8"/>
     </row>
-    <row r="504" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="504" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D504" s="8"/>
     </row>
-    <row r="505" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="505" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D505" s="8"/>
     </row>
-    <row r="506" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="506" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D506" s="8"/>
     </row>
-    <row r="507" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="507" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D507" s="8"/>
     </row>
-    <row r="508" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="508" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D508" s="8"/>
     </row>
-    <row r="509" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="509" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D509" s="8"/>
     </row>
-    <row r="510" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="510" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D510" s="8"/>
     </row>
-    <row r="511" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="511" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D511" s="8"/>
     </row>
-    <row r="512" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="512" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D512" s="8"/>
     </row>
-    <row r="513" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="513" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D513" s="8"/>
     </row>
-    <row r="514" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="514" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D514" s="8"/>
     </row>
-    <row r="515" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="515" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D515" s="8"/>
     </row>
-    <row r="516" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="516" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D516" s="8"/>
     </row>
-    <row r="517" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="517" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D517" s="8"/>
     </row>
-    <row r="518" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="518" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D518" s="8"/>
     </row>
-    <row r="519" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="519" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D519" s="8"/>
     </row>
-    <row r="520" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="520" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D520" s="8"/>
     </row>
-    <row r="521" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="521" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D521" s="8"/>
     </row>
-    <row r="522" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="522" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D522" s="8"/>
     </row>
-    <row r="523" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="523" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D523" s="8"/>
     </row>
-    <row r="524" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="524" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D524" s="8"/>
     </row>
-    <row r="525" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="525" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D525" s="8"/>
     </row>
-    <row r="526" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="526" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D526" s="8"/>
     </row>
-    <row r="527" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="527" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D527" s="8"/>
     </row>
-    <row r="528" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="528" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D528" s="8"/>
     </row>
-    <row r="529" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="529" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D529" s="8"/>
     </row>
-    <row r="530" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="530" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D530" s="8"/>
     </row>
-    <row r="531" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="531" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D531" s="8"/>
     </row>
-    <row r="532" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="532" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D532" s="8"/>
     </row>
-    <row r="533" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="533" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D533" s="8"/>
     </row>
-    <row r="534" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="534" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D534" s="8"/>
     </row>
-    <row r="535" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="535" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D535" s="8"/>
     </row>
-    <row r="536" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="536" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D536" s="8"/>
     </row>
-    <row r="537" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="537" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D537" s="8"/>
     </row>
-    <row r="538" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="538" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D538" s="8"/>
     </row>
-    <row r="539" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="539" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D539" s="8"/>
     </row>
-    <row r="540" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="540" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D540" s="8"/>
     </row>
-    <row r="541" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="541" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D541" s="8"/>
     </row>
-    <row r="542" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="542" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D542" s="8"/>
     </row>
-    <row r="543" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="543" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D543" s="8"/>
     </row>
-    <row r="544" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="544" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D544" s="8"/>
     </row>
-    <row r="545" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="545" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D545" s="8"/>
     </row>
-    <row r="546" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="546" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D546" s="8"/>
     </row>
-    <row r="547" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="547" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D547" s="8"/>
     </row>
-    <row r="548" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="548" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D548" s="8"/>
     </row>
-    <row r="549" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="549" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D549" s="8"/>
     </row>
-    <row r="550" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="550" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D550" s="8"/>
     </row>
-    <row r="551" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="551" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D551" s="8"/>
     </row>
-    <row r="552" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="552" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D552" s="8"/>
     </row>
-    <row r="553" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="553" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D553" s="8"/>
     </row>
-    <row r="554" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="554" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D554" s="8"/>
     </row>
-    <row r="555" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="555" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D555" s="8"/>
     </row>
-    <row r="556" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="556" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D556" s="8"/>
     </row>
   </sheetData>
@@ -3426,9 +3561,11 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="MEARSK, CMA or EVERGREEN" sqref="C2" xr:uid="{B78CC3E9-3AD1-4ADD-ADE6-D3BE0B9CCE5F}"/>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2" xr:uid="{B78CC3E9-3AD1-4ADD-ADE6-D3BE0B9CCE5F}">
+      <formula1>"OOCL,EVERGREEN,NAVEGACION"</formula1>
+    </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D19:D556" xr:uid="{A1576279-0AF6-4A01-B086-277E31EECE1F}">
-      <formula1>"20GP, 40GP, 40HC, 20RF, 40RF"</formula1>
+      <formula1>"40HC, 20DC"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
log add route events
</commit_message>
<xml_diff>
--- a/public/template/shipping_instruction_template.xlsx
+++ b/public/template/shipping_instruction_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syedazlan/MyLaravelProjects/gus/public/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE307A1-D81F-4073-B831-E78688DECD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E938C419-5379-5742-A5B3-3D72BE722463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{378D42B6-8EFA-4EF6-9C50-436D539EEED8}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{378D42B6-8EFA-4EF6-9C50-436D539EEED8}"/>
   </bookViews>
   <sheets>
     <sheet name="BillOfLading" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -285,7 +285,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -391,8 +391,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6229349" y="209550"/>
-          <a:ext cx="4819651" cy="1581150"/>
+          <a:off x="7102474" y="209550"/>
+          <a:ext cx="5394326" cy="1581150"/>
           <a:chOff x="6029324" y="276225"/>
           <a:chExt cx="4238625" cy="1390650"/>
         </a:xfrm>
@@ -936,22 +936,22 @@
   <dimension ref="B2:H556"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="53.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="53.33203125" customWidth="1"/>
     <col min="4" max="4" width="14" style="6" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="6" max="6" width="33.5" customWidth="1"/>
+    <col min="7" max="7" width="23.5" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
@@ -959,7 +959,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -967,7 +967,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
@@ -975,7 +975,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
@@ -983,22 +983,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C7" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C8" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C9" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C14" s="12" t="s">
         <v>24</v>
       </c>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C15" s="12" t="s">
         <v>25</v>
       </c>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C16" s="12" t="s">
         <v>26</v>
       </c>
@@ -1070,10 +1070,10 @@
       </c>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="9" t="s">
         <v>36</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="9" t="s">
         <v>37</v>
       </c>
@@ -1130,8 +1130,9 @@
         <v>45</v>
       </c>
       <c r="E20" s="18"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="9" t="s">
         <v>38</v>
       </c>
@@ -1142,8 +1143,9 @@
         <v>45</v>
       </c>
       <c r="E21" s="18"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="9" t="s">
         <v>39</v>
       </c>
@@ -1154,8 +1156,9 @@
         <v>45</v>
       </c>
       <c r="E22" s="18"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="9" t="s">
         <v>40</v>
       </c>
@@ -1166,8 +1169,9 @@
         <v>45</v>
       </c>
       <c r="E23" s="18"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="9" t="s">
         <v>41</v>
       </c>
@@ -1178,8 +1182,9 @@
         <v>45</v>
       </c>
       <c r="E24" s="18"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
         <v>42</v>
       </c>
@@ -1190,8 +1195,9 @@
         <v>45</v>
       </c>
       <c r="E25" s="18"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="9" t="s">
         <v>43</v>
       </c>
@@ -1202,8 +1208,9 @@
         <v>45</v>
       </c>
       <c r="E26" s="18"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="9" t="s">
         <v>44</v>
       </c>
@@ -1214,2344 +1221,2345 @@
         <v>45</v>
       </c>
       <c r="E27" s="18"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="10"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="10"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
       <c r="D41" s="10"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
       <c r="D42" s="10"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="10"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="10"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
       <c r="D46" s="10"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
       <c r="D47" s="10"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="10"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
       <c r="D49" s="10"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
       <c r="D51" s="10"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
       <c r="D52" s="10"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
       <c r="D53" s="10"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
       <c r="D54" s="10"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="10"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="10"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="10"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="10"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
       <c r="D61" s="10"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
       <c r="D63" s="10"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
       <c r="D64" s="10"/>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
       <c r="D65" s="10"/>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
       <c r="D66" s="10"/>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
       <c r="D67" s="10"/>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
       <c r="D68" s="10"/>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
       <c r="D69" s="10"/>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
       <c r="D70" s="10"/>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
       <c r="D71" s="10"/>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
       <c r="D72" s="10"/>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
       <c r="D73" s="10"/>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
       <c r="D74" s="10"/>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
       <c r="D75" s="10"/>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
       <c r="D76" s="10"/>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
       <c r="D77" s="10"/>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
       <c r="D78" s="10"/>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
       <c r="D79" s="10"/>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
       <c r="D80" s="10"/>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
       <c r="D81" s="10"/>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
       <c r="D82" s="10"/>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
       <c r="D83" s="10"/>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
       <c r="D84" s="10"/>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
       <c r="D85" s="10"/>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
       <c r="D86" s="10"/>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
       <c r="D87" s="10"/>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
       <c r="D88" s="10"/>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
       <c r="D89" s="10"/>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
       <c r="D90" s="10"/>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
       <c r="D91" s="10"/>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
       <c r="D92" s="10"/>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
       <c r="D93" s="10"/>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
       <c r="D94" s="10"/>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
       <c r="D95" s="10"/>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
       <c r="D96" s="10"/>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
       <c r="D97" s="10"/>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
       <c r="D98" s="10"/>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
       <c r="D99" s="10"/>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
       <c r="D101" s="10"/>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
       <c r="D102" s="10"/>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
       <c r="D103" s="10"/>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
       <c r="D104" s="10"/>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
       <c r="D105" s="10"/>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B106" s="9"/>
       <c r="C106" s="9"/>
       <c r="D106" s="10"/>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
       <c r="D107" s="10"/>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B108" s="9"/>
       <c r="C108" s="9"/>
       <c r="D108" s="10"/>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B109" s="9"/>
       <c r="C109" s="9"/>
       <c r="D109" s="10"/>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B110" s="9"/>
       <c r="C110" s="9"/>
       <c r="D110" s="10"/>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
       <c r="D111" s="10"/>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B112" s="9"/>
       <c r="C112" s="9"/>
       <c r="D112" s="10"/>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
       <c r="D113" s="10"/>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B114" s="9"/>
       <c r="C114" s="9"/>
       <c r="D114" s="10"/>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B115" s="9"/>
       <c r="C115" s="9"/>
       <c r="D115" s="10"/>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B116" s="9"/>
       <c r="C116" s="9"/>
       <c r="D116" s="10"/>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B117" s="9"/>
       <c r="C117" s="9"/>
       <c r="D117" s="10"/>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B118" s="9"/>
       <c r="C118" s="9"/>
       <c r="D118" s="10"/>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B119" s="9"/>
       <c r="C119" s="9"/>
       <c r="D119" s="10"/>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B120" s="9"/>
       <c r="C120" s="9"/>
       <c r="D120" s="10"/>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B121" s="9"/>
       <c r="C121" s="9"/>
       <c r="D121" s="10"/>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B122" s="9"/>
       <c r="C122" s="9"/>
       <c r="D122" s="10"/>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B123" s="9"/>
       <c r="C123" s="9"/>
       <c r="D123" s="10"/>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B124" s="9"/>
       <c r="C124" s="9"/>
       <c r="D124" s="10"/>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B125" s="9"/>
       <c r="C125" s="9"/>
       <c r="D125" s="10"/>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B126" s="9"/>
       <c r="C126" s="9"/>
       <c r="D126" s="10"/>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B127" s="9"/>
       <c r="C127" s="9"/>
       <c r="D127" s="10"/>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B128" s="9"/>
       <c r="C128" s="9"/>
       <c r="D128" s="10"/>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B129" s="9"/>
       <c r="C129" s="9"/>
       <c r="D129" s="10"/>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B130" s="9"/>
       <c r="C130" s="9"/>
       <c r="D130" s="10"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B131" s="9"/>
       <c r="C131" s="9"/>
       <c r="D131" s="10"/>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B132" s="9"/>
       <c r="C132" s="9"/>
       <c r="D132" s="10"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B133" s="9"/>
       <c r="C133" s="9"/>
       <c r="D133" s="10"/>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B134" s="9"/>
       <c r="C134" s="9"/>
       <c r="D134" s="10"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B135" s="9"/>
       <c r="C135" s="9"/>
       <c r="D135" s="10"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B136" s="9"/>
       <c r="C136" s="9"/>
       <c r="D136" s="10"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B137" s="9"/>
       <c r="C137" s="9"/>
       <c r="D137" s="10"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B138" s="9"/>
       <c r="C138" s="9"/>
       <c r="D138" s="10"/>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B139" s="9"/>
       <c r="C139" s="9"/>
       <c r="D139" s="10"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B140" s="9"/>
       <c r="C140" s="9"/>
       <c r="D140" s="10"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B141" s="9"/>
       <c r="C141" s="9"/>
       <c r="D141" s="10"/>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B142" s="9"/>
       <c r="C142" s="9"/>
       <c r="D142" s="10"/>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B143" s="9"/>
       <c r="C143" s="9"/>
       <c r="D143" s="10"/>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B144" s="9"/>
       <c r="C144" s="9"/>
       <c r="D144" s="10"/>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B145" s="9"/>
       <c r="C145" s="9"/>
       <c r="D145" s="10"/>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B146" s="9"/>
       <c r="C146" s="9"/>
       <c r="D146" s="10"/>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B147" s="9"/>
       <c r="C147" s="9"/>
       <c r="D147" s="10"/>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B148" s="9"/>
       <c r="C148" s="9"/>
       <c r="D148" s="10"/>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B149" s="9"/>
       <c r="C149" s="9"/>
       <c r="D149" s="10"/>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B150" s="9"/>
       <c r="C150" s="9"/>
       <c r="D150" s="10"/>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B151" s="9"/>
       <c r="C151" s="9"/>
       <c r="D151" s="10"/>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B152" s="9"/>
       <c r="C152" s="9"/>
       <c r="D152" s="10"/>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B153" s="9"/>
       <c r="C153" s="9"/>
       <c r="D153" s="10"/>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B154" s="9"/>
       <c r="C154" s="9"/>
       <c r="D154" s="10"/>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B155" s="9"/>
       <c r="C155" s="9"/>
       <c r="D155" s="10"/>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B156" s="9"/>
       <c r="C156" s="9"/>
       <c r="D156" s="10"/>
     </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B157" s="9"/>
       <c r="C157" s="9"/>
       <c r="D157" s="10"/>
     </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B158" s="9"/>
       <c r="C158" s="9"/>
       <c r="D158" s="10"/>
     </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B159" s="9"/>
       <c r="C159" s="9"/>
       <c r="D159" s="10"/>
     </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B160" s="9"/>
       <c r="C160" s="9"/>
       <c r="D160" s="10"/>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B161" s="9"/>
       <c r="C161" s="9"/>
       <c r="D161" s="10"/>
     </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B162" s="9"/>
       <c r="C162" s="9"/>
       <c r="D162" s="10"/>
     </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B163" s="9"/>
       <c r="C163" s="9"/>
       <c r="D163" s="10"/>
     </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B164" s="9"/>
       <c r="C164" s="9"/>
       <c r="D164" s="10"/>
     </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B165" s="9"/>
       <c r="C165" s="9"/>
       <c r="D165" s="10"/>
     </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B166" s="9"/>
       <c r="C166" s="9"/>
       <c r="D166" s="10"/>
     </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B167" s="9"/>
       <c r="C167" s="9"/>
       <c r="D167" s="10"/>
     </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B168" s="9"/>
       <c r="C168" s="9"/>
       <c r="D168" s="10"/>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B169" s="9"/>
       <c r="C169" s="9"/>
       <c r="D169" s="10"/>
     </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B170" s="9"/>
       <c r="C170" s="9"/>
       <c r="D170" s="10"/>
     </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B171" s="9"/>
       <c r="C171" s="9"/>
       <c r="D171" s="10"/>
     </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B172" s="9"/>
       <c r="C172" s="9"/>
       <c r="D172" s="10"/>
     </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B173" s="9"/>
       <c r="C173" s="9"/>
       <c r="D173" s="10"/>
     </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B174" s="9"/>
       <c r="C174" s="9"/>
       <c r="D174" s="10"/>
     </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B175" s="9"/>
       <c r="C175" s="9"/>
       <c r="D175" s="10"/>
     </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B176" s="9"/>
       <c r="C176" s="9"/>
       <c r="D176" s="10"/>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B177" s="9"/>
       <c r="C177" s="9"/>
       <c r="D177" s="10"/>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B178" s="9"/>
       <c r="C178" s="9"/>
       <c r="D178" s="10"/>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B179" s="9"/>
       <c r="C179" s="9"/>
       <c r="D179" s="10"/>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B180" s="9"/>
       <c r="C180" s="9"/>
       <c r="D180" s="10"/>
     </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B181" s="9"/>
       <c r="C181" s="9"/>
       <c r="D181" s="10"/>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B182" s="9"/>
       <c r="C182" s="9"/>
       <c r="D182" s="10"/>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B183" s="9"/>
       <c r="C183" s="9"/>
       <c r="D183" s="10"/>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B184" s="9"/>
       <c r="C184" s="9"/>
       <c r="D184" s="10"/>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B185" s="9"/>
       <c r="C185" s="9"/>
       <c r="D185" s="10"/>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B186" s="9"/>
       <c r="C186" s="9"/>
       <c r="D186" s="10"/>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B187" s="9"/>
       <c r="C187" s="9"/>
       <c r="D187" s="10"/>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B188" s="9"/>
       <c r="C188" s="9"/>
       <c r="D188" s="10"/>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B189" s="9"/>
       <c r="C189" s="9"/>
       <c r="D189" s="10"/>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B190" s="9"/>
       <c r="C190" s="9"/>
       <c r="D190" s="10"/>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B191" s="9"/>
       <c r="C191" s="9"/>
       <c r="D191" s="10"/>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B192" s="9"/>
       <c r="C192" s="9"/>
       <c r="D192" s="10"/>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B193" s="9"/>
       <c r="C193" s="9"/>
       <c r="D193" s="10"/>
     </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B194" s="9"/>
       <c r="C194" s="9"/>
       <c r="D194" s="10"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B195" s="9"/>
       <c r="C195" s="9"/>
       <c r="D195" s="10"/>
     </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B196" s="9"/>
       <c r="C196" s="9"/>
       <c r="D196" s="10"/>
     </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B197" s="9"/>
       <c r="C197" s="9"/>
       <c r="D197" s="10"/>
     </row>
-    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B198" s="9"/>
       <c r="C198" s="9"/>
       <c r="D198" s="10"/>
     </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B199" s="9"/>
       <c r="C199" s="9"/>
       <c r="D199" s="10"/>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B200" s="9"/>
       <c r="C200" s="9"/>
       <c r="D200" s="10"/>
     </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B201" s="9"/>
       <c r="C201" s="9"/>
       <c r="D201" s="10"/>
     </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B202" s="9"/>
       <c r="C202" s="9"/>
       <c r="D202" s="10"/>
     </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
       <c r="D203" s="8"/>
     </row>
-    <row r="204" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
       <c r="D204" s="8"/>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
       <c r="D205" s="8"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
       <c r="D206" s="8"/>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
       <c r="D207" s="8"/>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
       <c r="D208" s="8"/>
     </row>
-    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
       <c r="D209" s="8"/>
     </row>
-    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
       <c r="D210" s="8"/>
     </row>
-    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
       <c r="D211" s="8"/>
     </row>
-    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
       <c r="D212" s="8"/>
     </row>
-    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
       <c r="D213" s="8"/>
     </row>
-    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
       <c r="D214" s="8"/>
     </row>
-    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
       <c r="D215" s="8"/>
     </row>
-    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
       <c r="D216" s="8"/>
     </row>
-    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
       <c r="D217" s="8"/>
     </row>
-    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
       <c r="D218" s="8"/>
     </row>
-    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
       <c r="D219" s="8"/>
     </row>
-    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
       <c r="D220" s="8"/>
     </row>
-    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
       <c r="D221" s="8"/>
     </row>
-    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
       <c r="D222" s="8"/>
     </row>
-    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B223" s="2"/>
       <c r="C223" s="2"/>
       <c r="D223" s="8"/>
     </row>
-    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
       <c r="D224" s="8"/>
     </row>
-    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B225" s="2"/>
       <c r="C225" s="2"/>
       <c r="D225" s="8"/>
     </row>
-    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
       <c r="D226" s="8"/>
     </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
       <c r="D227" s="8"/>
     </row>
-    <row r="228" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
       <c r="D228" s="8"/>
     </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B229" s="2"/>
       <c r="C229" s="2"/>
       <c r="D229" s="8"/>
     </row>
-    <row r="230" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
       <c r="D230" s="8"/>
     </row>
-    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
       <c r="D231" s="8"/>
     </row>
-    <row r="232" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B232" s="2"/>
       <c r="C232" s="2"/>
       <c r="D232" s="8"/>
     </row>
-    <row r="233" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B233" s="2"/>
       <c r="C233" s="2"/>
       <c r="D233" s="8"/>
     </row>
-    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B234" s="2"/>
       <c r="C234" s="2"/>
       <c r="D234" s="8"/>
     </row>
-    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B235" s="2"/>
       <c r="C235" s="2"/>
       <c r="D235" s="8"/>
     </row>
-    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B236" s="2"/>
       <c r="C236" s="2"/>
       <c r="D236" s="8"/>
     </row>
-    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B237" s="2"/>
       <c r="C237" s="2"/>
       <c r="D237" s="8"/>
     </row>
-    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B238" s="2"/>
       <c r="C238" s="2"/>
       <c r="D238" s="8"/>
     </row>
-    <row r="239" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B239" s="2"/>
       <c r="C239" s="2"/>
       <c r="D239" s="8"/>
     </row>
-    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B240" s="2"/>
       <c r="C240" s="2"/>
       <c r="D240" s="8"/>
     </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B241" s="2"/>
       <c r="C241" s="2"/>
       <c r="D241" s="8"/>
     </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B242" s="2"/>
       <c r="C242" s="2"/>
       <c r="D242" s="8"/>
     </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B243" s="2"/>
       <c r="C243" s="2"/>
       <c r="D243" s="8"/>
     </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
       <c r="D244" s="8"/>
     </row>
-    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B245" s="2"/>
       <c r="C245" s="2"/>
       <c r="D245" s="8"/>
     </row>
-    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
       <c r="D246" s="8"/>
     </row>
-    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
       <c r="D247" s="8"/>
     </row>
-    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
       <c r="D248" s="8"/>
     </row>
-    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B249" s="2"/>
       <c r="C249" s="2"/>
       <c r="D249" s="8"/>
     </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
       <c r="D250" s="8"/>
     </row>
-    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
       <c r="D251" s="8"/>
     </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
       <c r="D252" s="8"/>
     </row>
-    <row r="253" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
       <c r="D253" s="8"/>
     </row>
-    <row r="254" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
       <c r="D254" s="8"/>
     </row>
-    <row r="255" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
       <c r="D255" s="8"/>
     </row>
-    <row r="256" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
       <c r="D256" s="8"/>
     </row>
-    <row r="257" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
       <c r="D257" s="8"/>
     </row>
-    <row r="258" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
       <c r="D258" s="8"/>
     </row>
-    <row r="259" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B259" s="2"/>
       <c r="C259" s="2"/>
       <c r="D259" s="8"/>
     </row>
-    <row r="260" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
       <c r="D260" s="8"/>
     </row>
-    <row r="261" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>
       <c r="D261" s="8"/>
     </row>
-    <row r="262" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B262" s="2"/>
       <c r="C262" s="2"/>
       <c r="D262" s="8"/>
     </row>
-    <row r="263" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B263" s="2"/>
       <c r="C263" s="2"/>
       <c r="D263" s="8"/>
     </row>
-    <row r="264" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
       <c r="D264" s="8"/>
     </row>
-    <row r="265" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B265" s="2"/>
       <c r="C265" s="2"/>
       <c r="D265" s="8"/>
     </row>
-    <row r="266" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B266" s="2"/>
       <c r="C266" s="2"/>
       <c r="D266" s="8"/>
     </row>
-    <row r="267" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B267" s="2"/>
       <c r="C267" s="2"/>
       <c r="D267" s="8"/>
     </row>
-    <row r="268" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B268" s="2"/>
       <c r="C268" s="2"/>
       <c r="D268" s="8"/>
     </row>
-    <row r="269" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B269" s="2"/>
       <c r="C269" s="2"/>
       <c r="D269" s="8"/>
     </row>
-    <row r="270" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B270" s="2"/>
       <c r="C270" s="2"/>
       <c r="D270" s="8"/>
     </row>
-    <row r="271" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B271" s="2"/>
       <c r="C271" s="2"/>
       <c r="D271" s="8"/>
     </row>
-    <row r="272" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B272" s="2"/>
       <c r="C272" s="2"/>
       <c r="D272" s="8"/>
     </row>
-    <row r="273" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B273" s="2"/>
       <c r="C273" s="2"/>
       <c r="D273" s="8"/>
     </row>
-    <row r="274" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B274" s="2"/>
       <c r="C274" s="2"/>
       <c r="D274" s="8"/>
     </row>
-    <row r="275" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B275" s="2"/>
       <c r="C275" s="2"/>
       <c r="D275" s="8"/>
     </row>
-    <row r="276" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B276" s="2"/>
       <c r="C276" s="2"/>
       <c r="D276" s="8"/>
     </row>
-    <row r="277" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B277" s="2"/>
       <c r="C277" s="2"/>
       <c r="D277" s="8"/>
     </row>
-    <row r="278" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B278" s="2"/>
       <c r="C278" s="2"/>
       <c r="D278" s="8"/>
     </row>
-    <row r="279" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B279" s="2"/>
       <c r="C279" s="2"/>
       <c r="D279" s="8"/>
     </row>
-    <row r="280" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B280" s="2"/>
       <c r="C280" s="2"/>
       <c r="D280" s="8"/>
     </row>
-    <row r="281" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B281" s="2"/>
       <c r="C281" s="2"/>
       <c r="D281" s="8"/>
     </row>
-    <row r="282" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B282" s="2"/>
       <c r="C282" s="2"/>
       <c r="D282" s="8"/>
     </row>
-    <row r="283" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B283" s="2"/>
       <c r="C283" s="2"/>
       <c r="D283" s="8"/>
     </row>
-    <row r="284" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B284" s="2"/>
       <c r="C284" s="2"/>
       <c r="D284" s="8"/>
     </row>
-    <row r="285" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B285" s="2"/>
       <c r="C285" s="2"/>
       <c r="D285" s="8"/>
     </row>
-    <row r="286" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B286" s="2"/>
       <c r="C286" s="2"/>
       <c r="D286" s="8"/>
     </row>
-    <row r="287" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B287" s="2"/>
       <c r="C287" s="2"/>
       <c r="D287" s="8"/>
     </row>
-    <row r="288" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B288" s="2"/>
       <c r="C288" s="2"/>
       <c r="D288" s="8"/>
     </row>
-    <row r="289" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B289" s="2"/>
       <c r="C289" s="2"/>
       <c r="D289" s="8"/>
     </row>
-    <row r="290" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B290" s="2"/>
       <c r="C290" s="2"/>
       <c r="D290" s="8"/>
     </row>
-    <row r="291" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B291" s="2"/>
       <c r="C291" s="2"/>
       <c r="D291" s="8"/>
     </row>
-    <row r="292" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B292" s="2"/>
       <c r="C292" s="2"/>
       <c r="D292" s="8"/>
     </row>
-    <row r="293" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B293" s="2"/>
       <c r="C293" s="2"/>
       <c r="D293" s="8"/>
     </row>
-    <row r="294" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B294" s="2"/>
       <c r="C294" s="2"/>
       <c r="D294" s="8"/>
     </row>
-    <row r="295" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B295" s="2"/>
       <c r="C295" s="2"/>
       <c r="D295" s="8"/>
     </row>
-    <row r="296" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B296" s="2"/>
       <c r="C296" s="2"/>
       <c r="D296" s="8"/>
     </row>
-    <row r="297" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B297" s="2"/>
       <c r="C297" s="2"/>
       <c r="D297" s="8"/>
     </row>
-    <row r="298" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B298" s="2"/>
       <c r="C298" s="2"/>
       <c r="D298" s="8"/>
     </row>
-    <row r="299" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B299" s="2"/>
       <c r="C299" s="2"/>
       <c r="D299" s="8"/>
     </row>
-    <row r="300" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B300" s="2"/>
       <c r="C300" s="2"/>
       <c r="D300" s="8"/>
     </row>
-    <row r="301" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B301" s="2"/>
       <c r="C301" s="2"/>
       <c r="D301" s="8"/>
     </row>
-    <row r="302" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="302" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B302" s="2"/>
       <c r="C302" s="2"/>
       <c r="D302" s="8"/>
     </row>
-    <row r="303" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B303" s="2"/>
       <c r="C303" s="2"/>
       <c r="D303" s="8"/>
     </row>
-    <row r="304" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B304" s="2"/>
       <c r="C304" s="2"/>
       <c r="D304" s="8"/>
     </row>
-    <row r="305" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B305" s="2"/>
       <c r="C305" s="2"/>
       <c r="D305" s="8"/>
     </row>
-    <row r="306" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B306" s="2"/>
       <c r="C306" s="2"/>
       <c r="D306" s="8"/>
     </row>
-    <row r="307" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B307" s="2"/>
       <c r="C307" s="2"/>
       <c r="D307" s="8"/>
     </row>
-    <row r="308" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B308" s="2"/>
       <c r="C308" s="2"/>
       <c r="D308" s="8"/>
     </row>
-    <row r="309" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B309" s="2"/>
       <c r="C309" s="2"/>
       <c r="D309" s="8"/>
     </row>
-    <row r="310" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B310" s="2"/>
       <c r="C310" s="2"/>
       <c r="D310" s="8"/>
     </row>
-    <row r="311" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B311" s="2"/>
       <c r="C311" s="2"/>
       <c r="D311" s="8"/>
     </row>
-    <row r="312" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B312" s="2"/>
       <c r="C312" s="2"/>
       <c r="D312" s="8"/>
     </row>
-    <row r="313" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B313" s="2"/>
       <c r="C313" s="2"/>
       <c r="D313" s="8"/>
     </row>
-    <row r="314" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="314" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B314" s="2"/>
       <c r="C314" s="2"/>
       <c r="D314" s="8"/>
     </row>
-    <row r="315" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="315" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B315" s="2"/>
       <c r="C315" s="2"/>
       <c r="D315" s="8"/>
     </row>
-    <row r="316" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="316" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B316" s="2"/>
       <c r="C316" s="2"/>
       <c r="D316" s="8"/>
     </row>
-    <row r="317" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="317" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B317" s="2"/>
       <c r="C317" s="2"/>
       <c r="D317" s="8"/>
     </row>
-    <row r="318" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="318" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B318" s="2"/>
       <c r="C318" s="2"/>
       <c r="D318" s="8"/>
     </row>
-    <row r="319" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="319" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B319" s="2"/>
       <c r="C319" s="2"/>
       <c r="D319" s="8"/>
     </row>
-    <row r="320" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="320" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B320" s="2"/>
       <c r="C320" s="2"/>
       <c r="D320" s="8"/>
     </row>
-    <row r="321" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B321" s="2"/>
       <c r="C321" s="2"/>
       <c r="D321" s="8"/>
     </row>
-    <row r="322" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="322" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B322" s="2"/>
       <c r="C322" s="2"/>
       <c r="D322" s="8"/>
     </row>
-    <row r="323" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="323" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B323" s="2"/>
       <c r="C323" s="2"/>
       <c r="D323" s="8"/>
     </row>
-    <row r="324" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B324" s="2"/>
       <c r="C324" s="2"/>
       <c r="D324" s="8"/>
     </row>
-    <row r="325" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B325" s="2"/>
       <c r="C325" s="2"/>
       <c r="D325" s="8"/>
     </row>
-    <row r="326" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="326" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B326" s="2"/>
       <c r="C326" s="2"/>
       <c r="D326" s="8"/>
     </row>
-    <row r="327" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="327" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B327" s="2"/>
       <c r="C327" s="2"/>
       <c r="D327" s="8"/>
     </row>
-    <row r="328" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="328" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B328" s="2"/>
       <c r="C328" s="2"/>
       <c r="D328" s="8"/>
     </row>
-    <row r="329" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="329" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B329" s="2"/>
       <c r="C329" s="2"/>
       <c r="D329" s="8"/>
     </row>
-    <row r="330" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="330" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B330" s="2"/>
       <c r="C330" s="2"/>
       <c r="D330" s="8"/>
     </row>
-    <row r="331" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="331" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B331" s="2"/>
       <c r="C331" s="2"/>
       <c r="D331" s="8"/>
     </row>
-    <row r="332" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="332" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B332" s="2"/>
       <c r="C332" s="2"/>
       <c r="D332" s="8"/>
     </row>
-    <row r="333" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="333" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B333" s="2"/>
       <c r="C333" s="2"/>
       <c r="D333" s="8"/>
     </row>
-    <row r="334" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="334" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B334" s="2"/>
       <c r="C334" s="2"/>
       <c r="D334" s="8"/>
     </row>
-    <row r="335" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="335" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B335" s="2"/>
       <c r="C335" s="2"/>
       <c r="D335" s="8"/>
     </row>
-    <row r="336" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="336" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B336" s="2"/>
       <c r="C336" s="2"/>
       <c r="D336" s="8"/>
     </row>
-    <row r="337" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="337" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B337" s="2"/>
       <c r="C337" s="2"/>
       <c r="D337" s="8"/>
     </row>
-    <row r="338" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="338" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B338" s="2"/>
       <c r="C338" s="2"/>
       <c r="D338" s="8"/>
     </row>
-    <row r="339" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="339" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B339" s="2"/>
       <c r="C339" s="2"/>
       <c r="D339" s="8"/>
     </row>
-    <row r="340" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="340" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B340" s="2"/>
       <c r="C340" s="2"/>
       <c r="D340" s="8"/>
     </row>
-    <row r="341" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="341" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B341" s="2"/>
       <c r="C341" s="2"/>
       <c r="D341" s="8"/>
     </row>
-    <row r="342" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="342" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B342" s="2"/>
       <c r="C342" s="2"/>
       <c r="D342" s="8"/>
     </row>
-    <row r="343" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="343" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B343" s="2"/>
       <c r="C343" s="2"/>
       <c r="D343" s="8"/>
     </row>
-    <row r="344" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="344" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B344" s="2"/>
       <c r="C344" s="2"/>
       <c r="D344" s="8"/>
     </row>
-    <row r="345" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="345" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B345" s="2"/>
       <c r="C345" s="2"/>
       <c r="D345" s="8"/>
     </row>
-    <row r="346" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="346" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B346" s="2"/>
       <c r="C346" s="2"/>
       <c r="D346" s="8"/>
     </row>
-    <row r="347" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="347" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B347" s="2"/>
       <c r="C347" s="2"/>
       <c r="D347" s="8"/>
     </row>
-    <row r="348" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="348" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B348" s="2"/>
       <c r="C348" s="2"/>
       <c r="D348" s="8"/>
     </row>
-    <row r="349" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="349" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B349" s="2"/>
       <c r="C349" s="2"/>
       <c r="D349" s="8"/>
     </row>
-    <row r="350" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="350" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B350" s="2"/>
       <c r="C350" s="2"/>
       <c r="D350" s="8"/>
     </row>
-    <row r="351" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="351" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B351" s="2"/>
       <c r="C351" s="2"/>
       <c r="D351" s="8"/>
     </row>
-    <row r="352" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="352" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B352" s="2"/>
       <c r="C352" s="2"/>
       <c r="D352" s="8"/>
     </row>
-    <row r="353" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="353" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B353" s="2"/>
       <c r="C353" s="2"/>
       <c r="D353" s="8"/>
     </row>
-    <row r="354" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="354" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B354" s="2"/>
       <c r="C354" s="2"/>
       <c r="D354" s="8"/>
     </row>
-    <row r="355" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="355" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B355" s="2"/>
       <c r="C355" s="2"/>
       <c r="D355" s="8"/>
     </row>
-    <row r="356" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="356" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B356" s="2"/>
       <c r="C356" s="2"/>
       <c r="D356" s="8"/>
     </row>
-    <row r="357" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="357" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B357" s="2"/>
       <c r="C357" s="2"/>
       <c r="D357" s="8"/>
     </row>
-    <row r="358" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="358" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B358" s="2"/>
       <c r="C358" s="2"/>
       <c r="D358" s="8"/>
     </row>
-    <row r="359" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="359" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B359" s="2"/>
       <c r="C359" s="2"/>
       <c r="D359" s="8"/>
     </row>
-    <row r="360" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="360" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B360" s="2"/>
       <c r="C360" s="2"/>
       <c r="D360" s="8"/>
     </row>
-    <row r="361" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="361" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B361" s="2"/>
       <c r="C361" s="2"/>
       <c r="D361" s="8"/>
     </row>
-    <row r="362" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="362" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B362" s="2"/>
       <c r="C362" s="2"/>
       <c r="D362" s="8"/>
     </row>
-    <row r="363" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="363" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B363" s="2"/>
       <c r="C363" s="2"/>
       <c r="D363" s="8"/>
     </row>
-    <row r="364" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="364" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B364" s="2"/>
       <c r="C364" s="2"/>
       <c r="D364" s="8"/>
     </row>
-    <row r="365" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="365" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B365" s="2"/>
       <c r="C365" s="2"/>
       <c r="D365" s="8"/>
     </row>
-    <row r="366" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="366" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B366" s="2"/>
       <c r="C366" s="2"/>
       <c r="D366" s="8"/>
     </row>
-    <row r="367" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="367" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B367" s="2"/>
       <c r="C367" s="2"/>
       <c r="D367" s="8"/>
     </row>
-    <row r="368" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="368" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B368" s="2"/>
       <c r="C368" s="2"/>
       <c r="D368" s="8"/>
     </row>
-    <row r="369" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="369" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B369" s="2"/>
       <c r="C369" s="2"/>
       <c r="D369" s="8"/>
     </row>
-    <row r="370" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="370" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B370" s="2"/>
       <c r="C370" s="2"/>
       <c r="D370" s="8"/>
     </row>
-    <row r="371" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="371" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B371" s="2"/>
       <c r="C371" s="2"/>
       <c r="D371" s="8"/>
     </row>
-    <row r="372" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="372" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B372" s="2"/>
       <c r="C372" s="2"/>
       <c r="D372" s="8"/>
     </row>
-    <row r="373" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="373" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B373" s="2"/>
       <c r="C373" s="2"/>
       <c r="D373" s="8"/>
     </row>
-    <row r="374" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="374" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B374" s="2"/>
       <c r="C374" s="2"/>
       <c r="D374" s="8"/>
     </row>
-    <row r="375" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="375" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B375" s="2"/>
       <c r="C375" s="2"/>
       <c r="D375" s="8"/>
     </row>
-    <row r="376" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="376" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B376" s="2"/>
       <c r="C376" s="2"/>
       <c r="D376" s="8"/>
     </row>
-    <row r="377" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="377" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B377" s="2"/>
       <c r="C377" s="2"/>
       <c r="D377" s="8"/>
     </row>
-    <row r="378" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="378" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B378" s="2"/>
       <c r="C378" s="2"/>
       <c r="D378" s="8"/>
     </row>
-    <row r="379" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="379" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B379" s="2"/>
       <c r="C379" s="2"/>
       <c r="D379" s="8"/>
     </row>
-    <row r="380" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="380" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B380" s="2"/>
       <c r="C380" s="2"/>
       <c r="D380" s="8"/>
     </row>
-    <row r="381" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="381" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B381" s="2"/>
       <c r="C381" s="2"/>
       <c r="D381" s="8"/>
     </row>
-    <row r="382" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="382" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B382" s="2"/>
       <c r="C382" s="2"/>
       <c r="D382" s="8"/>
     </row>
-    <row r="383" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="383" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B383" s="2"/>
       <c r="C383" s="2"/>
       <c r="D383" s="8"/>
     </row>
-    <row r="384" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="384" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B384" s="2"/>
       <c r="C384" s="2"/>
       <c r="D384" s="8"/>
     </row>
-    <row r="385" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="385" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B385" s="2"/>
       <c r="C385" s="2"/>
       <c r="D385" s="8"/>
     </row>
-    <row r="386" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="386" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B386" s="2"/>
       <c r="C386" s="2"/>
       <c r="D386" s="8"/>
     </row>
-    <row r="387" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="387" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B387" s="2"/>
       <c r="C387" s="2"/>
       <c r="D387" s="8"/>
     </row>
-    <row r="388" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="388" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B388" s="2"/>
       <c r="C388" s="2"/>
       <c r="D388" s="8"/>
     </row>
-    <row r="389" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="389" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B389" s="2"/>
       <c r="C389" s="2"/>
       <c r="D389" s="8"/>
     </row>
-    <row r="390" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="390" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B390" s="2"/>
       <c r="C390" s="2"/>
       <c r="D390" s="8"/>
     </row>
-    <row r="391" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="391" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B391" s="2"/>
       <c r="C391" s="2"/>
       <c r="D391" s="8"/>
     </row>
-    <row r="392" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="392" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B392" s="2"/>
       <c r="C392" s="2"/>
       <c r="D392" s="8"/>
     </row>
-    <row r="393" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="393" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B393" s="2"/>
       <c r="C393" s="2"/>
       <c r="D393" s="8"/>
     </row>
-    <row r="394" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="394" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B394" s="2"/>
       <c r="C394" s="2"/>
       <c r="D394" s="8"/>
     </row>
-    <row r="395" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="395" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B395" s="2"/>
       <c r="C395" s="2"/>
       <c r="D395" s="8"/>
     </row>
-    <row r="396" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="396" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B396" s="2"/>
       <c r="C396" s="2"/>
       <c r="D396" s="8"/>
     </row>
-    <row r="397" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="397" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B397" s="2"/>
       <c r="C397" s="2"/>
       <c r="D397" s="8"/>
     </row>
-    <row r="398" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="398" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B398" s="2"/>
       <c r="C398" s="2"/>
       <c r="D398" s="8"/>
     </row>
-    <row r="399" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="399" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B399" s="2"/>
       <c r="C399" s="2"/>
       <c r="D399" s="8"/>
     </row>
-    <row r="400" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="400" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B400" s="2"/>
       <c r="C400" s="2"/>
       <c r="D400" s="8"/>
     </row>
-    <row r="401" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="401" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B401" s="2"/>
       <c r="C401" s="2"/>
       <c r="D401" s="8"/>
     </row>
-    <row r="402" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="402" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B402" s="2"/>
       <c r="C402" s="2"/>
       <c r="D402" s="8"/>
     </row>
-    <row r="403" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="403" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B403" s="2"/>
       <c r="C403" s="2"/>
       <c r="D403" s="8"/>
     </row>
-    <row r="404" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="404" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D404" s="8"/>
     </row>
-    <row r="405" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="405" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D405" s="8"/>
     </row>
-    <row r="406" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="406" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D406" s="8"/>
     </row>
-    <row r="407" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="407" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D407" s="8"/>
     </row>
-    <row r="408" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="408" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D408" s="8"/>
     </row>
-    <row r="409" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="409" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D409" s="8"/>
     </row>
-    <row r="410" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="410" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D410" s="8"/>
     </row>
-    <row r="411" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="411" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D411" s="8"/>
     </row>
-    <row r="412" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="412" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D412" s="8"/>
     </row>
-    <row r="413" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="413" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D413" s="8"/>
     </row>
-    <row r="414" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="414" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D414" s="8"/>
     </row>
-    <row r="415" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="415" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D415" s="8"/>
     </row>
-    <row r="416" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="416" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D416" s="8"/>
     </row>
-    <row r="417" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="417" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D417" s="8"/>
     </row>
-    <row r="418" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="418" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D418" s="8"/>
     </row>
-    <row r="419" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="419" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D419" s="8"/>
     </row>
-    <row r="420" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="420" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D420" s="8"/>
     </row>
-    <row r="421" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="421" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D421" s="8"/>
     </row>
-    <row r="422" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="422" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D422" s="8"/>
     </row>
-    <row r="423" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="423" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D423" s="8"/>
     </row>
-    <row r="424" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="424" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D424" s="8"/>
     </row>
-    <row r="425" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="425" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D425" s="8"/>
     </row>
-    <row r="426" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="426" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D426" s="8"/>
     </row>
-    <row r="427" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="427" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D427" s="8"/>
     </row>
-    <row r="428" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="428" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D428" s="8"/>
     </row>
-    <row r="429" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="429" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D429" s="8"/>
     </row>
-    <row r="430" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="430" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D430" s="8"/>
     </row>
-    <row r="431" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="431" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D431" s="8"/>
     </row>
-    <row r="432" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="432" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D432" s="8"/>
     </row>
-    <row r="433" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="433" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D433" s="8"/>
     </row>
-    <row r="434" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="434" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D434" s="8"/>
     </row>
-    <row r="435" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="435" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D435" s="8"/>
     </row>
-    <row r="436" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="436" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D436" s="8"/>
     </row>
-    <row r="437" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="437" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D437" s="8"/>
     </row>
-    <row r="438" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="438" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D438" s="8"/>
     </row>
-    <row r="439" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="439" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D439" s="8"/>
     </row>
-    <row r="440" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="440" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D440" s="8"/>
     </row>
-    <row r="441" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="441" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D441" s="8"/>
     </row>
-    <row r="442" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="442" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D442" s="8"/>
     </row>
-    <row r="443" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="443" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D443" s="8"/>
     </row>
-    <row r="444" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="444" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D444" s="8"/>
     </row>
-    <row r="445" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="445" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D445" s="8"/>
     </row>
-    <row r="446" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="446" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D446" s="8"/>
     </row>
-    <row r="447" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="447" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D447" s="8"/>
     </row>
-    <row r="448" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="448" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D448" s="8"/>
     </row>
-    <row r="449" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="449" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D449" s="8"/>
     </row>
-    <row r="450" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="450" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D450" s="8"/>
     </row>
-    <row r="451" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="451" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D451" s="8"/>
     </row>
-    <row r="452" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="452" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D452" s="8"/>
     </row>
-    <row r="453" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="453" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D453" s="8"/>
     </row>
-    <row r="454" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="454" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D454" s="8"/>
     </row>
-    <row r="455" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="455" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D455" s="8"/>
     </row>
-    <row r="456" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="456" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D456" s="8"/>
     </row>
-    <row r="457" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="457" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D457" s="8"/>
     </row>
-    <row r="458" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="458" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D458" s="8"/>
     </row>
-    <row r="459" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="459" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D459" s="8"/>
     </row>
-    <row r="460" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="460" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D460" s="8"/>
     </row>
-    <row r="461" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="461" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D461" s="8"/>
     </row>
-    <row r="462" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="462" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D462" s="8"/>
     </row>
-    <row r="463" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="463" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D463" s="8"/>
     </row>
-    <row r="464" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="464" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D464" s="8"/>
     </row>
-    <row r="465" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="465" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D465" s="8"/>
     </row>
-    <row r="466" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="466" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D466" s="8"/>
     </row>
-    <row r="467" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="467" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D467" s="8"/>
     </row>
-    <row r="468" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="468" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D468" s="8"/>
     </row>
-    <row r="469" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="469" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D469" s="8"/>
     </row>
-    <row r="470" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="470" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D470" s="8"/>
     </row>
-    <row r="471" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="471" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D471" s="8"/>
     </row>
-    <row r="472" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="472" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D472" s="8"/>
     </row>
-    <row r="473" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="473" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D473" s="8"/>
     </row>
-    <row r="474" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="474" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D474" s="8"/>
     </row>
-    <row r="475" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="475" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D475" s="8"/>
     </row>
-    <row r="476" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="476" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D476" s="8"/>
     </row>
-    <row r="477" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="477" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D477" s="8"/>
     </row>
-    <row r="478" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="478" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D478" s="8"/>
     </row>
-    <row r="479" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="479" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D479" s="8"/>
     </row>
-    <row r="480" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="480" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D480" s="8"/>
     </row>
-    <row r="481" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="481" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D481" s="8"/>
     </row>
-    <row r="482" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="482" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D482" s="8"/>
     </row>
-    <row r="483" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="483" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D483" s="8"/>
     </row>
-    <row r="484" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="484" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D484" s="8"/>
     </row>
-    <row r="485" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="485" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D485" s="8"/>
     </row>
-    <row r="486" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="486" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D486" s="8"/>
     </row>
-    <row r="487" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="487" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D487" s="8"/>
     </row>
-    <row r="488" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="488" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D488" s="8"/>
     </row>
-    <row r="489" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="489" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D489" s="8"/>
     </row>
-    <row r="490" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="490" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D490" s="8"/>
     </row>
-    <row r="491" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="491" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D491" s="8"/>
     </row>
-    <row r="492" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="492" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D492" s="8"/>
     </row>
-    <row r="493" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="493" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D493" s="8"/>
     </row>
-    <row r="494" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="494" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D494" s="8"/>
     </row>
-    <row r="495" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="495" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D495" s="8"/>
     </row>
-    <row r="496" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="496" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D496" s="8"/>
     </row>
-    <row r="497" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="497" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D497" s="8"/>
     </row>
-    <row r="498" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="498" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D498" s="8"/>
     </row>
-    <row r="499" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="499" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D499" s="8"/>
     </row>
-    <row r="500" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="500" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D500" s="8"/>
     </row>
-    <row r="501" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="501" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D501" s="8"/>
     </row>
-    <row r="502" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="502" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D502" s="8"/>
     </row>
-    <row r="503" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="503" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D503" s="8"/>
     </row>
-    <row r="504" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="504" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D504" s="8"/>
     </row>
-    <row r="505" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="505" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D505" s="8"/>
     </row>
-    <row r="506" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="506" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D506" s="8"/>
     </row>
-    <row r="507" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="507" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D507" s="8"/>
     </row>
-    <row r="508" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="508" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D508" s="8"/>
     </row>
-    <row r="509" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="509" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D509" s="8"/>
     </row>
-    <row r="510" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="510" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D510" s="8"/>
     </row>
-    <row r="511" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="511" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D511" s="8"/>
     </row>
-    <row r="512" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="512" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D512" s="8"/>
     </row>
-    <row r="513" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="513" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D513" s="8"/>
     </row>
-    <row r="514" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="514" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D514" s="8"/>
     </row>
-    <row r="515" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="515" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D515" s="8"/>
     </row>
-    <row r="516" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="516" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D516" s="8"/>
     </row>
-    <row r="517" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="517" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D517" s="8"/>
     </row>
-    <row r="518" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="518" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D518" s="8"/>
     </row>
-    <row r="519" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="519" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D519" s="8"/>
     </row>
-    <row r="520" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="520" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D520" s="8"/>
     </row>
-    <row r="521" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="521" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D521" s="8"/>
     </row>
-    <row r="522" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="522" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D522" s="8"/>
     </row>
-    <row r="523" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="523" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D523" s="8"/>
     </row>
-    <row r="524" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="524" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D524" s="8"/>
     </row>
-    <row r="525" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="525" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D525" s="8"/>
     </row>
-    <row r="526" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="526" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D526" s="8"/>
     </row>
-    <row r="527" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="527" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D527" s="8"/>
     </row>
-    <row r="528" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="528" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D528" s="8"/>
     </row>
-    <row r="529" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="529" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D529" s="8"/>
     </row>
-    <row r="530" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="530" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D530" s="8"/>
     </row>
-    <row r="531" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="531" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D531" s="8"/>
     </row>
-    <row r="532" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="532" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D532" s="8"/>
     </row>
-    <row r="533" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="533" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D533" s="8"/>
     </row>
-    <row r="534" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="534" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D534" s="8"/>
     </row>
-    <row r="535" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="535" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D535" s="8"/>
     </row>
-    <row r="536" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="536" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D536" s="8"/>
     </row>
-    <row r="537" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="537" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D537" s="8"/>
     </row>
-    <row r="538" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="538" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D538" s="8"/>
     </row>
-    <row r="539" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="539" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D539" s="8"/>
     </row>
-    <row r="540" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="540" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D540" s="8"/>
     </row>
-    <row r="541" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="541" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D541" s="8"/>
     </row>
-    <row r="542" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="542" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D542" s="8"/>
     </row>
-    <row r="543" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="543" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D543" s="8"/>
     </row>
-    <row r="544" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="544" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D544" s="8"/>
     </row>
-    <row r="545" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="545" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D545" s="8"/>
     </row>
-    <row r="546" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="546" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D546" s="8"/>
     </row>
-    <row r="547" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="547" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D547" s="8"/>
     </row>
-    <row r="548" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="548" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D548" s="8"/>
     </row>
-    <row r="549" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="549" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D549" s="8"/>
     </row>
-    <row r="550" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="550" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D550" s="8"/>
     </row>
-    <row r="551" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="551" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D551" s="8"/>
     </row>
-    <row r="552" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="552" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D552" s="8"/>
     </row>
-    <row r="553" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="553" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D553" s="8"/>
     </row>
-    <row r="554" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="554" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D554" s="8"/>
     </row>
-    <row r="555" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="555" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D555" s="8"/>
     </row>
-    <row r="556" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="556" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D556" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update shipping instruction template
</commit_message>
<xml_diff>
--- a/public/template/shipping_instruction_template.xlsx
+++ b/public/template/shipping_instruction_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syedazlan/MyLaravelProjects/gus/public/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Sites\gus\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E938C419-5379-5742-A5B3-3D72BE722463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B5FCA9-D01F-46C0-AF1C-F53A20F9794C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{378D42B6-8EFA-4EF6-9C50-436D539EEED8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{378D42B6-8EFA-4EF6-9C50-436D539EEED8}"/>
   </bookViews>
   <sheets>
     <sheet name="BillOfLading" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -285,7 +285,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -391,8 +391,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7102474" y="209550"/>
-          <a:ext cx="5394326" cy="1581150"/>
+          <a:off x="6229349" y="209550"/>
+          <a:ext cx="4819651" cy="1581150"/>
           <a:chOff x="6029324" y="276225"/>
           <a:chExt cx="4238625" cy="1390650"/>
         </a:xfrm>
@@ -569,7 +569,7 @@
               <a:t>4. </a:t>
             </a:r>
             <a:r>
-              <a:rPr kumimoji="0" lang="en-MY" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:rPr kumimoji="0" lang="en-MY" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
                 <a:ln>
                   <a:noFill/>
                 </a:ln>
@@ -586,7 +586,7 @@
               <a:t>Seperate each document by different </a:t>
             </a:r>
             <a:r>
-              <a:rPr kumimoji="0" lang="en-MY" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:rPr kumimoji="0" lang="en-MY" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
                 <a:ln>
                   <a:noFill/>
                 </a:ln>
@@ -601,6 +601,42 @@
                 <a:cs typeface="+mn-cs"/>
               </a:rPr>
               <a:t>BOX OPERATOR</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr kumimoji="0" lang="en-MY" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:prstClr val="white"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:uLnTx/>
+                <a:uFillTx/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>5. Seal number is required field, use NIL if the container don't have seal</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -936,22 +972,22 @@
   <dimension ref="B2:H556"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="53.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="53.28515625" customWidth="1"/>
     <col min="4" max="4" width="14" style="6" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
-    <col min="6" max="6" width="33.5" customWidth="1"/>
-    <col min="7" max="7" width="23.5" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
@@ -959,7 +995,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -967,7 +1003,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
@@ -975,7 +1011,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
@@ -983,22 +1019,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C7" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C8" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C9" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1013,7 +1049,7 @@
       </c>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
@@ -1028,7 +1064,7 @@
       </c>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1043,7 +1079,7 @@
       </c>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C14" s="12" t="s">
         <v>24</v>
       </c>
@@ -1052,7 +1088,7 @@
       </c>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C15" s="12" t="s">
         <v>25</v>
       </c>
@@ -1061,7 +1097,7 @@
       </c>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C16" s="12" t="s">
         <v>26</v>
       </c>
@@ -1070,10 +1106,10 @@
       </c>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1096,7 +1132,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
         <v>36</v>
       </c>
@@ -1119,7 +1155,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
         <v>37</v>
       </c>
@@ -1132,7 +1168,7 @@
       <c r="E20" s="18"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
         <v>38</v>
       </c>
@@ -1145,7 +1181,7 @@
       <c r="E21" s="18"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
         <v>39</v>
       </c>
@@ -1158,7 +1194,7 @@
       <c r="E22" s="18"/>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
         <v>40</v>
       </c>
@@ -1171,7 +1207,7 @@
       <c r="E23" s="18"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
         <v>41</v>
       </c>
@@ -1184,7 +1220,7 @@
       <c r="E24" s="18"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
         <v>42</v>
       </c>
@@ -1197,7 +1233,7 @@
       <c r="E25" s="18"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
         <v>43</v>
       </c>
@@ -1210,7 +1246,7 @@
       <c r="E26" s="18"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="2:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
         <v>44</v>
       </c>
@@ -1223,2343 +1259,2343 @@
       <c r="E27" s="18"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="10"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="10"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
       <c r="D41" s="10"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
       <c r="D42" s="10"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="10"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="10"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
       <c r="D46" s="10"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
       <c r="D47" s="10"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="10"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
       <c r="D49" s="10"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
       <c r="D51" s="10"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
       <c r="D52" s="10"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
       <c r="D53" s="10"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
       <c r="D54" s="10"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="10"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="10"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="10"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="10"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
       <c r="D61" s="10"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
       <c r="D63" s="10"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
       <c r="D64" s="10"/>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
       <c r="D65" s="10"/>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
       <c r="D66" s="10"/>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
       <c r="D67" s="10"/>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
       <c r="D68" s="10"/>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
       <c r="D69" s="10"/>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
       <c r="D70" s="10"/>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
       <c r="D71" s="10"/>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
       <c r="D72" s="10"/>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
       <c r="D73" s="10"/>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
       <c r="D74" s="10"/>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
       <c r="D75" s="10"/>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
       <c r="D76" s="10"/>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
       <c r="D77" s="10"/>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
       <c r="D78" s="10"/>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
       <c r="D79" s="10"/>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
       <c r="D80" s="10"/>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
       <c r="D81" s="10"/>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
       <c r="D82" s="10"/>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
       <c r="D83" s="10"/>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
       <c r="D84" s="10"/>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
       <c r="D85" s="10"/>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
       <c r="D86" s="10"/>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
       <c r="D87" s="10"/>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
       <c r="D88" s="10"/>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
       <c r="D89" s="10"/>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
       <c r="D90" s="10"/>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
       <c r="D91" s="10"/>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
       <c r="D92" s="10"/>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
       <c r="D93" s="10"/>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
       <c r="D94" s="10"/>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
       <c r="D95" s="10"/>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
       <c r="D96" s="10"/>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
       <c r="D97" s="10"/>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
       <c r="D98" s="10"/>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
       <c r="D99" s="10"/>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
       <c r="D101" s="10"/>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
       <c r="D102" s="10"/>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
       <c r="D103" s="10"/>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
       <c r="D104" s="10"/>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
       <c r="D105" s="10"/>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="9"/>
       <c r="C106" s="9"/>
       <c r="D106" s="10"/>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
       <c r="D107" s="10"/>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" s="9"/>
       <c r="C108" s="9"/>
       <c r="D108" s="10"/>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" s="9"/>
       <c r="C109" s="9"/>
       <c r="D109" s="10"/>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" s="9"/>
       <c r="C110" s="9"/>
       <c r="D110" s="10"/>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
       <c r="D111" s="10"/>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" s="9"/>
       <c r="C112" s="9"/>
       <c r="D112" s="10"/>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
       <c r="D113" s="10"/>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="9"/>
       <c r="C114" s="9"/>
       <c r="D114" s="10"/>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="9"/>
       <c r="C115" s="9"/>
       <c r="D115" s="10"/>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="9"/>
       <c r="C116" s="9"/>
       <c r="D116" s="10"/>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="9"/>
       <c r="C117" s="9"/>
       <c r="D117" s="10"/>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="9"/>
       <c r="C118" s="9"/>
       <c r="D118" s="10"/>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" s="9"/>
       <c r="C119" s="9"/>
       <c r="D119" s="10"/>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" s="9"/>
       <c r="C120" s="9"/>
       <c r="D120" s="10"/>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" s="9"/>
       <c r="C121" s="9"/>
       <c r="D121" s="10"/>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" s="9"/>
       <c r="C122" s="9"/>
       <c r="D122" s="10"/>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" s="9"/>
       <c r="C123" s="9"/>
       <c r="D123" s="10"/>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="9"/>
       <c r="C124" s="9"/>
       <c r="D124" s="10"/>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="9"/>
       <c r="C125" s="9"/>
       <c r="D125" s="10"/>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="9"/>
       <c r="C126" s="9"/>
       <c r="D126" s="10"/>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" s="9"/>
       <c r="C127" s="9"/>
       <c r="D127" s="10"/>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" s="9"/>
       <c r="C128" s="9"/>
       <c r="D128" s="10"/>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" s="9"/>
       <c r="C129" s="9"/>
       <c r="D129" s="10"/>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="9"/>
       <c r="C130" s="9"/>
       <c r="D130" s="10"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" s="9"/>
       <c r="C131" s="9"/>
       <c r="D131" s="10"/>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="9"/>
       <c r="C132" s="9"/>
       <c r="D132" s="10"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" s="9"/>
       <c r="C133" s="9"/>
       <c r="D133" s="10"/>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" s="9"/>
       <c r="C134" s="9"/>
       <c r="D134" s="10"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" s="9"/>
       <c r="C135" s="9"/>
       <c r="D135" s="10"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" s="9"/>
       <c r="C136" s="9"/>
       <c r="D136" s="10"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" s="9"/>
       <c r="C137" s="9"/>
       <c r="D137" s="10"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="9"/>
       <c r="C138" s="9"/>
       <c r="D138" s="10"/>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="9"/>
       <c r="C139" s="9"/>
       <c r="D139" s="10"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140" s="9"/>
       <c r="C140" s="9"/>
       <c r="D140" s="10"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B141" s="9"/>
       <c r="C141" s="9"/>
       <c r="D141" s="10"/>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B142" s="9"/>
       <c r="C142" s="9"/>
       <c r="D142" s="10"/>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B143" s="9"/>
       <c r="C143" s="9"/>
       <c r="D143" s="10"/>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" s="9"/>
       <c r="C144" s="9"/>
       <c r="D144" s="10"/>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B145" s="9"/>
       <c r="C145" s="9"/>
       <c r="D145" s="10"/>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B146" s="9"/>
       <c r="C146" s="9"/>
       <c r="D146" s="10"/>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B147" s="9"/>
       <c r="C147" s="9"/>
       <c r="D147" s="10"/>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B148" s="9"/>
       <c r="C148" s="9"/>
       <c r="D148" s="10"/>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B149" s="9"/>
       <c r="C149" s="9"/>
       <c r="D149" s="10"/>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B150" s="9"/>
       <c r="C150" s="9"/>
       <c r="D150" s="10"/>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B151" s="9"/>
       <c r="C151" s="9"/>
       <c r="D151" s="10"/>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B152" s="9"/>
       <c r="C152" s="9"/>
       <c r="D152" s="10"/>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" s="9"/>
       <c r="C153" s="9"/>
       <c r="D153" s="10"/>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B154" s="9"/>
       <c r="C154" s="9"/>
       <c r="D154" s="10"/>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B155" s="9"/>
       <c r="C155" s="9"/>
       <c r="D155" s="10"/>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B156" s="9"/>
       <c r="C156" s="9"/>
       <c r="D156" s="10"/>
     </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B157" s="9"/>
       <c r="C157" s="9"/>
       <c r="D157" s="10"/>
     </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B158" s="9"/>
       <c r="C158" s="9"/>
       <c r="D158" s="10"/>
     </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B159" s="9"/>
       <c r="C159" s="9"/>
       <c r="D159" s="10"/>
     </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B160" s="9"/>
       <c r="C160" s="9"/>
       <c r="D160" s="10"/>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="9"/>
       <c r="C161" s="9"/>
       <c r="D161" s="10"/>
     </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" s="9"/>
       <c r="C162" s="9"/>
       <c r="D162" s="10"/>
     </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="9"/>
       <c r="C163" s="9"/>
       <c r="D163" s="10"/>
     </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="9"/>
       <c r="C164" s="9"/>
       <c r="D164" s="10"/>
     </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="9"/>
       <c r="C165" s="9"/>
       <c r="D165" s="10"/>
     </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="9"/>
       <c r="C166" s="9"/>
       <c r="D166" s="10"/>
     </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" s="9"/>
       <c r="C167" s="9"/>
       <c r="D167" s="10"/>
     </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="9"/>
       <c r="C168" s="9"/>
       <c r="D168" s="10"/>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="9"/>
       <c r="C169" s="9"/>
       <c r="D169" s="10"/>
     </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="9"/>
       <c r="C170" s="9"/>
       <c r="D170" s="10"/>
     </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="9"/>
       <c r="C171" s="9"/>
       <c r="D171" s="10"/>
     </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" s="9"/>
       <c r="C172" s="9"/>
       <c r="D172" s="10"/>
     </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" s="9"/>
       <c r="C173" s="9"/>
       <c r="D173" s="10"/>
     </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="9"/>
       <c r="C174" s="9"/>
       <c r="D174" s="10"/>
     </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" s="9"/>
       <c r="C175" s="9"/>
       <c r="D175" s="10"/>
     </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" s="9"/>
       <c r="C176" s="9"/>
       <c r="D176" s="10"/>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B177" s="9"/>
       <c r="C177" s="9"/>
       <c r="D177" s="10"/>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B178" s="9"/>
       <c r="C178" s="9"/>
       <c r="D178" s="10"/>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B179" s="9"/>
       <c r="C179" s="9"/>
       <c r="D179" s="10"/>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B180" s="9"/>
       <c r="C180" s="9"/>
       <c r="D180" s="10"/>
     </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B181" s="9"/>
       <c r="C181" s="9"/>
       <c r="D181" s="10"/>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B182" s="9"/>
       <c r="C182" s="9"/>
       <c r="D182" s="10"/>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B183" s="9"/>
       <c r="C183" s="9"/>
       <c r="D183" s="10"/>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B184" s="9"/>
       <c r="C184" s="9"/>
       <c r="D184" s="10"/>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" s="9"/>
       <c r="C185" s="9"/>
       <c r="D185" s="10"/>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B186" s="9"/>
       <c r="C186" s="9"/>
       <c r="D186" s="10"/>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B187" s="9"/>
       <c r="C187" s="9"/>
       <c r="D187" s="10"/>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B188" s="9"/>
       <c r="C188" s="9"/>
       <c r="D188" s="10"/>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B189" s="9"/>
       <c r="C189" s="9"/>
       <c r="D189" s="10"/>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B190" s="9"/>
       <c r="C190" s="9"/>
       <c r="D190" s="10"/>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B191" s="9"/>
       <c r="C191" s="9"/>
       <c r="D191" s="10"/>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B192" s="9"/>
       <c r="C192" s="9"/>
       <c r="D192" s="10"/>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" s="9"/>
       <c r="C193" s="9"/>
       <c r="D193" s="10"/>
     </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" s="9"/>
       <c r="C194" s="9"/>
       <c r="D194" s="10"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" s="9"/>
       <c r="C195" s="9"/>
       <c r="D195" s="10"/>
     </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B196" s="9"/>
       <c r="C196" s="9"/>
       <c r="D196" s="10"/>
     </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B197" s="9"/>
       <c r="C197" s="9"/>
       <c r="D197" s="10"/>
     </row>
-    <row r="198" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B198" s="9"/>
       <c r="C198" s="9"/>
       <c r="D198" s="10"/>
     </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" s="9"/>
       <c r="C199" s="9"/>
       <c r="D199" s="10"/>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B200" s="9"/>
       <c r="C200" s="9"/>
       <c r="D200" s="10"/>
     </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B201" s="9"/>
       <c r="C201" s="9"/>
       <c r="D201" s="10"/>
     </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B202" s="9"/>
       <c r="C202" s="9"/>
       <c r="D202" s="10"/>
     </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
       <c r="D203" s="8"/>
     </row>
-    <row r="204" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
       <c r="D204" s="8"/>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
       <c r="D205" s="8"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
       <c r="D206" s="8"/>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
       <c r="D207" s="8"/>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
       <c r="D208" s="8"/>
     </row>
-    <row r="209" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
       <c r="D209" s="8"/>
     </row>
-    <row r="210" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
       <c r="D210" s="8"/>
     </row>
-    <row r="211" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
       <c r="D211" s="8"/>
     </row>
-    <row r="212" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
       <c r="D212" s="8"/>
     </row>
-    <row r="213" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
       <c r="D213" s="8"/>
     </row>
-    <row r="214" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
       <c r="D214" s="8"/>
     </row>
-    <row r="215" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
       <c r="D215" s="8"/>
     </row>
-    <row r="216" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
       <c r="D216" s="8"/>
     </row>
-    <row r="217" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
       <c r="D217" s="8"/>
     </row>
-    <row r="218" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
       <c r="D218" s="8"/>
     </row>
-    <row r="219" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
       <c r="D219" s="8"/>
     </row>
-    <row r="220" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
       <c r="D220" s="8"/>
     </row>
-    <row r="221" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
       <c r="D221" s="8"/>
     </row>
-    <row r="222" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
       <c r="D222" s="8"/>
     </row>
-    <row r="223" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B223" s="2"/>
       <c r="C223" s="2"/>
       <c r="D223" s="8"/>
     </row>
-    <row r="224" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
       <c r="D224" s="8"/>
     </row>
-    <row r="225" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B225" s="2"/>
       <c r="C225" s="2"/>
       <c r="D225" s="8"/>
     </row>
-    <row r="226" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
       <c r="D226" s="8"/>
     </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
       <c r="D227" s="8"/>
     </row>
-    <row r="228" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
       <c r="D228" s="8"/>
     </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B229" s="2"/>
       <c r="C229" s="2"/>
       <c r="D229" s="8"/>
     </row>
-    <row r="230" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
       <c r="D230" s="8"/>
     </row>
-    <row r="231" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
       <c r="D231" s="8"/>
     </row>
-    <row r="232" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B232" s="2"/>
       <c r="C232" s="2"/>
       <c r="D232" s="8"/>
     </row>
-    <row r="233" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B233" s="2"/>
       <c r="C233" s="2"/>
       <c r="D233" s="8"/>
     </row>
-    <row r="234" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B234" s="2"/>
       <c r="C234" s="2"/>
       <c r="D234" s="8"/>
     </row>
-    <row r="235" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B235" s="2"/>
       <c r="C235" s="2"/>
       <c r="D235" s="8"/>
     </row>
-    <row r="236" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B236" s="2"/>
       <c r="C236" s="2"/>
       <c r="D236" s="8"/>
     </row>
-    <row r="237" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B237" s="2"/>
       <c r="C237" s="2"/>
       <c r="D237" s="8"/>
     </row>
-    <row r="238" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B238" s="2"/>
       <c r="C238" s="2"/>
       <c r="D238" s="8"/>
     </row>
-    <row r="239" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B239" s="2"/>
       <c r="C239" s="2"/>
       <c r="D239" s="8"/>
     </row>
-    <row r="240" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B240" s="2"/>
       <c r="C240" s="2"/>
       <c r="D240" s="8"/>
     </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="2"/>
       <c r="C241" s="2"/>
       <c r="D241" s="8"/>
     </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="2"/>
       <c r="C242" s="2"/>
       <c r="D242" s="8"/>
     </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="2"/>
       <c r="C243" s="2"/>
       <c r="D243" s="8"/>
     </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
       <c r="D244" s="8"/>
     </row>
-    <row r="245" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="2"/>
       <c r="C245" s="2"/>
       <c r="D245" s="8"/>
     </row>
-    <row r="246" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
       <c r="D246" s="8"/>
     </row>
-    <row r="247" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
       <c r="D247" s="8"/>
     </row>
-    <row r="248" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
       <c r="D248" s="8"/>
     </row>
-    <row r="249" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B249" s="2"/>
       <c r="C249" s="2"/>
       <c r="D249" s="8"/>
     </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
       <c r="D250" s="8"/>
     </row>
-    <row r="251" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
       <c r="D251" s="8"/>
     </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
       <c r="D252" s="8"/>
     </row>
-    <row r="253" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="253" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
       <c r="D253" s="8"/>
     </row>
-    <row r="254" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="254" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
       <c r="D254" s="8"/>
     </row>
-    <row r="255" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="255" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
       <c r="D255" s="8"/>
     </row>
-    <row r="256" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="256" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
       <c r="D256" s="8"/>
     </row>
-    <row r="257" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="257" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
       <c r="D257" s="8"/>
     </row>
-    <row r="258" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="258" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
       <c r="D258" s="8"/>
     </row>
-    <row r="259" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="259" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B259" s="2"/>
       <c r="C259" s="2"/>
       <c r="D259" s="8"/>
     </row>
-    <row r="260" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="260" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
       <c r="D260" s="8"/>
     </row>
-    <row r="261" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="261" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>
       <c r="D261" s="8"/>
     </row>
-    <row r="262" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="262" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B262" s="2"/>
       <c r="C262" s="2"/>
       <c r="D262" s="8"/>
     </row>
-    <row r="263" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="263" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B263" s="2"/>
       <c r="C263" s="2"/>
       <c r="D263" s="8"/>
     </row>
-    <row r="264" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="264" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
       <c r="D264" s="8"/>
     </row>
-    <row r="265" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="265" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B265" s="2"/>
       <c r="C265" s="2"/>
       <c r="D265" s="8"/>
     </row>
-    <row r="266" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="266" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B266" s="2"/>
       <c r="C266" s="2"/>
       <c r="D266" s="8"/>
     </row>
-    <row r="267" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="267" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B267" s="2"/>
       <c r="C267" s="2"/>
       <c r="D267" s="8"/>
     </row>
-    <row r="268" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="268" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B268" s="2"/>
       <c r="C268" s="2"/>
       <c r="D268" s="8"/>
     </row>
-    <row r="269" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="269" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B269" s="2"/>
       <c r="C269" s="2"/>
       <c r="D269" s="8"/>
     </row>
-    <row r="270" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="270" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B270" s="2"/>
       <c r="C270" s="2"/>
       <c r="D270" s="8"/>
     </row>
-    <row r="271" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="271" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B271" s="2"/>
       <c r="C271" s="2"/>
       <c r="D271" s="8"/>
     </row>
-    <row r="272" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="272" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B272" s="2"/>
       <c r="C272" s="2"/>
       <c r="D272" s="8"/>
     </row>
-    <row r="273" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="273" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B273" s="2"/>
       <c r="C273" s="2"/>
       <c r="D273" s="8"/>
     </row>
-    <row r="274" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="274" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B274" s="2"/>
       <c r="C274" s="2"/>
       <c r="D274" s="8"/>
     </row>
-    <row r="275" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="275" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B275" s="2"/>
       <c r="C275" s="2"/>
       <c r="D275" s="8"/>
     </row>
-    <row r="276" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="276" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B276" s="2"/>
       <c r="C276" s="2"/>
       <c r="D276" s="8"/>
     </row>
-    <row r="277" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="277" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B277" s="2"/>
       <c r="C277" s="2"/>
       <c r="D277" s="8"/>
     </row>
-    <row r="278" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="278" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B278" s="2"/>
       <c r="C278" s="2"/>
       <c r="D278" s="8"/>
     </row>
-    <row r="279" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="279" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B279" s="2"/>
       <c r="C279" s="2"/>
       <c r="D279" s="8"/>
     </row>
-    <row r="280" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="280" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B280" s="2"/>
       <c r="C280" s="2"/>
       <c r="D280" s="8"/>
     </row>
-    <row r="281" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="281" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B281" s="2"/>
       <c r="C281" s="2"/>
       <c r="D281" s="8"/>
     </row>
-    <row r="282" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="282" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B282" s="2"/>
       <c r="C282" s="2"/>
       <c r="D282" s="8"/>
     </row>
-    <row r="283" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="283" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B283" s="2"/>
       <c r="C283" s="2"/>
       <c r="D283" s="8"/>
     </row>
-    <row r="284" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="284" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B284" s="2"/>
       <c r="C284" s="2"/>
       <c r="D284" s="8"/>
     </row>
-    <row r="285" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="285" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B285" s="2"/>
       <c r="C285" s="2"/>
       <c r="D285" s="8"/>
     </row>
-    <row r="286" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="286" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B286" s="2"/>
       <c r="C286" s="2"/>
       <c r="D286" s="8"/>
     </row>
-    <row r="287" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="287" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B287" s="2"/>
       <c r="C287" s="2"/>
       <c r="D287" s="8"/>
     </row>
-    <row r="288" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="288" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B288" s="2"/>
       <c r="C288" s="2"/>
       <c r="D288" s="8"/>
     </row>
-    <row r="289" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="289" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B289" s="2"/>
       <c r="C289" s="2"/>
       <c r="D289" s="8"/>
     </row>
-    <row r="290" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="290" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B290" s="2"/>
       <c r="C290" s="2"/>
       <c r="D290" s="8"/>
     </row>
-    <row r="291" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="291" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B291" s="2"/>
       <c r="C291" s="2"/>
       <c r="D291" s="8"/>
     </row>
-    <row r="292" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="292" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B292" s="2"/>
       <c r="C292" s="2"/>
       <c r="D292" s="8"/>
     </row>
-    <row r="293" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="293" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B293" s="2"/>
       <c r="C293" s="2"/>
       <c r="D293" s="8"/>
     </row>
-    <row r="294" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="294" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B294" s="2"/>
       <c r="C294" s="2"/>
       <c r="D294" s="8"/>
     </row>
-    <row r="295" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="295" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B295" s="2"/>
       <c r="C295" s="2"/>
       <c r="D295" s="8"/>
     </row>
-    <row r="296" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="296" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B296" s="2"/>
       <c r="C296" s="2"/>
       <c r="D296" s="8"/>
     </row>
-    <row r="297" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="297" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B297" s="2"/>
       <c r="C297" s="2"/>
       <c r="D297" s="8"/>
     </row>
-    <row r="298" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="298" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B298" s="2"/>
       <c r="C298" s="2"/>
       <c r="D298" s="8"/>
     </row>
-    <row r="299" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="299" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B299" s="2"/>
       <c r="C299" s="2"/>
       <c r="D299" s="8"/>
     </row>
-    <row r="300" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="300" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B300" s="2"/>
       <c r="C300" s="2"/>
       <c r="D300" s="8"/>
     </row>
-    <row r="301" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="301" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B301" s="2"/>
       <c r="C301" s="2"/>
       <c r="D301" s="8"/>
     </row>
-    <row r="302" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="302" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B302" s="2"/>
       <c r="C302" s="2"/>
       <c r="D302" s="8"/>
     </row>
-    <row r="303" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="303" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B303" s="2"/>
       <c r="C303" s="2"/>
       <c r="D303" s="8"/>
     </row>
-    <row r="304" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="304" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B304" s="2"/>
       <c r="C304" s="2"/>
       <c r="D304" s="8"/>
     </row>
-    <row r="305" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="305" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B305" s="2"/>
       <c r="C305" s="2"/>
       <c r="D305" s="8"/>
     </row>
-    <row r="306" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="306" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B306" s="2"/>
       <c r="C306" s="2"/>
       <c r="D306" s="8"/>
     </row>
-    <row r="307" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="307" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B307" s="2"/>
       <c r="C307" s="2"/>
       <c r="D307" s="8"/>
     </row>
-    <row r="308" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="308" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B308" s="2"/>
       <c r="C308" s="2"/>
       <c r="D308" s="8"/>
     </row>
-    <row r="309" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="309" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B309" s="2"/>
       <c r="C309" s="2"/>
       <c r="D309" s="8"/>
     </row>
-    <row r="310" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="310" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B310" s="2"/>
       <c r="C310" s="2"/>
       <c r="D310" s="8"/>
     </row>
-    <row r="311" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="311" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B311" s="2"/>
       <c r="C311" s="2"/>
       <c r="D311" s="8"/>
     </row>
-    <row r="312" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="312" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B312" s="2"/>
       <c r="C312" s="2"/>
       <c r="D312" s="8"/>
     </row>
-    <row r="313" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="313" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B313" s="2"/>
       <c r="C313" s="2"/>
       <c r="D313" s="8"/>
     </row>
-    <row r="314" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="314" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B314" s="2"/>
       <c r="C314" s="2"/>
       <c r="D314" s="8"/>
     </row>
-    <row r="315" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="315" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B315" s="2"/>
       <c r="C315" s="2"/>
       <c r="D315" s="8"/>
     </row>
-    <row r="316" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="316" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B316" s="2"/>
       <c r="C316" s="2"/>
       <c r="D316" s="8"/>
     </row>
-    <row r="317" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="317" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B317" s="2"/>
       <c r="C317" s="2"/>
       <c r="D317" s="8"/>
     </row>
-    <row r="318" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="318" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B318" s="2"/>
       <c r="C318" s="2"/>
       <c r="D318" s="8"/>
     </row>
-    <row r="319" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="319" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B319" s="2"/>
       <c r="C319" s="2"/>
       <c r="D319" s="8"/>
     </row>
-    <row r="320" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="320" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B320" s="2"/>
       <c r="C320" s="2"/>
       <c r="D320" s="8"/>
     </row>
-    <row r="321" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="321" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B321" s="2"/>
       <c r="C321" s="2"/>
       <c r="D321" s="8"/>
     </row>
-    <row r="322" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="322" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B322" s="2"/>
       <c r="C322" s="2"/>
       <c r="D322" s="8"/>
     </row>
-    <row r="323" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="323" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B323" s="2"/>
       <c r="C323" s="2"/>
       <c r="D323" s="8"/>
     </row>
-    <row r="324" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="324" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B324" s="2"/>
       <c r="C324" s="2"/>
       <c r="D324" s="8"/>
     </row>
-    <row r="325" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="325" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B325" s="2"/>
       <c r="C325" s="2"/>
       <c r="D325" s="8"/>
     </row>
-    <row r="326" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="326" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B326" s="2"/>
       <c r="C326" s="2"/>
       <c r="D326" s="8"/>
     </row>
-    <row r="327" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="327" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B327" s="2"/>
       <c r="C327" s="2"/>
       <c r="D327" s="8"/>
     </row>
-    <row r="328" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="328" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B328" s="2"/>
       <c r="C328" s="2"/>
       <c r="D328" s="8"/>
     </row>
-    <row r="329" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="329" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B329" s="2"/>
       <c r="C329" s="2"/>
       <c r="D329" s="8"/>
     </row>
-    <row r="330" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="330" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B330" s="2"/>
       <c r="C330" s="2"/>
       <c r="D330" s="8"/>
     </row>
-    <row r="331" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="331" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B331" s="2"/>
       <c r="C331" s="2"/>
       <c r="D331" s="8"/>
     </row>
-    <row r="332" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="332" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B332" s="2"/>
       <c r="C332" s="2"/>
       <c r="D332" s="8"/>
     </row>
-    <row r="333" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="333" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B333" s="2"/>
       <c r="C333" s="2"/>
       <c r="D333" s="8"/>
     </row>
-    <row r="334" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="334" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B334" s="2"/>
       <c r="C334" s="2"/>
       <c r="D334" s="8"/>
     </row>
-    <row r="335" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="335" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B335" s="2"/>
       <c r="C335" s="2"/>
       <c r="D335" s="8"/>
     </row>
-    <row r="336" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="336" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B336" s="2"/>
       <c r="C336" s="2"/>
       <c r="D336" s="8"/>
     </row>
-    <row r="337" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="337" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B337" s="2"/>
       <c r="C337" s="2"/>
       <c r="D337" s="8"/>
     </row>
-    <row r="338" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="338" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B338" s="2"/>
       <c r="C338" s="2"/>
       <c r="D338" s="8"/>
     </row>
-    <row r="339" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="339" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B339" s="2"/>
       <c r="C339" s="2"/>
       <c r="D339" s="8"/>
     </row>
-    <row r="340" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="340" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B340" s="2"/>
       <c r="C340" s="2"/>
       <c r="D340" s="8"/>
     </row>
-    <row r="341" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="341" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B341" s="2"/>
       <c r="C341" s="2"/>
       <c r="D341" s="8"/>
     </row>
-    <row r="342" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="342" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B342" s="2"/>
       <c r="C342" s="2"/>
       <c r="D342" s="8"/>
     </row>
-    <row r="343" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="343" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B343" s="2"/>
       <c r="C343" s="2"/>
       <c r="D343" s="8"/>
     </row>
-    <row r="344" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="344" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B344" s="2"/>
       <c r="C344" s="2"/>
       <c r="D344" s="8"/>
     </row>
-    <row r="345" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="345" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B345" s="2"/>
       <c r="C345" s="2"/>
       <c r="D345" s="8"/>
     </row>
-    <row r="346" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="346" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B346" s="2"/>
       <c r="C346" s="2"/>
       <c r="D346" s="8"/>
     </row>
-    <row r="347" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="347" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B347" s="2"/>
       <c r="C347" s="2"/>
       <c r="D347" s="8"/>
     </row>
-    <row r="348" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="348" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B348" s="2"/>
       <c r="C348" s="2"/>
       <c r="D348" s="8"/>
     </row>
-    <row r="349" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="349" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B349" s="2"/>
       <c r="C349" s="2"/>
       <c r="D349" s="8"/>
     </row>
-    <row r="350" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="350" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B350" s="2"/>
       <c r="C350" s="2"/>
       <c r="D350" s="8"/>
     </row>
-    <row r="351" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="351" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B351" s="2"/>
       <c r="C351" s="2"/>
       <c r="D351" s="8"/>
     </row>
-    <row r="352" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="352" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B352" s="2"/>
       <c r="C352" s="2"/>
       <c r="D352" s="8"/>
     </row>
-    <row r="353" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="353" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B353" s="2"/>
       <c r="C353" s="2"/>
       <c r="D353" s="8"/>
     </row>
-    <row r="354" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="354" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B354" s="2"/>
       <c r="C354" s="2"/>
       <c r="D354" s="8"/>
     </row>
-    <row r="355" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="355" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B355" s="2"/>
       <c r="C355" s="2"/>
       <c r="D355" s="8"/>
     </row>
-    <row r="356" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="356" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B356" s="2"/>
       <c r="C356" s="2"/>
       <c r="D356" s="8"/>
     </row>
-    <row r="357" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="357" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B357" s="2"/>
       <c r="C357" s="2"/>
       <c r="D357" s="8"/>
     </row>
-    <row r="358" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="358" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B358" s="2"/>
       <c r="C358" s="2"/>
       <c r="D358" s="8"/>
     </row>
-    <row r="359" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="359" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B359" s="2"/>
       <c r="C359" s="2"/>
       <c r="D359" s="8"/>
     </row>
-    <row r="360" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="360" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B360" s="2"/>
       <c r="C360" s="2"/>
       <c r="D360" s="8"/>
     </row>
-    <row r="361" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="361" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B361" s="2"/>
       <c r="C361" s="2"/>
       <c r="D361" s="8"/>
     </row>
-    <row r="362" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="362" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B362" s="2"/>
       <c r="C362" s="2"/>
       <c r="D362" s="8"/>
     </row>
-    <row r="363" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="363" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B363" s="2"/>
       <c r="C363" s="2"/>
       <c r="D363" s="8"/>
     </row>
-    <row r="364" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="364" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B364" s="2"/>
       <c r="C364" s="2"/>
       <c r="D364" s="8"/>
     </row>
-    <row r="365" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="365" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B365" s="2"/>
       <c r="C365" s="2"/>
       <c r="D365" s="8"/>
     </row>
-    <row r="366" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="366" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B366" s="2"/>
       <c r="C366" s="2"/>
       <c r="D366" s="8"/>
     </row>
-    <row r="367" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="367" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B367" s="2"/>
       <c r="C367" s="2"/>
       <c r="D367" s="8"/>
     </row>
-    <row r="368" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="368" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B368" s="2"/>
       <c r="C368" s="2"/>
       <c r="D368" s="8"/>
     </row>
-    <row r="369" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="369" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B369" s="2"/>
       <c r="C369" s="2"/>
       <c r="D369" s="8"/>
     </row>
-    <row r="370" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="370" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B370" s="2"/>
       <c r="C370" s="2"/>
       <c r="D370" s="8"/>
     </row>
-    <row r="371" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="371" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B371" s="2"/>
       <c r="C371" s="2"/>
       <c r="D371" s="8"/>
     </row>
-    <row r="372" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="372" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B372" s="2"/>
       <c r="C372" s="2"/>
       <c r="D372" s="8"/>
     </row>
-    <row r="373" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="373" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B373" s="2"/>
       <c r="C373" s="2"/>
       <c r="D373" s="8"/>
     </row>
-    <row r="374" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="374" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B374" s="2"/>
       <c r="C374" s="2"/>
       <c r="D374" s="8"/>
     </row>
-    <row r="375" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="375" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B375" s="2"/>
       <c r="C375" s="2"/>
       <c r="D375" s="8"/>
     </row>
-    <row r="376" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="376" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B376" s="2"/>
       <c r="C376" s="2"/>
       <c r="D376" s="8"/>
     </row>
-    <row r="377" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="377" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B377" s="2"/>
       <c r="C377" s="2"/>
       <c r="D377" s="8"/>
     </row>
-    <row r="378" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="378" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B378" s="2"/>
       <c r="C378" s="2"/>
       <c r="D378" s="8"/>
     </row>
-    <row r="379" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="379" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B379" s="2"/>
       <c r="C379" s="2"/>
       <c r="D379" s="8"/>
     </row>
-    <row r="380" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="380" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B380" s="2"/>
       <c r="C380" s="2"/>
       <c r="D380" s="8"/>
     </row>
-    <row r="381" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="381" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B381" s="2"/>
       <c r="C381" s="2"/>
       <c r="D381" s="8"/>
     </row>
-    <row r="382" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="382" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B382" s="2"/>
       <c r="C382" s="2"/>
       <c r="D382" s="8"/>
     </row>
-    <row r="383" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="383" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B383" s="2"/>
       <c r="C383" s="2"/>
       <c r="D383" s="8"/>
     </row>
-    <row r="384" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="384" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B384" s="2"/>
       <c r="C384" s="2"/>
       <c r="D384" s="8"/>
     </row>
-    <row r="385" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="385" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B385" s="2"/>
       <c r="C385" s="2"/>
       <c r="D385" s="8"/>
     </row>
-    <row r="386" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="386" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B386" s="2"/>
       <c r="C386" s="2"/>
       <c r="D386" s="8"/>
     </row>
-    <row r="387" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="387" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B387" s="2"/>
       <c r="C387" s="2"/>
       <c r="D387" s="8"/>
     </row>
-    <row r="388" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="388" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B388" s="2"/>
       <c r="C388" s="2"/>
       <c r="D388" s="8"/>
     </row>
-    <row r="389" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="389" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B389" s="2"/>
       <c r="C389" s="2"/>
       <c r="D389" s="8"/>
     </row>
-    <row r="390" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="390" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B390" s="2"/>
       <c r="C390" s="2"/>
       <c r="D390" s="8"/>
     </row>
-    <row r="391" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="391" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B391" s="2"/>
       <c r="C391" s="2"/>
       <c r="D391" s="8"/>
     </row>
-    <row r="392" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="392" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B392" s="2"/>
       <c r="C392" s="2"/>
       <c r="D392" s="8"/>
     </row>
-    <row r="393" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="393" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B393" s="2"/>
       <c r="C393" s="2"/>
       <c r="D393" s="8"/>
     </row>
-    <row r="394" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="394" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B394" s="2"/>
       <c r="C394" s="2"/>
       <c r="D394" s="8"/>
     </row>
-    <row r="395" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="395" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B395" s="2"/>
       <c r="C395" s="2"/>
       <c r="D395" s="8"/>
     </row>
-    <row r="396" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="396" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B396" s="2"/>
       <c r="C396" s="2"/>
       <c r="D396" s="8"/>
     </row>
-    <row r="397" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="397" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B397" s="2"/>
       <c r="C397" s="2"/>
       <c r="D397" s="8"/>
     </row>
-    <row r="398" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="398" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B398" s="2"/>
       <c r="C398" s="2"/>
       <c r="D398" s="8"/>
     </row>
-    <row r="399" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="399" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B399" s="2"/>
       <c r="C399" s="2"/>
       <c r="D399" s="8"/>
     </row>
-    <row r="400" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="400" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B400" s="2"/>
       <c r="C400" s="2"/>
       <c r="D400" s="8"/>
     </row>
-    <row r="401" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="401" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B401" s="2"/>
       <c r="C401" s="2"/>
       <c r="D401" s="8"/>
     </row>
-    <row r="402" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="402" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B402" s="2"/>
       <c r="C402" s="2"/>
       <c r="D402" s="8"/>
     </row>
-    <row r="403" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="403" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B403" s="2"/>
       <c r="C403" s="2"/>
       <c r="D403" s="8"/>
     </row>
-    <row r="404" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="404" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D404" s="8"/>
     </row>
-    <row r="405" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="405" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D405" s="8"/>
     </row>
-    <row r="406" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="406" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D406" s="8"/>
     </row>
-    <row r="407" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="407" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D407" s="8"/>
     </row>
-    <row r="408" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="408" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D408" s="8"/>
     </row>
-    <row r="409" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="409" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D409" s="8"/>
     </row>
-    <row r="410" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="410" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D410" s="8"/>
     </row>
-    <row r="411" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="411" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D411" s="8"/>
     </row>
-    <row r="412" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="412" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D412" s="8"/>
     </row>
-    <row r="413" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="413" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D413" s="8"/>
     </row>
-    <row r="414" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="414" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D414" s="8"/>
     </row>
-    <row r="415" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="415" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D415" s="8"/>
     </row>
-    <row r="416" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="416" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D416" s="8"/>
     </row>
-    <row r="417" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="417" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D417" s="8"/>
     </row>
-    <row r="418" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="418" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D418" s="8"/>
     </row>
-    <row r="419" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="419" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D419" s="8"/>
     </row>
-    <row r="420" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="420" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D420" s="8"/>
     </row>
-    <row r="421" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="421" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D421" s="8"/>
     </row>
-    <row r="422" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="422" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D422" s="8"/>
     </row>
-    <row r="423" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="423" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D423" s="8"/>
     </row>
-    <row r="424" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="424" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D424" s="8"/>
     </row>
-    <row r="425" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="425" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D425" s="8"/>
     </row>
-    <row r="426" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="426" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D426" s="8"/>
     </row>
-    <row r="427" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="427" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D427" s="8"/>
     </row>
-    <row r="428" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="428" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D428" s="8"/>
     </row>
-    <row r="429" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="429" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D429" s="8"/>
     </row>
-    <row r="430" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="430" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D430" s="8"/>
     </row>
-    <row r="431" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="431" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D431" s="8"/>
     </row>
-    <row r="432" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="432" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D432" s="8"/>
     </row>
-    <row r="433" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="433" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D433" s="8"/>
     </row>
-    <row r="434" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="434" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D434" s="8"/>
     </row>
-    <row r="435" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="435" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D435" s="8"/>
     </row>
-    <row r="436" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="436" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D436" s="8"/>
     </row>
-    <row r="437" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="437" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D437" s="8"/>
     </row>
-    <row r="438" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="438" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D438" s="8"/>
     </row>
-    <row r="439" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="439" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D439" s="8"/>
     </row>
-    <row r="440" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="440" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D440" s="8"/>
     </row>
-    <row r="441" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="441" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D441" s="8"/>
     </row>
-    <row r="442" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="442" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D442" s="8"/>
     </row>
-    <row r="443" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="443" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D443" s="8"/>
     </row>
-    <row r="444" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="444" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D444" s="8"/>
     </row>
-    <row r="445" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="445" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D445" s="8"/>
     </row>
-    <row r="446" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="446" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D446" s="8"/>
     </row>
-    <row r="447" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="447" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D447" s="8"/>
     </row>
-    <row r="448" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="448" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D448" s="8"/>
     </row>
-    <row r="449" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="449" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D449" s="8"/>
     </row>
-    <row r="450" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="450" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D450" s="8"/>
     </row>
-    <row r="451" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="451" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D451" s="8"/>
     </row>
-    <row r="452" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="452" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D452" s="8"/>
     </row>
-    <row r="453" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="453" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D453" s="8"/>
     </row>
-    <row r="454" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="454" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D454" s="8"/>
     </row>
-    <row r="455" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="455" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D455" s="8"/>
     </row>
-    <row r="456" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="456" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D456" s="8"/>
     </row>
-    <row r="457" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="457" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D457" s="8"/>
     </row>
-    <row r="458" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="458" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D458" s="8"/>
     </row>
-    <row r="459" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="459" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D459" s="8"/>
     </row>
-    <row r="460" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="460" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D460" s="8"/>
     </row>
-    <row r="461" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="461" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D461" s="8"/>
     </row>
-    <row r="462" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="462" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D462" s="8"/>
     </row>
-    <row r="463" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="463" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D463" s="8"/>
     </row>
-    <row r="464" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="464" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D464" s="8"/>
     </row>
-    <row r="465" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="465" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D465" s="8"/>
     </row>
-    <row r="466" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="466" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D466" s="8"/>
     </row>
-    <row r="467" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="467" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D467" s="8"/>
     </row>
-    <row r="468" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="468" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D468" s="8"/>
     </row>
-    <row r="469" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="469" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D469" s="8"/>
     </row>
-    <row r="470" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="470" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D470" s="8"/>
     </row>
-    <row r="471" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="471" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D471" s="8"/>
     </row>
-    <row r="472" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="472" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D472" s="8"/>
     </row>
-    <row r="473" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="473" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D473" s="8"/>
     </row>
-    <row r="474" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="474" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D474" s="8"/>
     </row>
-    <row r="475" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="475" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D475" s="8"/>
     </row>
-    <row r="476" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="476" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D476" s="8"/>
     </row>
-    <row r="477" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="477" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D477" s="8"/>
     </row>
-    <row r="478" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="478" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D478" s="8"/>
     </row>
-    <row r="479" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="479" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D479" s="8"/>
     </row>
-    <row r="480" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="480" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D480" s="8"/>
     </row>
-    <row r="481" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="481" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D481" s="8"/>
     </row>
-    <row r="482" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="482" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D482" s="8"/>
     </row>
-    <row r="483" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="483" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D483" s="8"/>
     </row>
-    <row r="484" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="484" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D484" s="8"/>
     </row>
-    <row r="485" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="485" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D485" s="8"/>
     </row>
-    <row r="486" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="486" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D486" s="8"/>
     </row>
-    <row r="487" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="487" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D487" s="8"/>
     </row>
-    <row r="488" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="488" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D488" s="8"/>
     </row>
-    <row r="489" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="489" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D489" s="8"/>
     </row>
-    <row r="490" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="490" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D490" s="8"/>
     </row>
-    <row r="491" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="491" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D491" s="8"/>
     </row>
-    <row r="492" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="492" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D492" s="8"/>
     </row>
-    <row r="493" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="493" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D493" s="8"/>
     </row>
-    <row r="494" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="494" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D494" s="8"/>
     </row>
-    <row r="495" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="495" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D495" s="8"/>
     </row>
-    <row r="496" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="496" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D496" s="8"/>
     </row>
-    <row r="497" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="497" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D497" s="8"/>
     </row>
-    <row r="498" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="498" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D498" s="8"/>
     </row>
-    <row r="499" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="499" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D499" s="8"/>
     </row>
-    <row r="500" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="500" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D500" s="8"/>
     </row>
-    <row r="501" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="501" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D501" s="8"/>
     </row>
-    <row r="502" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="502" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D502" s="8"/>
     </row>
-    <row r="503" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="503" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D503" s="8"/>
     </row>
-    <row r="504" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="504" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D504" s="8"/>
     </row>
-    <row r="505" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="505" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D505" s="8"/>
     </row>
-    <row r="506" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="506" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D506" s="8"/>
     </row>
-    <row r="507" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="507" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D507" s="8"/>
     </row>
-    <row r="508" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="508" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D508" s="8"/>
     </row>
-    <row r="509" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="509" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D509" s="8"/>
     </row>
-    <row r="510" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="510" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D510" s="8"/>
     </row>
-    <row r="511" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="511" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D511" s="8"/>
     </row>
-    <row r="512" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="512" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D512" s="8"/>
     </row>
-    <row r="513" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="513" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D513" s="8"/>
     </row>
-    <row r="514" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="514" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D514" s="8"/>
     </row>
-    <row r="515" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="515" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D515" s="8"/>
     </row>
-    <row r="516" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="516" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D516" s="8"/>
     </row>
-    <row r="517" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="517" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D517" s="8"/>
     </row>
-    <row r="518" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="518" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D518" s="8"/>
     </row>
-    <row r="519" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="519" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D519" s="8"/>
     </row>
-    <row r="520" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="520" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D520" s="8"/>
     </row>
-    <row r="521" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="521" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D521" s="8"/>
     </row>
-    <row r="522" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="522" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D522" s="8"/>
     </row>
-    <row r="523" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="523" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D523" s="8"/>
     </row>
-    <row r="524" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="524" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D524" s="8"/>
     </row>
-    <row r="525" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="525" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D525" s="8"/>
     </row>
-    <row r="526" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="526" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D526" s="8"/>
     </row>
-    <row r="527" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="527" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D527" s="8"/>
     </row>
-    <row r="528" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="528" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D528" s="8"/>
     </row>
-    <row r="529" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="529" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D529" s="8"/>
     </row>
-    <row r="530" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="530" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D530" s="8"/>
     </row>
-    <row r="531" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="531" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D531" s="8"/>
     </row>
-    <row r="532" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="532" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D532" s="8"/>
     </row>
-    <row r="533" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="533" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D533" s="8"/>
     </row>
-    <row r="534" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="534" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D534" s="8"/>
     </row>
-    <row r="535" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="535" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D535" s="8"/>
     </row>
-    <row r="536" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="536" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D536" s="8"/>
     </row>
-    <row r="537" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="537" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D537" s="8"/>
     </row>
-    <row r="538" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="538" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D538" s="8"/>
     </row>
-    <row r="539" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="539" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D539" s="8"/>
     </row>
-    <row r="540" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="540" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D540" s="8"/>
     </row>
-    <row r="541" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="541" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D541" s="8"/>
     </row>
-    <row r="542" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="542" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D542" s="8"/>
     </row>
-    <row r="543" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="543" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D543" s="8"/>
     </row>
-    <row r="544" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="544" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D544" s="8"/>
     </row>
-    <row r="545" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="545" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D545" s="8"/>
     </row>
-    <row r="546" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="546" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D546" s="8"/>
     </row>
-    <row r="547" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="547" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D547" s="8"/>
     </row>
-    <row r="548" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="548" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D548" s="8"/>
     </row>
-    <row r="549" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="549" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D549" s="8"/>
     </row>
-    <row r="550" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="550" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D550" s="8"/>
     </row>
-    <row r="551" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="551" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D551" s="8"/>
     </row>
-    <row r="552" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="552" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D552" s="8"/>
     </row>
-    <row r="553" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="553" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D553" s="8"/>
     </row>
-    <row r="554" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="554" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D554" s="8"/>
     </row>
-    <row r="555" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="555" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D555" s="8"/>
     </row>
-    <row r="556" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="556" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D556" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add enable edit and disable edit button after telex bl released
</commit_message>
<xml_diff>
--- a/public/template/shipping_instruction_template.xlsx
+++ b/public/template/shipping_instruction_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Sites\gus\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syedazlan/MyLaravelProjects/gus/public/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C6D679-30F9-4700-83F0-F794442A59F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A642CF-7A1C-C44E-BDDA-7F19A915C6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{378D42B6-8EFA-4EF6-9C50-436D539EEED8}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" xr2:uid="{378D42B6-8EFA-4EF6-9C50-436D539EEED8}"/>
   </bookViews>
   <sheets>
     <sheet name="BillOfLading" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -285,7 +285,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -391,8 +391,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6229349" y="209550"/>
-          <a:ext cx="4819651" cy="1581150"/>
+          <a:off x="7102474" y="209550"/>
+          <a:ext cx="5394326" cy="1581150"/>
           <a:chOff x="6029324" y="276225"/>
           <a:chExt cx="4238625" cy="1390650"/>
         </a:xfrm>
@@ -975,19 +975,19 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="53.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="53.33203125" customWidth="1"/>
     <col min="4" max="4" width="14" style="6" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="6" max="6" width="33.5" customWidth="1"/>
+    <col min="7" max="7" width="23.5" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
@@ -995,7 +995,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1019,22 +1019,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C7" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C8" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C9" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C14" s="12" t="s">
         <v>24</v>
       </c>
@@ -1088,7 +1088,7 @@
       </c>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C15" s="12" t="s">
         <v>25</v>
       </c>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C16" s="12" t="s">
         <v>26</v>
       </c>
@@ -1106,10 +1106,10 @@
       </c>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="9" t="s">
         <v>36</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="9" t="s">
         <v>37</v>
       </c>
@@ -1168,7 +1168,7 @@
       <c r="E20" s="18"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="9" t="s">
         <v>38</v>
       </c>
@@ -1181,7 +1181,7 @@
       <c r="E21" s="18"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="9" t="s">
         <v>39</v>
       </c>
@@ -1194,7 +1194,7 @@
       <c r="E22" s="18"/>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="9" t="s">
         <v>40</v>
       </c>
@@ -1207,7 +1207,7 @@
       <c r="E23" s="18"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="9" t="s">
         <v>41</v>
       </c>
@@ -1220,7 +1220,7 @@
       <c r="E24" s="18"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
         <v>42</v>
       </c>
@@ -1233,7 +1233,7 @@
       <c r="E25" s="18"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="9" t="s">
         <v>43</v>
       </c>
@@ -1246,7 +1246,7 @@
       <c r="E26" s="18"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="9" t="s">
         <v>44</v>
       </c>
@@ -1259,2346 +1259,2347 @@
       <c r="E27" s="18"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="10"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="10"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
       <c r="D41" s="10"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
       <c r="D42" s="10"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="10"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="10"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
       <c r="D46" s="10"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
       <c r="D47" s="10"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="10"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
       <c r="D49" s="10"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
       <c r="D51" s="10"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
       <c r="D52" s="10"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
       <c r="D53" s="10"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
       <c r="D54" s="10"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="10"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="10"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="10"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="10"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
       <c r="D61" s="10"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
       <c r="D63" s="10"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
       <c r="D64" s="10"/>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
       <c r="D65" s="10"/>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
       <c r="D66" s="10"/>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
       <c r="D67" s="10"/>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
       <c r="D68" s="10"/>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
       <c r="D69" s="10"/>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
       <c r="D70" s="10"/>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
       <c r="D71" s="10"/>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
       <c r="D72" s="10"/>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
       <c r="D73" s="10"/>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
       <c r="D74" s="10"/>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
       <c r="D75" s="10"/>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
       <c r="D76" s="10"/>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
       <c r="D77" s="10"/>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
       <c r="D78" s="10"/>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
       <c r="D79" s="10"/>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
       <c r="D80" s="10"/>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
       <c r="D81" s="10"/>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
       <c r="D82" s="10"/>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
       <c r="D83" s="10"/>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
       <c r="D84" s="10"/>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
       <c r="D85" s="10"/>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
       <c r="D86" s="10"/>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
       <c r="D87" s="10"/>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
       <c r="D88" s="10"/>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
       <c r="D89" s="10"/>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
       <c r="D90" s="10"/>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
       <c r="D91" s="10"/>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
       <c r="D92" s="10"/>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
       <c r="D93" s="10"/>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
       <c r="D94" s="10"/>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
       <c r="D95" s="10"/>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
       <c r="D96" s="10"/>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
       <c r="D97" s="10"/>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
       <c r="D98" s="10"/>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
       <c r="D99" s="10"/>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
       <c r="D101" s="10"/>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
       <c r="D102" s="10"/>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
       <c r="D103" s="10"/>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
       <c r="D104" s="10"/>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
       <c r="D105" s="10"/>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B106" s="9"/>
       <c r="C106" s="9"/>
       <c r="D106" s="10"/>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
       <c r="D107" s="10"/>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B108" s="9"/>
       <c r="C108" s="9"/>
       <c r="D108" s="10"/>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B109" s="9"/>
       <c r="C109" s="9"/>
       <c r="D109" s="10"/>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B110" s="9"/>
       <c r="C110" s="9"/>
       <c r="D110" s="10"/>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
       <c r="D111" s="10"/>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B112" s="9"/>
       <c r="C112" s="9"/>
       <c r="D112" s="10"/>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
       <c r="D113" s="10"/>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B114" s="9"/>
       <c r="C114" s="9"/>
       <c r="D114" s="10"/>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B115" s="9"/>
       <c r="C115" s="9"/>
       <c r="D115" s="10"/>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B116" s="9"/>
       <c r="C116" s="9"/>
       <c r="D116" s="10"/>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B117" s="9"/>
       <c r="C117" s="9"/>
       <c r="D117" s="10"/>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B118" s="9"/>
       <c r="C118" s="9"/>
       <c r="D118" s="10"/>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B119" s="9"/>
       <c r="C119" s="9"/>
       <c r="D119" s="10"/>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B120" s="9"/>
       <c r="C120" s="9"/>
       <c r="D120" s="10"/>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B121" s="9"/>
       <c r="C121" s="9"/>
       <c r="D121" s="10"/>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B122" s="9"/>
       <c r="C122" s="9"/>
       <c r="D122" s="10"/>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B123" s="9"/>
       <c r="C123" s="9"/>
       <c r="D123" s="10"/>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B124" s="9"/>
       <c r="C124" s="9"/>
       <c r="D124" s="10"/>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B125" s="9"/>
       <c r="C125" s="9"/>
       <c r="D125" s="10"/>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B126" s="9"/>
       <c r="C126" s="9"/>
       <c r="D126" s="10"/>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B127" s="9"/>
       <c r="C127" s="9"/>
       <c r="D127" s="10"/>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B128" s="9"/>
       <c r="C128" s="9"/>
       <c r="D128" s="10"/>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B129" s="9"/>
       <c r="C129" s="9"/>
       <c r="D129" s="10"/>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B130" s="9"/>
       <c r="C130" s="9"/>
       <c r="D130" s="10"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B131" s="9"/>
       <c r="C131" s="9"/>
       <c r="D131" s="10"/>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B132" s="9"/>
       <c r="C132" s="9"/>
       <c r="D132" s="10"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B133" s="9"/>
       <c r="C133" s="9"/>
       <c r="D133" s="10"/>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B134" s="9"/>
       <c r="C134" s="9"/>
       <c r="D134" s="10"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B135" s="9"/>
       <c r="C135" s="9"/>
       <c r="D135" s="10"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B136" s="9"/>
       <c r="C136" s="9"/>
       <c r="D136" s="10"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B137" s="9"/>
       <c r="C137" s="9"/>
       <c r="D137" s="10"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B138" s="9"/>
       <c r="C138" s="9"/>
       <c r="D138" s="10"/>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B139" s="9"/>
       <c r="C139" s="9"/>
       <c r="D139" s="10"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B140" s="9"/>
       <c r="C140" s="9"/>
       <c r="D140" s="10"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B141" s="9"/>
       <c r="C141" s="9"/>
       <c r="D141" s="10"/>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B142" s="9"/>
       <c r="C142" s="9"/>
       <c r="D142" s="10"/>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B143" s="9"/>
       <c r="C143" s="9"/>
       <c r="D143" s="10"/>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B144" s="9"/>
       <c r="C144" s="9"/>
       <c r="D144" s="10"/>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B145" s="9"/>
       <c r="C145" s="9"/>
       <c r="D145" s="10"/>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B146" s="9"/>
       <c r="C146" s="9"/>
       <c r="D146" s="10"/>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B147" s="9"/>
       <c r="C147" s="9"/>
       <c r="D147" s="10"/>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B148" s="9"/>
       <c r="C148" s="9"/>
       <c r="D148" s="10"/>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B149" s="9"/>
       <c r="C149" s="9"/>
       <c r="D149" s="10"/>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B150" s="9"/>
       <c r="C150" s="9"/>
       <c r="D150" s="10"/>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B151" s="9"/>
       <c r="C151" s="9"/>
       <c r="D151" s="10"/>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B152" s="9"/>
       <c r="C152" s="9"/>
       <c r="D152" s="10"/>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B153" s="9"/>
       <c r="C153" s="9"/>
       <c r="D153" s="10"/>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B154" s="9"/>
       <c r="C154" s="9"/>
       <c r="D154" s="10"/>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B155" s="9"/>
       <c r="C155" s="9"/>
       <c r="D155" s="10"/>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B156" s="9"/>
       <c r="C156" s="9"/>
       <c r="D156" s="10"/>
     </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B157" s="9"/>
       <c r="C157" s="9"/>
       <c r="D157" s="10"/>
     </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B158" s="9"/>
       <c r="C158" s="9"/>
       <c r="D158" s="10"/>
     </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B159" s="9"/>
       <c r="C159" s="9"/>
       <c r="D159" s="10"/>
     </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B160" s="9"/>
       <c r="C160" s="9"/>
       <c r="D160" s="10"/>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B161" s="9"/>
       <c r="C161" s="9"/>
       <c r="D161" s="10"/>
     </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B162" s="9"/>
       <c r="C162" s="9"/>
       <c r="D162" s="10"/>
     </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B163" s="9"/>
       <c r="C163" s="9"/>
       <c r="D163" s="10"/>
     </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B164" s="9"/>
       <c r="C164" s="9"/>
       <c r="D164" s="10"/>
     </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B165" s="9"/>
       <c r="C165" s="9"/>
       <c r="D165" s="10"/>
     </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B166" s="9"/>
       <c r="C166" s="9"/>
       <c r="D166" s="10"/>
     </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B167" s="9"/>
       <c r="C167" s="9"/>
       <c r="D167" s="10"/>
     </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B168" s="9"/>
       <c r="C168" s="9"/>
       <c r="D168" s="10"/>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B169" s="9"/>
       <c r="C169" s="9"/>
       <c r="D169" s="10"/>
     </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B170" s="9"/>
       <c r="C170" s="9"/>
       <c r="D170" s="10"/>
     </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B171" s="9"/>
       <c r="C171" s="9"/>
       <c r="D171" s="10"/>
     </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B172" s="9"/>
       <c r="C172" s="9"/>
       <c r="D172" s="10"/>
     </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B173" s="9"/>
       <c r="C173" s="9"/>
       <c r="D173" s="10"/>
     </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B174" s="9"/>
       <c r="C174" s="9"/>
       <c r="D174" s="10"/>
     </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B175" s="9"/>
       <c r="C175" s="9"/>
       <c r="D175" s="10"/>
     </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B176" s="9"/>
       <c r="C176" s="9"/>
       <c r="D176" s="10"/>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B177" s="9"/>
       <c r="C177" s="9"/>
       <c r="D177" s="10"/>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B178" s="9"/>
       <c r="C178" s="9"/>
       <c r="D178" s="10"/>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B179" s="9"/>
       <c r="C179" s="9"/>
       <c r="D179" s="10"/>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B180" s="9"/>
       <c r="C180" s="9"/>
       <c r="D180" s="10"/>
     </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B181" s="9"/>
       <c r="C181" s="9"/>
       <c r="D181" s="10"/>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B182" s="9"/>
       <c r="C182" s="9"/>
       <c r="D182" s="10"/>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B183" s="9"/>
       <c r="C183" s="9"/>
       <c r="D183" s="10"/>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B184" s="9"/>
       <c r="C184" s="9"/>
       <c r="D184" s="10"/>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B185" s="9"/>
       <c r="C185" s="9"/>
       <c r="D185" s="10"/>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B186" s="9"/>
       <c r="C186" s="9"/>
       <c r="D186" s="10"/>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B187" s="9"/>
       <c r="C187" s="9"/>
       <c r="D187" s="10"/>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B188" s="9"/>
       <c r="C188" s="9"/>
       <c r="D188" s="10"/>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B189" s="9"/>
       <c r="C189" s="9"/>
       <c r="D189" s="10"/>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B190" s="9"/>
       <c r="C190" s="9"/>
       <c r="D190" s="10"/>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B191" s="9"/>
       <c r="C191" s="9"/>
       <c r="D191" s="10"/>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B192" s="9"/>
       <c r="C192" s="9"/>
       <c r="D192" s="10"/>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B193" s="9"/>
       <c r="C193" s="9"/>
       <c r="D193" s="10"/>
     </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B194" s="9"/>
       <c r="C194" s="9"/>
       <c r="D194" s="10"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B195" s="9"/>
       <c r="C195" s="9"/>
       <c r="D195" s="10"/>
     </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B196" s="9"/>
       <c r="C196" s="9"/>
       <c r="D196" s="10"/>
     </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B197" s="9"/>
       <c r="C197" s="9"/>
       <c r="D197" s="10"/>
     </row>
-    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B198" s="9"/>
       <c r="C198" s="9"/>
       <c r="D198" s="10"/>
     </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B199" s="9"/>
       <c r="C199" s="9"/>
       <c r="D199" s="10"/>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B200" s="9"/>
       <c r="C200" s="9"/>
       <c r="D200" s="10"/>
     </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B201" s="9"/>
       <c r="C201" s="9"/>
       <c r="D201" s="10"/>
     </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B202" s="9"/>
       <c r="C202" s="9"/>
       <c r="D202" s="10"/>
     </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
       <c r="D203" s="8"/>
     </row>
-    <row r="204" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
       <c r="D204" s="8"/>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
       <c r="D205" s="8"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
       <c r="D206" s="8"/>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
       <c r="D207" s="8"/>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
       <c r="D208" s="8"/>
     </row>
-    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
       <c r="D209" s="8"/>
     </row>
-    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
       <c r="D210" s="8"/>
     </row>
-    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
       <c r="D211" s="8"/>
     </row>
-    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
       <c r="D212" s="8"/>
     </row>
-    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
       <c r="D213" s="8"/>
     </row>
-    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
       <c r="D214" s="8"/>
     </row>
-    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
       <c r="D215" s="8"/>
     </row>
-    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
       <c r="D216" s="8"/>
     </row>
-    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
       <c r="D217" s="8"/>
     </row>
-    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
       <c r="D218" s="8"/>
     </row>
-    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
       <c r="D219" s="8"/>
     </row>
-    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
       <c r="D220" s="8"/>
     </row>
-    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
       <c r="D221" s="8"/>
     </row>
-    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
       <c r="D222" s="8"/>
     </row>
-    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B223" s="2"/>
       <c r="C223" s="2"/>
       <c r="D223" s="8"/>
     </row>
-    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
       <c r="D224" s="8"/>
     </row>
-    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B225" s="2"/>
       <c r="C225" s="2"/>
       <c r="D225" s="8"/>
     </row>
-    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
       <c r="D226" s="8"/>
     </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
       <c r="D227" s="8"/>
     </row>
-    <row r="228" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
       <c r="D228" s="8"/>
     </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B229" s="2"/>
       <c r="C229" s="2"/>
       <c r="D229" s="8"/>
     </row>
-    <row r="230" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
       <c r="D230" s="8"/>
     </row>
-    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
       <c r="D231" s="8"/>
     </row>
-    <row r="232" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B232" s="2"/>
       <c r="C232" s="2"/>
       <c r="D232" s="8"/>
     </row>
-    <row r="233" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B233" s="2"/>
       <c r="C233" s="2"/>
       <c r="D233" s="8"/>
     </row>
-    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B234" s="2"/>
       <c r="C234" s="2"/>
       <c r="D234" s="8"/>
     </row>
-    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B235" s="2"/>
       <c r="C235" s="2"/>
       <c r="D235" s="8"/>
     </row>
-    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B236" s="2"/>
       <c r="C236" s="2"/>
       <c r="D236" s="8"/>
     </row>
-    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B237" s="2"/>
       <c r="C237" s="2"/>
       <c r="D237" s="8"/>
     </row>
-    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B238" s="2"/>
       <c r="C238" s="2"/>
       <c r="D238" s="8"/>
     </row>
-    <row r="239" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B239" s="2"/>
       <c r="C239" s="2"/>
       <c r="D239" s="8"/>
     </row>
-    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B240" s="2"/>
       <c r="C240" s="2"/>
       <c r="D240" s="8"/>
     </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B241" s="2"/>
       <c r="C241" s="2"/>
       <c r="D241" s="8"/>
     </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B242" s="2"/>
       <c r="C242" s="2"/>
       <c r="D242" s="8"/>
     </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B243" s="2"/>
       <c r="C243" s="2"/>
       <c r="D243" s="8"/>
     </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
       <c r="D244" s="8"/>
     </row>
-    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B245" s="2"/>
       <c r="C245" s="2"/>
       <c r="D245" s="8"/>
     </row>
-    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
       <c r="D246" s="8"/>
     </row>
-    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
       <c r="D247" s="8"/>
     </row>
-    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
       <c r="D248" s="8"/>
     </row>
-    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B249" s="2"/>
       <c r="C249" s="2"/>
       <c r="D249" s="8"/>
     </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
       <c r="D250" s="8"/>
     </row>
-    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
       <c r="D251" s="8"/>
     </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
       <c r="D252" s="8"/>
     </row>
-    <row r="253" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
       <c r="D253" s="8"/>
     </row>
-    <row r="254" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
       <c r="D254" s="8"/>
     </row>
-    <row r="255" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
       <c r="D255" s="8"/>
     </row>
-    <row r="256" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
       <c r="D256" s="8"/>
     </row>
-    <row r="257" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
       <c r="D257" s="8"/>
     </row>
-    <row r="258" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
       <c r="D258" s="8"/>
     </row>
-    <row r="259" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B259" s="2"/>
       <c r="C259" s="2"/>
       <c r="D259" s="8"/>
     </row>
-    <row r="260" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
       <c r="D260" s="8"/>
     </row>
-    <row r="261" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>
       <c r="D261" s="8"/>
     </row>
-    <row r="262" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B262" s="2"/>
       <c r="C262" s="2"/>
       <c r="D262" s="8"/>
     </row>
-    <row r="263" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B263" s="2"/>
       <c r="C263" s="2"/>
       <c r="D263" s="8"/>
     </row>
-    <row r="264" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
       <c r="D264" s="8"/>
     </row>
-    <row r="265" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B265" s="2"/>
       <c r="C265" s="2"/>
       <c r="D265" s="8"/>
     </row>
-    <row r="266" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B266" s="2"/>
       <c r="C266" s="2"/>
       <c r="D266" s="8"/>
     </row>
-    <row r="267" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B267" s="2"/>
       <c r="C267" s="2"/>
       <c r="D267" s="8"/>
     </row>
-    <row r="268" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B268" s="2"/>
       <c r="C268" s="2"/>
       <c r="D268" s="8"/>
     </row>
-    <row r="269" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B269" s="2"/>
       <c r="C269" s="2"/>
       <c r="D269" s="8"/>
     </row>
-    <row r="270" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B270" s="2"/>
       <c r="C270" s="2"/>
       <c r="D270" s="8"/>
     </row>
-    <row r="271" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B271" s="2"/>
       <c r="C271" s="2"/>
       <c r="D271" s="8"/>
     </row>
-    <row r="272" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B272" s="2"/>
       <c r="C272" s="2"/>
       <c r="D272" s="8"/>
     </row>
-    <row r="273" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B273" s="2"/>
       <c r="C273" s="2"/>
       <c r="D273" s="8"/>
     </row>
-    <row r="274" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B274" s="2"/>
       <c r="C274" s="2"/>
       <c r="D274" s="8"/>
     </row>
-    <row r="275" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B275" s="2"/>
       <c r="C275" s="2"/>
       <c r="D275" s="8"/>
     </row>
-    <row r="276" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B276" s="2"/>
       <c r="C276" s="2"/>
       <c r="D276" s="8"/>
     </row>
-    <row r="277" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B277" s="2"/>
       <c r="C277" s="2"/>
       <c r="D277" s="8"/>
     </row>
-    <row r="278" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B278" s="2"/>
       <c r="C278" s="2"/>
       <c r="D278" s="8"/>
     </row>
-    <row r="279" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B279" s="2"/>
       <c r="C279" s="2"/>
       <c r="D279" s="8"/>
     </row>
-    <row r="280" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B280" s="2"/>
       <c r="C280" s="2"/>
       <c r="D280" s="8"/>
     </row>
-    <row r="281" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B281" s="2"/>
       <c r="C281" s="2"/>
       <c r="D281" s="8"/>
     </row>
-    <row r="282" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B282" s="2"/>
       <c r="C282" s="2"/>
       <c r="D282" s="8"/>
     </row>
-    <row r="283" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B283" s="2"/>
       <c r="C283" s="2"/>
       <c r="D283" s="8"/>
     </row>
-    <row r="284" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B284" s="2"/>
       <c r="C284" s="2"/>
       <c r="D284" s="8"/>
     </row>
-    <row r="285" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B285" s="2"/>
       <c r="C285" s="2"/>
       <c r="D285" s="8"/>
     </row>
-    <row r="286" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B286" s="2"/>
       <c r="C286" s="2"/>
       <c r="D286" s="8"/>
     </row>
-    <row r="287" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B287" s="2"/>
       <c r="C287" s="2"/>
       <c r="D287" s="8"/>
     </row>
-    <row r="288" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B288" s="2"/>
       <c r="C288" s="2"/>
       <c r="D288" s="8"/>
     </row>
-    <row r="289" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B289" s="2"/>
       <c r="C289" s="2"/>
       <c r="D289" s="8"/>
     </row>
-    <row r="290" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B290" s="2"/>
       <c r="C290" s="2"/>
       <c r="D290" s="8"/>
     </row>
-    <row r="291" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B291" s="2"/>
       <c r="C291" s="2"/>
       <c r="D291" s="8"/>
     </row>
-    <row r="292" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B292" s="2"/>
       <c r="C292" s="2"/>
       <c r="D292" s="8"/>
     </row>
-    <row r="293" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B293" s="2"/>
       <c r="C293" s="2"/>
       <c r="D293" s="8"/>
     </row>
-    <row r="294" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B294" s="2"/>
       <c r="C294" s="2"/>
       <c r="D294" s="8"/>
     </row>
-    <row r="295" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B295" s="2"/>
       <c r="C295" s="2"/>
       <c r="D295" s="8"/>
     </row>
-    <row r="296" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B296" s="2"/>
       <c r="C296" s="2"/>
       <c r="D296" s="8"/>
     </row>
-    <row r="297" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B297" s="2"/>
       <c r="C297" s="2"/>
       <c r="D297" s="8"/>
     </row>
-    <row r="298" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B298" s="2"/>
       <c r="C298" s="2"/>
       <c r="D298" s="8"/>
     </row>
-    <row r="299" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B299" s="2"/>
       <c r="C299" s="2"/>
       <c r="D299" s="8"/>
     </row>
-    <row r="300" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B300" s="2"/>
       <c r="C300" s="2"/>
       <c r="D300" s="8"/>
     </row>
-    <row r="301" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B301" s="2"/>
       <c r="C301" s="2"/>
       <c r="D301" s="8"/>
     </row>
-    <row r="302" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="302" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B302" s="2"/>
       <c r="C302" s="2"/>
       <c r="D302" s="8"/>
     </row>
-    <row r="303" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B303" s="2"/>
       <c r="C303" s="2"/>
       <c r="D303" s="8"/>
     </row>
-    <row r="304" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B304" s="2"/>
       <c r="C304" s="2"/>
       <c r="D304" s="8"/>
     </row>
-    <row r="305" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B305" s="2"/>
       <c r="C305" s="2"/>
       <c r="D305" s="8"/>
     </row>
-    <row r="306" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B306" s="2"/>
       <c r="C306" s="2"/>
       <c r="D306" s="8"/>
     </row>
-    <row r="307" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B307" s="2"/>
       <c r="C307" s="2"/>
       <c r="D307" s="8"/>
     </row>
-    <row r="308" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B308" s="2"/>
       <c r="C308" s="2"/>
       <c r="D308" s="8"/>
     </row>
-    <row r="309" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B309" s="2"/>
       <c r="C309" s="2"/>
       <c r="D309" s="8"/>
     </row>
-    <row r="310" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B310" s="2"/>
       <c r="C310" s="2"/>
       <c r="D310" s="8"/>
     </row>
-    <row r="311" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B311" s="2"/>
       <c r="C311" s="2"/>
       <c r="D311" s="8"/>
     </row>
-    <row r="312" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B312" s="2"/>
       <c r="C312" s="2"/>
       <c r="D312" s="8"/>
     </row>
-    <row r="313" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B313" s="2"/>
       <c r="C313" s="2"/>
       <c r="D313" s="8"/>
     </row>
-    <row r="314" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="314" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B314" s="2"/>
       <c r="C314" s="2"/>
       <c r="D314" s="8"/>
     </row>
-    <row r="315" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="315" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B315" s="2"/>
       <c r="C315" s="2"/>
       <c r="D315" s="8"/>
     </row>
-    <row r="316" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="316" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B316" s="2"/>
       <c r="C316" s="2"/>
       <c r="D316" s="8"/>
     </row>
-    <row r="317" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="317" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B317" s="2"/>
       <c r="C317" s="2"/>
       <c r="D317" s="8"/>
     </row>
-    <row r="318" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="318" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B318" s="2"/>
       <c r="C318" s="2"/>
       <c r="D318" s="8"/>
     </row>
-    <row r="319" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="319" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B319" s="2"/>
       <c r="C319" s="2"/>
       <c r="D319" s="8"/>
     </row>
-    <row r="320" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="320" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B320" s="2"/>
       <c r="C320" s="2"/>
       <c r="D320" s="8"/>
     </row>
-    <row r="321" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B321" s="2"/>
       <c r="C321" s="2"/>
       <c r="D321" s="8"/>
     </row>
-    <row r="322" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="322" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B322" s="2"/>
       <c r="C322" s="2"/>
       <c r="D322" s="8"/>
     </row>
-    <row r="323" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="323" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B323" s="2"/>
       <c r="C323" s="2"/>
       <c r="D323" s="8"/>
     </row>
-    <row r="324" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B324" s="2"/>
       <c r="C324" s="2"/>
       <c r="D324" s="8"/>
     </row>
-    <row r="325" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B325" s="2"/>
       <c r="C325" s="2"/>
       <c r="D325" s="8"/>
     </row>
-    <row r="326" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="326" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B326" s="2"/>
       <c r="C326" s="2"/>
       <c r="D326" s="8"/>
     </row>
-    <row r="327" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="327" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B327" s="2"/>
       <c r="C327" s="2"/>
       <c r="D327" s="8"/>
     </row>
-    <row r="328" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="328" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B328" s="2"/>
       <c r="C328" s="2"/>
       <c r="D328" s="8"/>
     </row>
-    <row r="329" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="329" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B329" s="2"/>
       <c r="C329" s="2"/>
       <c r="D329" s="8"/>
     </row>
-    <row r="330" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="330" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B330" s="2"/>
       <c r="C330" s="2"/>
       <c r="D330" s="8"/>
     </row>
-    <row r="331" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="331" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B331" s="2"/>
       <c r="C331" s="2"/>
       <c r="D331" s="8"/>
     </row>
-    <row r="332" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="332" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B332" s="2"/>
       <c r="C332" s="2"/>
       <c r="D332" s="8"/>
     </row>
-    <row r="333" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="333" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B333" s="2"/>
       <c r="C333" s="2"/>
       <c r="D333" s="8"/>
     </row>
-    <row r="334" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="334" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B334" s="2"/>
       <c r="C334" s="2"/>
       <c r="D334" s="8"/>
     </row>
-    <row r="335" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="335" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B335" s="2"/>
       <c r="C335" s="2"/>
       <c r="D335" s="8"/>
     </row>
-    <row r="336" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="336" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B336" s="2"/>
       <c r="C336" s="2"/>
       <c r="D336" s="8"/>
     </row>
-    <row r="337" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="337" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B337" s="2"/>
       <c r="C337" s="2"/>
       <c r="D337" s="8"/>
     </row>
-    <row r="338" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="338" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B338" s="2"/>
       <c r="C338" s="2"/>
       <c r="D338" s="8"/>
     </row>
-    <row r="339" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="339" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B339" s="2"/>
       <c r="C339" s="2"/>
       <c r="D339" s="8"/>
     </row>
-    <row r="340" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="340" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B340" s="2"/>
       <c r="C340" s="2"/>
       <c r="D340" s="8"/>
     </row>
-    <row r="341" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="341" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B341" s="2"/>
       <c r="C341" s="2"/>
       <c r="D341" s="8"/>
     </row>
-    <row r="342" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="342" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B342" s="2"/>
       <c r="C342" s="2"/>
       <c r="D342" s="8"/>
     </row>
-    <row r="343" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="343" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B343" s="2"/>
       <c r="C343" s="2"/>
       <c r="D343" s="8"/>
     </row>
-    <row r="344" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="344" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B344" s="2"/>
       <c r="C344" s="2"/>
       <c r="D344" s="8"/>
     </row>
-    <row r="345" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="345" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B345" s="2"/>
       <c r="C345" s="2"/>
       <c r="D345" s="8"/>
     </row>
-    <row r="346" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="346" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B346" s="2"/>
       <c r="C346" s="2"/>
       <c r="D346" s="8"/>
     </row>
-    <row r="347" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="347" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B347" s="2"/>
       <c r="C347" s="2"/>
       <c r="D347" s="8"/>
     </row>
-    <row r="348" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="348" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B348" s="2"/>
       <c r="C348" s="2"/>
       <c r="D348" s="8"/>
     </row>
-    <row r="349" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="349" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B349" s="2"/>
       <c r="C349" s="2"/>
       <c r="D349" s="8"/>
     </row>
-    <row r="350" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="350" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B350" s="2"/>
       <c r="C350" s="2"/>
       <c r="D350" s="8"/>
     </row>
-    <row r="351" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="351" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B351" s="2"/>
       <c r="C351" s="2"/>
       <c r="D351" s="8"/>
     </row>
-    <row r="352" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="352" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B352" s="2"/>
       <c r="C352" s="2"/>
       <c r="D352" s="8"/>
     </row>
-    <row r="353" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="353" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B353" s="2"/>
       <c r="C353" s="2"/>
       <c r="D353" s="8"/>
     </row>
-    <row r="354" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="354" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B354" s="2"/>
       <c r="C354" s="2"/>
       <c r="D354" s="8"/>
     </row>
-    <row r="355" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="355" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B355" s="2"/>
       <c r="C355" s="2"/>
       <c r="D355" s="8"/>
     </row>
-    <row r="356" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="356" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B356" s="2"/>
       <c r="C356" s="2"/>
       <c r="D356" s="8"/>
     </row>
-    <row r="357" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="357" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B357" s="2"/>
       <c r="C357" s="2"/>
       <c r="D357" s="8"/>
     </row>
-    <row r="358" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="358" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B358" s="2"/>
       <c r="C358" s="2"/>
       <c r="D358" s="8"/>
     </row>
-    <row r="359" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="359" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B359" s="2"/>
       <c r="C359" s="2"/>
       <c r="D359" s="8"/>
     </row>
-    <row r="360" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="360" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B360" s="2"/>
       <c r="C360" s="2"/>
       <c r="D360" s="8"/>
     </row>
-    <row r="361" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="361" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B361" s="2"/>
       <c r="C361" s="2"/>
       <c r="D361" s="8"/>
     </row>
-    <row r="362" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="362" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B362" s="2"/>
       <c r="C362" s="2"/>
       <c r="D362" s="8"/>
     </row>
-    <row r="363" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="363" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B363" s="2"/>
       <c r="C363" s="2"/>
       <c r="D363" s="8"/>
     </row>
-    <row r="364" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="364" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B364" s="2"/>
       <c r="C364" s="2"/>
       <c r="D364" s="8"/>
     </row>
-    <row r="365" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="365" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B365" s="2"/>
       <c r="C365" s="2"/>
       <c r="D365" s="8"/>
     </row>
-    <row r="366" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="366" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B366" s="2"/>
       <c r="C366" s="2"/>
       <c r="D366" s="8"/>
     </row>
-    <row r="367" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="367" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B367" s="2"/>
       <c r="C367" s="2"/>
       <c r="D367" s="8"/>
     </row>
-    <row r="368" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="368" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B368" s="2"/>
       <c r="C368" s="2"/>
       <c r="D368" s="8"/>
     </row>
-    <row r="369" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="369" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B369" s="2"/>
       <c r="C369" s="2"/>
       <c r="D369" s="8"/>
     </row>
-    <row r="370" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="370" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B370" s="2"/>
       <c r="C370" s="2"/>
       <c r="D370" s="8"/>
     </row>
-    <row r="371" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="371" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B371" s="2"/>
       <c r="C371" s="2"/>
       <c r="D371" s="8"/>
     </row>
-    <row r="372" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="372" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B372" s="2"/>
       <c r="C372" s="2"/>
       <c r="D372" s="8"/>
     </row>
-    <row r="373" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="373" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B373" s="2"/>
       <c r="C373" s="2"/>
       <c r="D373" s="8"/>
     </row>
-    <row r="374" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="374" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B374" s="2"/>
       <c r="C374" s="2"/>
       <c r="D374" s="8"/>
     </row>
-    <row r="375" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="375" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B375" s="2"/>
       <c r="C375" s="2"/>
       <c r="D375" s="8"/>
     </row>
-    <row r="376" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="376" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B376" s="2"/>
       <c r="C376" s="2"/>
       <c r="D376" s="8"/>
     </row>
-    <row r="377" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="377" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B377" s="2"/>
       <c r="C377" s="2"/>
       <c r="D377" s="8"/>
     </row>
-    <row r="378" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="378" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B378" s="2"/>
       <c r="C378" s="2"/>
       <c r="D378" s="8"/>
     </row>
-    <row r="379" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="379" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B379" s="2"/>
       <c r="C379" s="2"/>
       <c r="D379" s="8"/>
     </row>
-    <row r="380" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="380" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B380" s="2"/>
       <c r="C380" s="2"/>
       <c r="D380" s="8"/>
     </row>
-    <row r="381" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="381" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B381" s="2"/>
       <c r="C381" s="2"/>
       <c r="D381" s="8"/>
     </row>
-    <row r="382" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="382" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B382" s="2"/>
       <c r="C382" s="2"/>
       <c r="D382" s="8"/>
     </row>
-    <row r="383" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="383" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B383" s="2"/>
       <c r="C383" s="2"/>
       <c r="D383" s="8"/>
     </row>
-    <row r="384" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="384" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B384" s="2"/>
       <c r="C384" s="2"/>
       <c r="D384" s="8"/>
     </row>
-    <row r="385" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="385" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B385" s="2"/>
       <c r="C385" s="2"/>
       <c r="D385" s="8"/>
     </row>
-    <row r="386" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="386" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B386" s="2"/>
       <c r="C386" s="2"/>
       <c r="D386" s="8"/>
     </row>
-    <row r="387" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="387" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B387" s="2"/>
       <c r="C387" s="2"/>
       <c r="D387" s="8"/>
     </row>
-    <row r="388" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="388" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B388" s="2"/>
       <c r="C388" s="2"/>
       <c r="D388" s="8"/>
     </row>
-    <row r="389" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="389" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B389" s="2"/>
       <c r="C389" s="2"/>
       <c r="D389" s="8"/>
     </row>
-    <row r="390" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="390" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B390" s="2"/>
       <c r="C390" s="2"/>
       <c r="D390" s="8"/>
     </row>
-    <row r="391" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="391" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B391" s="2"/>
       <c r="C391" s="2"/>
       <c r="D391" s="8"/>
     </row>
-    <row r="392" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="392" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B392" s="2"/>
       <c r="C392" s="2"/>
       <c r="D392" s="8"/>
     </row>
-    <row r="393" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="393" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B393" s="2"/>
       <c r="C393" s="2"/>
       <c r="D393" s="8"/>
     </row>
-    <row r="394" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="394" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B394" s="2"/>
       <c r="C394" s="2"/>
       <c r="D394" s="8"/>
     </row>
-    <row r="395" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="395" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B395" s="2"/>
       <c r="C395" s="2"/>
       <c r="D395" s="8"/>
     </row>
-    <row r="396" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="396" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B396" s="2"/>
       <c r="C396" s="2"/>
       <c r="D396" s="8"/>
     </row>
-    <row r="397" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="397" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B397" s="2"/>
       <c r="C397" s="2"/>
       <c r="D397" s="8"/>
     </row>
-    <row r="398" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="398" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B398" s="2"/>
       <c r="C398" s="2"/>
       <c r="D398" s="8"/>
     </row>
-    <row r="399" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="399" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B399" s="2"/>
       <c r="C399" s="2"/>
       <c r="D399" s="8"/>
     </row>
-    <row r="400" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="400" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B400" s="2"/>
       <c r="C400" s="2"/>
       <c r="D400" s="8"/>
     </row>
-    <row r="401" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="401" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B401" s="2"/>
       <c r="C401" s="2"/>
       <c r="D401" s="8"/>
     </row>
-    <row r="402" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="402" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B402" s="2"/>
       <c r="C402" s="2"/>
       <c r="D402" s="8"/>
     </row>
-    <row r="403" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="403" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B403" s="2"/>
       <c r="C403" s="2"/>
       <c r="D403" s="8"/>
     </row>
-    <row r="404" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="404" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D404" s="8"/>
     </row>
-    <row r="405" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="405" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D405" s="8"/>
     </row>
-    <row r="406" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="406" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D406" s="8"/>
     </row>
-    <row r="407" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="407" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D407" s="8"/>
     </row>
-    <row r="408" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="408" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D408" s="8"/>
     </row>
-    <row r="409" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="409" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D409" s="8"/>
     </row>
-    <row r="410" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="410" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D410" s="8"/>
     </row>
-    <row r="411" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="411" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D411" s="8"/>
     </row>
-    <row r="412" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="412" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D412" s="8"/>
     </row>
-    <row r="413" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="413" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D413" s="8"/>
     </row>
-    <row r="414" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="414" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D414" s="8"/>
     </row>
-    <row r="415" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="415" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D415" s="8"/>
     </row>
-    <row r="416" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="416" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D416" s="8"/>
     </row>
-    <row r="417" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="417" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D417" s="8"/>
     </row>
-    <row r="418" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="418" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D418" s="8"/>
     </row>
-    <row r="419" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="419" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D419" s="8"/>
     </row>
-    <row r="420" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="420" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D420" s="8"/>
     </row>
-    <row r="421" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="421" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D421" s="8"/>
     </row>
-    <row r="422" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="422" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D422" s="8"/>
     </row>
-    <row r="423" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="423" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D423" s="8"/>
     </row>
-    <row r="424" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="424" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D424" s="8"/>
     </row>
-    <row r="425" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="425" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D425" s="8"/>
     </row>
-    <row r="426" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="426" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D426" s="8"/>
     </row>
-    <row r="427" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="427" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D427" s="8"/>
     </row>
-    <row r="428" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="428" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D428" s="8"/>
     </row>
-    <row r="429" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="429" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D429" s="8"/>
     </row>
-    <row r="430" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="430" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D430" s="8"/>
     </row>
-    <row r="431" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="431" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D431" s="8"/>
     </row>
-    <row r="432" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="432" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D432" s="8"/>
     </row>
-    <row r="433" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="433" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D433" s="8"/>
     </row>
-    <row r="434" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="434" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D434" s="8"/>
     </row>
-    <row r="435" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="435" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D435" s="8"/>
     </row>
-    <row r="436" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="436" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D436" s="8"/>
     </row>
-    <row r="437" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="437" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D437" s="8"/>
     </row>
-    <row r="438" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="438" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D438" s="8"/>
     </row>
-    <row r="439" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="439" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D439" s="8"/>
     </row>
-    <row r="440" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="440" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D440" s="8"/>
     </row>
-    <row r="441" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="441" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D441" s="8"/>
     </row>
-    <row r="442" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="442" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D442" s="8"/>
     </row>
-    <row r="443" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="443" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D443" s="8"/>
     </row>
-    <row r="444" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="444" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D444" s="8"/>
     </row>
-    <row r="445" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="445" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D445" s="8"/>
     </row>
-    <row r="446" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="446" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D446" s="8"/>
     </row>
-    <row r="447" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="447" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D447" s="8"/>
     </row>
-    <row r="448" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="448" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D448" s="8"/>
     </row>
-    <row r="449" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="449" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D449" s="8"/>
     </row>
-    <row r="450" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="450" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D450" s="8"/>
     </row>
-    <row r="451" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="451" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D451" s="8"/>
     </row>
-    <row r="452" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="452" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D452" s="8"/>
     </row>
-    <row r="453" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="453" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D453" s="8"/>
     </row>
-    <row r="454" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="454" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D454" s="8"/>
     </row>
-    <row r="455" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="455" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D455" s="8"/>
     </row>
-    <row r="456" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="456" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D456" s="8"/>
     </row>
-    <row r="457" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="457" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D457" s="8"/>
     </row>
-    <row r="458" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="458" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D458" s="8"/>
     </row>
-    <row r="459" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="459" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D459" s="8"/>
     </row>
-    <row r="460" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="460" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D460" s="8"/>
     </row>
-    <row r="461" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="461" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D461" s="8"/>
     </row>
-    <row r="462" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="462" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D462" s="8"/>
     </row>
-    <row r="463" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="463" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D463" s="8"/>
     </row>
-    <row r="464" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="464" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D464" s="8"/>
     </row>
-    <row r="465" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="465" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D465" s="8"/>
     </row>
-    <row r="466" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="466" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D466" s="8"/>
     </row>
-    <row r="467" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="467" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D467" s="8"/>
     </row>
-    <row r="468" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="468" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D468" s="8"/>
     </row>
-    <row r="469" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="469" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D469" s="8"/>
     </row>
-    <row r="470" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="470" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D470" s="8"/>
     </row>
-    <row r="471" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="471" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D471" s="8"/>
     </row>
-    <row r="472" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="472" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D472" s="8"/>
     </row>
-    <row r="473" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="473" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D473" s="8"/>
     </row>
-    <row r="474" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="474" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D474" s="8"/>
     </row>
-    <row r="475" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="475" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D475" s="8"/>
     </row>
-    <row r="476" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="476" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D476" s="8"/>
     </row>
-    <row r="477" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="477" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D477" s="8"/>
     </row>
-    <row r="478" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="478" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D478" s="8"/>
     </row>
-    <row r="479" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="479" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D479" s="8"/>
     </row>
-    <row r="480" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="480" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D480" s="8"/>
     </row>
-    <row r="481" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="481" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D481" s="8"/>
     </row>
-    <row r="482" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="482" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D482" s="8"/>
     </row>
-    <row r="483" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="483" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D483" s="8"/>
     </row>
-    <row r="484" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="484" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D484" s="8"/>
     </row>
-    <row r="485" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="485" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D485" s="8"/>
     </row>
-    <row r="486" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="486" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D486" s="8"/>
     </row>
-    <row r="487" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="487" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D487" s="8"/>
     </row>
-    <row r="488" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="488" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D488" s="8"/>
     </row>
-    <row r="489" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="489" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D489" s="8"/>
     </row>
-    <row r="490" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="490" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D490" s="8"/>
     </row>
-    <row r="491" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="491" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D491" s="8"/>
     </row>
-    <row r="492" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="492" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D492" s="8"/>
     </row>
-    <row r="493" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="493" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D493" s="8"/>
     </row>
-    <row r="494" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="494" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D494" s="8"/>
     </row>
-    <row r="495" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="495" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D495" s="8"/>
     </row>
-    <row r="496" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="496" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D496" s="8"/>
     </row>
-    <row r="497" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="497" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D497" s="8"/>
     </row>
-    <row r="498" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="498" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D498" s="8"/>
     </row>
-    <row r="499" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="499" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D499" s="8"/>
     </row>
-    <row r="500" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="500" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D500" s="8"/>
     </row>
-    <row r="501" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="501" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D501" s="8"/>
     </row>
-    <row r="502" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="502" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D502" s="8"/>
     </row>
-    <row r="503" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="503" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D503" s="8"/>
     </row>
-    <row r="504" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="504" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D504" s="8"/>
     </row>
-    <row r="505" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="505" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D505" s="8"/>
     </row>
-    <row r="506" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="506" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D506" s="8"/>
     </row>
-    <row r="507" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="507" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D507" s="8"/>
     </row>
-    <row r="508" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="508" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D508" s="8"/>
     </row>
-    <row r="509" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="509" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D509" s="8"/>
     </row>
-    <row r="510" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="510" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D510" s="8"/>
     </row>
-    <row r="511" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="511" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D511" s="8"/>
     </row>
-    <row r="512" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="512" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D512" s="8"/>
     </row>
-    <row r="513" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="513" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D513" s="8"/>
     </row>
-    <row r="514" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="514" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D514" s="8"/>
     </row>
-    <row r="515" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="515" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D515" s="8"/>
     </row>
-    <row r="516" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="516" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D516" s="8"/>
     </row>
-    <row r="517" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="517" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D517" s="8"/>
     </row>
-    <row r="518" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="518" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D518" s="8"/>
     </row>
-    <row r="519" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="519" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D519" s="8"/>
     </row>
-    <row r="520" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="520" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D520" s="8"/>
     </row>
-    <row r="521" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="521" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D521" s="8"/>
     </row>
-    <row r="522" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="522" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D522" s="8"/>
     </row>
-    <row r="523" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="523" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D523" s="8"/>
     </row>
-    <row r="524" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="524" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D524" s="8"/>
     </row>
-    <row r="525" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="525" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D525" s="8"/>
     </row>
-    <row r="526" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="526" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D526" s="8"/>
     </row>
-    <row r="527" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="527" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D527" s="8"/>
     </row>
-    <row r="528" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="528" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D528" s="8"/>
     </row>
-    <row r="529" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="529" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D529" s="8"/>
     </row>
-    <row r="530" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="530" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D530" s="8"/>
     </row>
-    <row r="531" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="531" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D531" s="8"/>
     </row>
-    <row r="532" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="532" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D532" s="8"/>
     </row>
-    <row r="533" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="533" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D533" s="8"/>
     </row>
-    <row r="534" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="534" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D534" s="8"/>
     </row>
-    <row r="535" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="535" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D535" s="8"/>
     </row>
-    <row r="536" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="536" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D536" s="8"/>
     </row>
-    <row r="537" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="537" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D537" s="8"/>
     </row>
-    <row r="538" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="538" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D538" s="8"/>
     </row>
-    <row r="539" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="539" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D539" s="8"/>
     </row>
-    <row r="540" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="540" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D540" s="8"/>
     </row>
-    <row r="541" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="541" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D541" s="8"/>
     </row>
-    <row r="542" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="542" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D542" s="8"/>
     </row>
-    <row r="543" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="543" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D543" s="8"/>
     </row>
-    <row r="544" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="544" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D544" s="8"/>
     </row>
-    <row r="545" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="545" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D545" s="8"/>
     </row>
-    <row r="546" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="546" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D546" s="8"/>
     </row>
-    <row r="547" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="547" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D547" s="8"/>
     </row>
-    <row r="548" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="548" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D548" s="8"/>
     </row>
-    <row r="549" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="549" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D549" s="8"/>
     </row>
-    <row r="550" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="550" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D550" s="8"/>
     </row>
-    <row r="551" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="551" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D551" s="8"/>
     </row>
-    <row r="552" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="552" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D552" s="8"/>
     </row>
-    <row r="553" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="553" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D553" s="8"/>
     </row>
-    <row r="554" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="554" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D554" s="8"/>
     </row>
-    <row r="555" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="555" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D555" s="8"/>
     </row>
-    <row r="556" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="556" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D556" s="8"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="E19:E27"/>
   </mergeCells>

</xml_diff>

<commit_message>
deactivated empty shipping instructions card
</commit_message>
<xml_diff>
--- a/public/template/shipping_instruction_template.xlsx
+++ b/public/template/shipping_instruction_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syedazlan/MyLaravelProjects/gus/public/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\MyLaravelApps\gus-automate\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A642CF-7A1C-C44E-BDDA-7F19A915C6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2F77B8-D023-4838-9644-411FF560B3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" xr2:uid="{378D42B6-8EFA-4EF6-9C50-436D539EEED8}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{378D42B6-8EFA-4EF6-9C50-436D539EEED8}"/>
   </bookViews>
   <sheets>
     <sheet name="BillOfLading" sheetId="1" r:id="rId1"/>
@@ -34,25 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
-  <si>
-    <t>METAL SCRAP</t>
-  </si>
-  <si>
-    <t>SEAL001</t>
-  </si>
-  <si>
-    <t>SEAL002</t>
-  </si>
-  <si>
-    <t>SEAL003</t>
-  </si>
-  <si>
-    <t>SEAL004</t>
-  </si>
-  <si>
-    <t>SEAL005</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>BOX OPERATOR</t>
   </si>
@@ -102,78 +84,6 @@
     <t>NOTIFY PARTY CONTACT</t>
   </si>
   <si>
-    <t>PETRONAS CHEMICAL</t>
-  </si>
-  <si>
-    <t>PETRONAS CHEMICALS MARKETING (LABUAN) LTD</t>
-  </si>
-  <si>
-    <t>LEVEL 34, TOWER 1, PETRONAS TWIN TOWERS,</t>
-  </si>
-  <si>
-    <t>KUALA LUMPUR CITY CENTRE, 50088 KUALA LUMPUR,</t>
-  </si>
-  <si>
-    <t>MALAYSIA</t>
-  </si>
-  <si>
-    <t>0331693303</t>
-  </si>
-  <si>
-    <t>FGV TRANSPORT SERVICES SDN. BHD.</t>
-  </si>
-  <si>
-    <t>LEVEL 6 EAST, WISMA FGV,</t>
-  </si>
-  <si>
-    <t>JALAN RAJA LAUT,</t>
-  </si>
-  <si>
-    <t>50350 KUALA LUMPUR,</t>
-  </si>
-  <si>
-    <t>SEAL006</t>
-  </si>
-  <si>
-    <t>SEAL007</t>
-  </si>
-  <si>
-    <t>SEAL008</t>
-  </si>
-  <si>
-    <t>SEAL009</t>
-  </si>
-  <si>
-    <t>TEMU1172101</t>
-  </si>
-  <si>
-    <t>TEMU1172102</t>
-  </si>
-  <si>
-    <t>TEMU1172103</t>
-  </si>
-  <si>
-    <t>TEMU1172104</t>
-  </si>
-  <si>
-    <t>TEMU1172105</t>
-  </si>
-  <si>
-    <t>TEMU1172106</t>
-  </si>
-  <si>
-    <t>TEMU1172107</t>
-  </si>
-  <si>
-    <t>TEMU1172108</t>
-  </si>
-  <si>
-    <t>TEMU1172109</t>
-  </si>
-  <si>
-    <t>40HC</t>
-  </si>
-  <si>
     <t>EVERGREEN</t>
   </si>
   <si>
@@ -185,7 +95,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -285,7 +195,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -391,8 +301,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7102474" y="209550"/>
-          <a:ext cx="5394326" cy="1581150"/>
+          <a:off x="6518274" y="203200"/>
+          <a:ext cx="5013326" cy="1530350"/>
           <a:chOff x="6029324" y="276225"/>
           <a:chExt cx="4238625" cy="1390650"/>
         </a:xfrm>
@@ -673,9 +583,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -713,7 +623,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -819,7 +729,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -961,7 +871,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -972,2630 +882,2532 @@
   <dimension ref="B2:H556"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="53.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.6328125" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="3" width="53.36328125" customWidth="1"/>
     <col min="4" max="4" width="14" style="6" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
-    <col min="6" max="6" width="33.5" customWidth="1"/>
-    <col min="7" max="7" width="23.5" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.1796875" customWidth="1"/>
+    <col min="6" max="6" width="33.453125" customWidth="1"/>
+    <col min="7" max="7" width="23.453125" customWidth="1"/>
+    <col min="8" max="8" width="21.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="14"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C9" s="12"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="E11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="E12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="E13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>46</v>
+      <c r="F13" s="12"/>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="15"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="B18" s="5" t="s">
+        <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+      <c r="C18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C7" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C8" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C9" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="15"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="15"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C14" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="15"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C15" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="15"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C16" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="15"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B19" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F19" s="9">
-        <v>837800</v>
-      </c>
-      <c r="G19" s="11">
-        <v>3000</v>
-      </c>
-      <c r="H19" s="11">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B20" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>45</v>
-      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="18"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B21" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>45</v>
-      </c>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="18"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B22" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>45</v>
-      </c>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="18"/>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B23" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>45</v>
-      </c>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="18"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B24" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>45</v>
-      </c>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="10"/>
       <c r="E24" s="18"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B25" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>45</v>
-      </c>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="10"/>
       <c r="E25" s="18"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B26" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>45</v>
-      </c>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
       <c r="E26" s="18"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B27" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>45</v>
-      </c>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="10"/>
       <c r="E27" s="18"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="10"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="10"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
       <c r="D41" s="10"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
       <c r="D42" s="10"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="10"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="10"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
       <c r="D46" s="10"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
       <c r="D47" s="10"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="10"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
       <c r="D49" s="10"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
       <c r="D51" s="10"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
       <c r="D52" s="10"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
       <c r="D53" s="10"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
       <c r="D54" s="10"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="10"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="10"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="10"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="10"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
       <c r="D61" s="10"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
       <c r="D63" s="10"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
       <c r="D64" s="10"/>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
       <c r="D65" s="10"/>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
       <c r="D66" s="10"/>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
       <c r="D67" s="10"/>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
       <c r="D68" s="10"/>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
       <c r="D69" s="10"/>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
       <c r="D70" s="10"/>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
       <c r="D71" s="10"/>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
       <c r="D72" s="10"/>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
       <c r="D73" s="10"/>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
       <c r="D74" s="10"/>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
       <c r="D75" s="10"/>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
       <c r="D76" s="10"/>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
       <c r="D77" s="10"/>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
       <c r="D78" s="10"/>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
       <c r="D79" s="10"/>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
       <c r="D80" s="10"/>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
       <c r="D81" s="10"/>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
       <c r="D82" s="10"/>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
       <c r="D83" s="10"/>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
       <c r="D84" s="10"/>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
       <c r="D85" s="10"/>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
       <c r="D86" s="10"/>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
       <c r="D87" s="10"/>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
       <c r="D88" s="10"/>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
       <c r="D89" s="10"/>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
       <c r="D90" s="10"/>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
       <c r="D91" s="10"/>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
       <c r="D92" s="10"/>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
       <c r="D93" s="10"/>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
       <c r="D94" s="10"/>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
       <c r="D95" s="10"/>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
       <c r="D96" s="10"/>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
       <c r="D97" s="10"/>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
       <c r="D98" s="10"/>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
       <c r="D99" s="10"/>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
       <c r="D101" s="10"/>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
       <c r="D102" s="10"/>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
       <c r="D103" s="10"/>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
       <c r="D104" s="10"/>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
       <c r="D105" s="10"/>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B106" s="9"/>
       <c r="C106" s="9"/>
       <c r="D106" s="10"/>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
       <c r="D107" s="10"/>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B108" s="9"/>
       <c r="C108" s="9"/>
       <c r="D108" s="10"/>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B109" s="9"/>
       <c r="C109" s="9"/>
       <c r="D109" s="10"/>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B110" s="9"/>
       <c r="C110" s="9"/>
       <c r="D110" s="10"/>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
       <c r="D111" s="10"/>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B112" s="9"/>
       <c r="C112" s="9"/>
       <c r="D112" s="10"/>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
       <c r="D113" s="10"/>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B114" s="9"/>
       <c r="C114" s="9"/>
       <c r="D114" s="10"/>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B115" s="9"/>
       <c r="C115" s="9"/>
       <c r="D115" s="10"/>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B116" s="9"/>
       <c r="C116" s="9"/>
       <c r="D116" s="10"/>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B117" s="9"/>
       <c r="C117" s="9"/>
       <c r="D117" s="10"/>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B118" s="9"/>
       <c r="C118" s="9"/>
       <c r="D118" s="10"/>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B119" s="9"/>
       <c r="C119" s="9"/>
       <c r="D119" s="10"/>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B120" s="9"/>
       <c r="C120" s="9"/>
       <c r="D120" s="10"/>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B121" s="9"/>
       <c r="C121" s="9"/>
       <c r="D121" s="10"/>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B122" s="9"/>
       <c r="C122" s="9"/>
       <c r="D122" s="10"/>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B123" s="9"/>
       <c r="C123" s="9"/>
       <c r="D123" s="10"/>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B124" s="9"/>
       <c r="C124" s="9"/>
       <c r="D124" s="10"/>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B125" s="9"/>
       <c r="C125" s="9"/>
       <c r="D125" s="10"/>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B126" s="9"/>
       <c r="C126" s="9"/>
       <c r="D126" s="10"/>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B127" s="9"/>
       <c r="C127" s="9"/>
       <c r="D127" s="10"/>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B128" s="9"/>
       <c r="C128" s="9"/>
       <c r="D128" s="10"/>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B129" s="9"/>
       <c r="C129" s="9"/>
       <c r="D129" s="10"/>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B130" s="9"/>
       <c r="C130" s="9"/>
       <c r="D130" s="10"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B131" s="9"/>
       <c r="C131" s="9"/>
       <c r="D131" s="10"/>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B132" s="9"/>
       <c r="C132" s="9"/>
       <c r="D132" s="10"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B133" s="9"/>
       <c r="C133" s="9"/>
       <c r="D133" s="10"/>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B134" s="9"/>
       <c r="C134" s="9"/>
       <c r="D134" s="10"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B135" s="9"/>
       <c r="C135" s="9"/>
       <c r="D135" s="10"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B136" s="9"/>
       <c r="C136" s="9"/>
       <c r="D136" s="10"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B137" s="9"/>
       <c r="C137" s="9"/>
       <c r="D137" s="10"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B138" s="9"/>
       <c r="C138" s="9"/>
       <c r="D138" s="10"/>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B139" s="9"/>
       <c r="C139" s="9"/>
       <c r="D139" s="10"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B140" s="9"/>
       <c r="C140" s="9"/>
       <c r="D140" s="10"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B141" s="9"/>
       <c r="C141" s="9"/>
       <c r="D141" s="10"/>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B142" s="9"/>
       <c r="C142" s="9"/>
       <c r="D142" s="10"/>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B143" s="9"/>
       <c r="C143" s="9"/>
       <c r="D143" s="10"/>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B144" s="9"/>
       <c r="C144" s="9"/>
       <c r="D144" s="10"/>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B145" s="9"/>
       <c r="C145" s="9"/>
       <c r="D145" s="10"/>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B146" s="9"/>
       <c r="C146" s="9"/>
       <c r="D146" s="10"/>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B147" s="9"/>
       <c r="C147" s="9"/>
       <c r="D147" s="10"/>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B148" s="9"/>
       <c r="C148" s="9"/>
       <c r="D148" s="10"/>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B149" s="9"/>
       <c r="C149" s="9"/>
       <c r="D149" s="10"/>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B150" s="9"/>
       <c r="C150" s="9"/>
       <c r="D150" s="10"/>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B151" s="9"/>
       <c r="C151" s="9"/>
       <c r="D151" s="10"/>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B152" s="9"/>
       <c r="C152" s="9"/>
       <c r="D152" s="10"/>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B153" s="9"/>
       <c r="C153" s="9"/>
       <c r="D153" s="10"/>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B154" s="9"/>
       <c r="C154" s="9"/>
       <c r="D154" s="10"/>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B155" s="9"/>
       <c r="C155" s="9"/>
       <c r="D155" s="10"/>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B156" s="9"/>
       <c r="C156" s="9"/>
       <c r="D156" s="10"/>
     </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B157" s="9"/>
       <c r="C157" s="9"/>
       <c r="D157" s="10"/>
     </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B158" s="9"/>
       <c r="C158" s="9"/>
       <c r="D158" s="10"/>
     </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B159" s="9"/>
       <c r="C159" s="9"/>
       <c r="D159" s="10"/>
     </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B160" s="9"/>
       <c r="C160" s="9"/>
       <c r="D160" s="10"/>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B161" s="9"/>
       <c r="C161" s="9"/>
       <c r="D161" s="10"/>
     </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B162" s="9"/>
       <c r="C162" s="9"/>
       <c r="D162" s="10"/>
     </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B163" s="9"/>
       <c r="C163" s="9"/>
       <c r="D163" s="10"/>
     </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B164" s="9"/>
       <c r="C164" s="9"/>
       <c r="D164" s="10"/>
     </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B165" s="9"/>
       <c r="C165" s="9"/>
       <c r="D165" s="10"/>
     </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B166" s="9"/>
       <c r="C166" s="9"/>
       <c r="D166" s="10"/>
     </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B167" s="9"/>
       <c r="C167" s="9"/>
       <c r="D167" s="10"/>
     </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B168" s="9"/>
       <c r="C168" s="9"/>
       <c r="D168" s="10"/>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B169" s="9"/>
       <c r="C169" s="9"/>
       <c r="D169" s="10"/>
     </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B170" s="9"/>
       <c r="C170" s="9"/>
       <c r="D170" s="10"/>
     </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B171" s="9"/>
       <c r="C171" s="9"/>
       <c r="D171" s="10"/>
     </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B172" s="9"/>
       <c r="C172" s="9"/>
       <c r="D172" s="10"/>
     </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B173" s="9"/>
       <c r="C173" s="9"/>
       <c r="D173" s="10"/>
     </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B174" s="9"/>
       <c r="C174" s="9"/>
       <c r="D174" s="10"/>
     </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B175" s="9"/>
       <c r="C175" s="9"/>
       <c r="D175" s="10"/>
     </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B176" s="9"/>
       <c r="C176" s="9"/>
       <c r="D176" s="10"/>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B177" s="9"/>
       <c r="C177" s="9"/>
       <c r="D177" s="10"/>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B178" s="9"/>
       <c r="C178" s="9"/>
       <c r="D178" s="10"/>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B179" s="9"/>
       <c r="C179" s="9"/>
       <c r="D179" s="10"/>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B180" s="9"/>
       <c r="C180" s="9"/>
       <c r="D180" s="10"/>
     </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B181" s="9"/>
       <c r="C181" s="9"/>
       <c r="D181" s="10"/>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B182" s="9"/>
       <c r="C182" s="9"/>
       <c r="D182" s="10"/>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B183" s="9"/>
       <c r="C183" s="9"/>
       <c r="D183" s="10"/>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B184" s="9"/>
       <c r="C184" s="9"/>
       <c r="D184" s="10"/>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B185" s="9"/>
       <c r="C185" s="9"/>
       <c r="D185" s="10"/>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B186" s="9"/>
       <c r="C186" s="9"/>
       <c r="D186" s="10"/>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B187" s="9"/>
       <c r="C187" s="9"/>
       <c r="D187" s="10"/>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B188" s="9"/>
       <c r="C188" s="9"/>
       <c r="D188" s="10"/>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B189" s="9"/>
       <c r="C189" s="9"/>
       <c r="D189" s="10"/>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B190" s="9"/>
       <c r="C190" s="9"/>
       <c r="D190" s="10"/>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B191" s="9"/>
       <c r="C191" s="9"/>
       <c r="D191" s="10"/>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B192" s="9"/>
       <c r="C192" s="9"/>
       <c r="D192" s="10"/>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B193" s="9"/>
       <c r="C193" s="9"/>
       <c r="D193" s="10"/>
     </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B194" s="9"/>
       <c r="C194" s="9"/>
       <c r="D194" s="10"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B195" s="9"/>
       <c r="C195" s="9"/>
       <c r="D195" s="10"/>
     </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B196" s="9"/>
       <c r="C196" s="9"/>
       <c r="D196" s="10"/>
     </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B197" s="9"/>
       <c r="C197" s="9"/>
       <c r="D197" s="10"/>
     </row>
-    <row r="198" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B198" s="9"/>
       <c r="C198" s="9"/>
       <c r="D198" s="10"/>
     </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B199" s="9"/>
       <c r="C199" s="9"/>
       <c r="D199" s="10"/>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B200" s="9"/>
       <c r="C200" s="9"/>
       <c r="D200" s="10"/>
     </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B201" s="9"/>
       <c r="C201" s="9"/>
       <c r="D201" s="10"/>
     </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B202" s="9"/>
       <c r="C202" s="9"/>
       <c r="D202" s="10"/>
     </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
       <c r="D203" s="8"/>
     </row>
-    <row r="204" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
       <c r="D204" s="8"/>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
       <c r="D205" s="8"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
       <c r="D206" s="8"/>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
       <c r="D207" s="8"/>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
       <c r="D208" s="8"/>
     </row>
-    <row r="209" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
       <c r="D209" s="8"/>
     </row>
-    <row r="210" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
       <c r="D210" s="8"/>
     </row>
-    <row r="211" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
       <c r="D211" s="8"/>
     </row>
-    <row r="212" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
       <c r="D212" s="8"/>
     </row>
-    <row r="213" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
       <c r="D213" s="8"/>
     </row>
-    <row r="214" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
       <c r="D214" s="8"/>
     </row>
-    <row r="215" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
       <c r="D215" s="8"/>
     </row>
-    <row r="216" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
       <c r="D216" s="8"/>
     </row>
-    <row r="217" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
       <c r="D217" s="8"/>
     </row>
-    <row r="218" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
       <c r="D218" s="8"/>
     </row>
-    <row r="219" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
       <c r="D219" s="8"/>
     </row>
-    <row r="220" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
       <c r="D220" s="8"/>
     </row>
-    <row r="221" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
       <c r="D221" s="8"/>
     </row>
-    <row r="222" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
       <c r="D222" s="8"/>
     </row>
-    <row r="223" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B223" s="2"/>
       <c r="C223" s="2"/>
       <c r="D223" s="8"/>
     </row>
-    <row r="224" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
       <c r="D224" s="8"/>
     </row>
-    <row r="225" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B225" s="2"/>
       <c r="C225" s="2"/>
       <c r="D225" s="8"/>
     </row>
-    <row r="226" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
       <c r="D226" s="8"/>
     </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
       <c r="D227" s="8"/>
     </row>
-    <row r="228" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
       <c r="D228" s="8"/>
     </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B229" s="2"/>
       <c r="C229" s="2"/>
       <c r="D229" s="8"/>
     </row>
-    <row r="230" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
       <c r="D230" s="8"/>
     </row>
-    <row r="231" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
       <c r="D231" s="8"/>
     </row>
-    <row r="232" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B232" s="2"/>
       <c r="C232" s="2"/>
       <c r="D232" s="8"/>
     </row>
-    <row r="233" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B233" s="2"/>
       <c r="C233" s="2"/>
       <c r="D233" s="8"/>
     </row>
-    <row r="234" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B234" s="2"/>
       <c r="C234" s="2"/>
       <c r="D234" s="8"/>
     </row>
-    <row r="235" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="235" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B235" s="2"/>
       <c r="C235" s="2"/>
       <c r="D235" s="8"/>
     </row>
-    <row r="236" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B236" s="2"/>
       <c r="C236" s="2"/>
       <c r="D236" s="8"/>
     </row>
-    <row r="237" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B237" s="2"/>
       <c r="C237" s="2"/>
       <c r="D237" s="8"/>
     </row>
-    <row r="238" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B238" s="2"/>
       <c r="C238" s="2"/>
       <c r="D238" s="8"/>
     </row>
-    <row r="239" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B239" s="2"/>
       <c r="C239" s="2"/>
       <c r="D239" s="8"/>
     </row>
-    <row r="240" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B240" s="2"/>
       <c r="C240" s="2"/>
       <c r="D240" s="8"/>
     </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B241" s="2"/>
       <c r="C241" s="2"/>
       <c r="D241" s="8"/>
     </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B242" s="2"/>
       <c r="C242" s="2"/>
       <c r="D242" s="8"/>
     </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B243" s="2"/>
       <c r="C243" s="2"/>
       <c r="D243" s="8"/>
     </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
       <c r="D244" s="8"/>
     </row>
-    <row r="245" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B245" s="2"/>
       <c r="C245" s="2"/>
       <c r="D245" s="8"/>
     </row>
-    <row r="246" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
       <c r="D246" s="8"/>
     </row>
-    <row r="247" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
       <c r="D247" s="8"/>
     </row>
-    <row r="248" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
       <c r="D248" s="8"/>
     </row>
-    <row r="249" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="249" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B249" s="2"/>
       <c r="C249" s="2"/>
       <c r="D249" s="8"/>
     </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="250" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
       <c r="D250" s="8"/>
     </row>
-    <row r="251" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="251" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
       <c r="D251" s="8"/>
     </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="252" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
       <c r="D252" s="8"/>
     </row>
-    <row r="253" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="253" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
       <c r="D253" s="8"/>
     </row>
-    <row r="254" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="254" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
       <c r="D254" s="8"/>
     </row>
-    <row r="255" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="255" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
       <c r="D255" s="8"/>
     </row>
-    <row r="256" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="256" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
       <c r="D256" s="8"/>
     </row>
-    <row r="257" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="257" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
       <c r="D257" s="8"/>
     </row>
-    <row r="258" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="258" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
       <c r="D258" s="8"/>
     </row>
-    <row r="259" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="259" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B259" s="2"/>
       <c r="C259" s="2"/>
       <c r="D259" s="8"/>
     </row>
-    <row r="260" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="260" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
       <c r="D260" s="8"/>
     </row>
-    <row r="261" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="261" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>
       <c r="D261" s="8"/>
     </row>
-    <row r="262" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="262" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B262" s="2"/>
       <c r="C262" s="2"/>
       <c r="D262" s="8"/>
     </row>
-    <row r="263" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="263" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B263" s="2"/>
       <c r="C263" s="2"/>
       <c r="D263" s="8"/>
     </row>
-    <row r="264" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="264" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
       <c r="D264" s="8"/>
     </row>
-    <row r="265" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="265" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B265" s="2"/>
       <c r="C265" s="2"/>
       <c r="D265" s="8"/>
     </row>
-    <row r="266" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="266" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B266" s="2"/>
       <c r="C266" s="2"/>
       <c r="D266" s="8"/>
     </row>
-    <row r="267" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="267" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B267" s="2"/>
       <c r="C267" s="2"/>
       <c r="D267" s="8"/>
     </row>
-    <row r="268" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="268" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B268" s="2"/>
       <c r="C268" s="2"/>
       <c r="D268" s="8"/>
     </row>
-    <row r="269" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="269" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B269" s="2"/>
       <c r="C269" s="2"/>
       <c r="D269" s="8"/>
     </row>
-    <row r="270" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="270" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B270" s="2"/>
       <c r="C270" s="2"/>
       <c r="D270" s="8"/>
     </row>
-    <row r="271" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="271" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B271" s="2"/>
       <c r="C271" s="2"/>
       <c r="D271" s="8"/>
     </row>
-    <row r="272" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="272" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B272" s="2"/>
       <c r="C272" s="2"/>
       <c r="D272" s="8"/>
     </row>
-    <row r="273" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="273" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B273" s="2"/>
       <c r="C273" s="2"/>
       <c r="D273" s="8"/>
     </row>
-    <row r="274" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="274" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B274" s="2"/>
       <c r="C274" s="2"/>
       <c r="D274" s="8"/>
     </row>
-    <row r="275" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="275" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B275" s="2"/>
       <c r="C275" s="2"/>
       <c r="D275" s="8"/>
     </row>
-    <row r="276" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="276" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B276" s="2"/>
       <c r="C276" s="2"/>
       <c r="D276" s="8"/>
     </row>
-    <row r="277" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="277" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B277" s="2"/>
       <c r="C277" s="2"/>
       <c r="D277" s="8"/>
     </row>
-    <row r="278" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="278" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B278" s="2"/>
       <c r="C278" s="2"/>
       <c r="D278" s="8"/>
     </row>
-    <row r="279" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="279" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B279" s="2"/>
       <c r="C279" s="2"/>
       <c r="D279" s="8"/>
     </row>
-    <row r="280" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="280" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B280" s="2"/>
       <c r="C280" s="2"/>
       <c r="D280" s="8"/>
     </row>
-    <row r="281" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="281" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B281" s="2"/>
       <c r="C281" s="2"/>
       <c r="D281" s="8"/>
     </row>
-    <row r="282" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="282" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B282" s="2"/>
       <c r="C282" s="2"/>
       <c r="D282" s="8"/>
     </row>
-    <row r="283" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="283" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B283" s="2"/>
       <c r="C283" s="2"/>
       <c r="D283" s="8"/>
     </row>
-    <row r="284" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="284" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B284" s="2"/>
       <c r="C284" s="2"/>
       <c r="D284" s="8"/>
     </row>
-    <row r="285" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="285" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B285" s="2"/>
       <c r="C285" s="2"/>
       <c r="D285" s="8"/>
     </row>
-    <row r="286" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="286" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B286" s="2"/>
       <c r="C286" s="2"/>
       <c r="D286" s="8"/>
     </row>
-    <row r="287" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="287" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B287" s="2"/>
       <c r="C287" s="2"/>
       <c r="D287" s="8"/>
     </row>
-    <row r="288" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="288" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B288" s="2"/>
       <c r="C288" s="2"/>
       <c r="D288" s="8"/>
     </row>
-    <row r="289" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="289" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B289" s="2"/>
       <c r="C289" s="2"/>
       <c r="D289" s="8"/>
     </row>
-    <row r="290" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="290" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B290" s="2"/>
       <c r="C290" s="2"/>
       <c r="D290" s="8"/>
     </row>
-    <row r="291" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="291" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B291" s="2"/>
       <c r="C291" s="2"/>
       <c r="D291" s="8"/>
     </row>
-    <row r="292" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="292" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B292" s="2"/>
       <c r="C292" s="2"/>
       <c r="D292" s="8"/>
     </row>
-    <row r="293" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="293" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B293" s="2"/>
       <c r="C293" s="2"/>
       <c r="D293" s="8"/>
     </row>
-    <row r="294" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="294" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B294" s="2"/>
       <c r="C294" s="2"/>
       <c r="D294" s="8"/>
     </row>
-    <row r="295" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="295" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B295" s="2"/>
       <c r="C295" s="2"/>
       <c r="D295" s="8"/>
     </row>
-    <row r="296" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="296" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B296" s="2"/>
       <c r="C296" s="2"/>
       <c r="D296" s="8"/>
     </row>
-    <row r="297" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="297" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B297" s="2"/>
       <c r="C297" s="2"/>
       <c r="D297" s="8"/>
     </row>
-    <row r="298" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="298" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B298" s="2"/>
       <c r="C298" s="2"/>
       <c r="D298" s="8"/>
     </row>
-    <row r="299" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="299" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B299" s="2"/>
       <c r="C299" s="2"/>
       <c r="D299" s="8"/>
     </row>
-    <row r="300" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="300" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B300" s="2"/>
       <c r="C300" s="2"/>
       <c r="D300" s="8"/>
     </row>
-    <row r="301" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="301" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B301" s="2"/>
       <c r="C301" s="2"/>
       <c r="D301" s="8"/>
     </row>
-    <row r="302" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="302" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B302" s="2"/>
       <c r="C302" s="2"/>
       <c r="D302" s="8"/>
     </row>
-    <row r="303" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="303" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B303" s="2"/>
       <c r="C303" s="2"/>
       <c r="D303" s="8"/>
     </row>
-    <row r="304" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="304" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B304" s="2"/>
       <c r="C304" s="2"/>
       <c r="D304" s="8"/>
     </row>
-    <row r="305" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="305" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B305" s="2"/>
       <c r="C305" s="2"/>
       <c r="D305" s="8"/>
     </row>
-    <row r="306" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="306" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B306" s="2"/>
       <c r="C306" s="2"/>
       <c r="D306" s="8"/>
     </row>
-    <row r="307" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="307" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B307" s="2"/>
       <c r="C307" s="2"/>
       <c r="D307" s="8"/>
     </row>
-    <row r="308" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="308" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B308" s="2"/>
       <c r="C308" s="2"/>
       <c r="D308" s="8"/>
     </row>
-    <row r="309" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="309" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B309" s="2"/>
       <c r="C309" s="2"/>
       <c r="D309" s="8"/>
     </row>
-    <row r="310" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="310" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B310" s="2"/>
       <c r="C310" s="2"/>
       <c r="D310" s="8"/>
     </row>
-    <row r="311" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="311" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B311" s="2"/>
       <c r="C311" s="2"/>
       <c r="D311" s="8"/>
     </row>
-    <row r="312" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="312" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B312" s="2"/>
       <c r="C312" s="2"/>
       <c r="D312" s="8"/>
     </row>
-    <row r="313" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="313" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B313" s="2"/>
       <c r="C313" s="2"/>
       <c r="D313" s="8"/>
     </row>
-    <row r="314" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="314" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B314" s="2"/>
       <c r="C314" s="2"/>
       <c r="D314" s="8"/>
     </row>
-    <row r="315" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="315" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B315" s="2"/>
       <c r="C315" s="2"/>
       <c r="D315" s="8"/>
     </row>
-    <row r="316" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="316" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B316" s="2"/>
       <c r="C316" s="2"/>
       <c r="D316" s="8"/>
     </row>
-    <row r="317" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="317" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B317" s="2"/>
       <c r="C317" s="2"/>
       <c r="D317" s="8"/>
     </row>
-    <row r="318" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="318" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B318" s="2"/>
       <c r="C318" s="2"/>
       <c r="D318" s="8"/>
     </row>
-    <row r="319" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="319" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B319" s="2"/>
       <c r="C319" s="2"/>
       <c r="D319" s="8"/>
     </row>
-    <row r="320" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="320" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B320" s="2"/>
       <c r="C320" s="2"/>
       <c r="D320" s="8"/>
     </row>
-    <row r="321" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="321" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B321" s="2"/>
       <c r="C321" s="2"/>
       <c r="D321" s="8"/>
     </row>
-    <row r="322" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="322" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B322" s="2"/>
       <c r="C322" s="2"/>
       <c r="D322" s="8"/>
     </row>
-    <row r="323" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="323" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B323" s="2"/>
       <c r="C323" s="2"/>
       <c r="D323" s="8"/>
     </row>
-    <row r="324" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="324" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B324" s="2"/>
       <c r="C324" s="2"/>
       <c r="D324" s="8"/>
     </row>
-    <row r="325" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="325" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B325" s="2"/>
       <c r="C325" s="2"/>
       <c r="D325" s="8"/>
     </row>
-    <row r="326" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="326" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B326" s="2"/>
       <c r="C326" s="2"/>
       <c r="D326" s="8"/>
     </row>
-    <row r="327" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="327" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B327" s="2"/>
       <c r="C327" s="2"/>
       <c r="D327" s="8"/>
     </row>
-    <row r="328" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="328" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B328" s="2"/>
       <c r="C328" s="2"/>
       <c r="D328" s="8"/>
     </row>
-    <row r="329" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="329" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B329" s="2"/>
       <c r="C329" s="2"/>
       <c r="D329" s="8"/>
     </row>
-    <row r="330" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="330" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B330" s="2"/>
       <c r="C330" s="2"/>
       <c r="D330" s="8"/>
     </row>
-    <row r="331" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="331" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B331" s="2"/>
       <c r="C331" s="2"/>
       <c r="D331" s="8"/>
     </row>
-    <row r="332" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="332" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B332" s="2"/>
       <c r="C332" s="2"/>
       <c r="D332" s="8"/>
     </row>
-    <row r="333" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="333" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B333" s="2"/>
       <c r="C333" s="2"/>
       <c r="D333" s="8"/>
     </row>
-    <row r="334" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="334" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B334" s="2"/>
       <c r="C334" s="2"/>
       <c r="D334" s="8"/>
     </row>
-    <row r="335" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="335" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B335" s="2"/>
       <c r="C335" s="2"/>
       <c r="D335" s="8"/>
     </row>
-    <row r="336" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="336" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B336" s="2"/>
       <c r="C336" s="2"/>
       <c r="D336" s="8"/>
     </row>
-    <row r="337" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="337" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B337" s="2"/>
       <c r="C337" s="2"/>
       <c r="D337" s="8"/>
     </row>
-    <row r="338" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="338" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B338" s="2"/>
       <c r="C338" s="2"/>
       <c r="D338" s="8"/>
     </row>
-    <row r="339" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="339" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B339" s="2"/>
       <c r="C339" s="2"/>
       <c r="D339" s="8"/>
     </row>
-    <row r="340" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="340" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B340" s="2"/>
       <c r="C340" s="2"/>
       <c r="D340" s="8"/>
     </row>
-    <row r="341" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="341" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B341" s="2"/>
       <c r="C341" s="2"/>
       <c r="D341" s="8"/>
     </row>
-    <row r="342" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="342" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B342" s="2"/>
       <c r="C342" s="2"/>
       <c r="D342" s="8"/>
     </row>
-    <row r="343" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="343" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B343" s="2"/>
       <c r="C343" s="2"/>
       <c r="D343" s="8"/>
     </row>
-    <row r="344" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="344" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B344" s="2"/>
       <c r="C344" s="2"/>
       <c r="D344" s="8"/>
     </row>
-    <row r="345" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="345" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B345" s="2"/>
       <c r="C345" s="2"/>
       <c r="D345" s="8"/>
     </row>
-    <row r="346" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="346" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B346" s="2"/>
       <c r="C346" s="2"/>
       <c r="D346" s="8"/>
     </row>
-    <row r="347" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="347" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B347" s="2"/>
       <c r="C347" s="2"/>
       <c r="D347" s="8"/>
     </row>
-    <row r="348" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="348" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B348" s="2"/>
       <c r="C348" s="2"/>
       <c r="D348" s="8"/>
     </row>
-    <row r="349" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="349" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B349" s="2"/>
       <c r="C349" s="2"/>
       <c r="D349" s="8"/>
     </row>
-    <row r="350" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="350" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B350" s="2"/>
       <c r="C350" s="2"/>
       <c r="D350" s="8"/>
     </row>
-    <row r="351" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="351" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B351" s="2"/>
       <c r="C351" s="2"/>
       <c r="D351" s="8"/>
     </row>
-    <row r="352" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="352" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B352" s="2"/>
       <c r="C352" s="2"/>
       <c r="D352" s="8"/>
     </row>
-    <row r="353" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="353" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B353" s="2"/>
       <c r="C353" s="2"/>
       <c r="D353" s="8"/>
     </row>
-    <row r="354" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="354" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B354" s="2"/>
       <c r="C354" s="2"/>
       <c r="D354" s="8"/>
     </row>
-    <row r="355" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="355" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B355" s="2"/>
       <c r="C355" s="2"/>
       <c r="D355" s="8"/>
     </row>
-    <row r="356" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="356" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B356" s="2"/>
       <c r="C356" s="2"/>
       <c r="D356" s="8"/>
     </row>
-    <row r="357" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="357" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B357" s="2"/>
       <c r="C357" s="2"/>
       <c r="D357" s="8"/>
     </row>
-    <row r="358" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="358" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B358" s="2"/>
       <c r="C358" s="2"/>
       <c r="D358" s="8"/>
     </row>
-    <row r="359" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="359" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B359" s="2"/>
       <c r="C359" s="2"/>
       <c r="D359" s="8"/>
     </row>
-    <row r="360" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="360" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B360" s="2"/>
       <c r="C360" s="2"/>
       <c r="D360" s="8"/>
     </row>
-    <row r="361" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="361" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B361" s="2"/>
       <c r="C361" s="2"/>
       <c r="D361" s="8"/>
     </row>
-    <row r="362" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="362" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B362" s="2"/>
       <c r="C362" s="2"/>
       <c r="D362" s="8"/>
     </row>
-    <row r="363" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="363" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B363" s="2"/>
       <c r="C363" s="2"/>
       <c r="D363" s="8"/>
     </row>
-    <row r="364" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="364" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B364" s="2"/>
       <c r="C364" s="2"/>
       <c r="D364" s="8"/>
     </row>
-    <row r="365" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="365" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B365" s="2"/>
       <c r="C365" s="2"/>
       <c r="D365" s="8"/>
     </row>
-    <row r="366" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="366" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B366" s="2"/>
       <c r="C366" s="2"/>
       <c r="D366" s="8"/>
     </row>
-    <row r="367" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="367" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B367" s="2"/>
       <c r="C367" s="2"/>
       <c r="D367" s="8"/>
     </row>
-    <row r="368" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="368" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B368" s="2"/>
       <c r="C368" s="2"/>
       <c r="D368" s="8"/>
     </row>
-    <row r="369" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="369" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B369" s="2"/>
       <c r="C369" s="2"/>
       <c r="D369" s="8"/>
     </row>
-    <row r="370" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="370" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B370" s="2"/>
       <c r="C370" s="2"/>
       <c r="D370" s="8"/>
     </row>
-    <row r="371" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="371" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B371" s="2"/>
       <c r="C371" s="2"/>
       <c r="D371" s="8"/>
     </row>
-    <row r="372" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="372" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B372" s="2"/>
       <c r="C372" s="2"/>
       <c r="D372" s="8"/>
     </row>
-    <row r="373" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="373" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B373" s="2"/>
       <c r="C373" s="2"/>
       <c r="D373" s="8"/>
     </row>
-    <row r="374" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="374" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B374" s="2"/>
       <c r="C374" s="2"/>
       <c r="D374" s="8"/>
     </row>
-    <row r="375" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="375" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B375" s="2"/>
       <c r="C375" s="2"/>
       <c r="D375" s="8"/>
     </row>
-    <row r="376" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="376" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B376" s="2"/>
       <c r="C376" s="2"/>
       <c r="D376" s="8"/>
     </row>
-    <row r="377" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="377" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B377" s="2"/>
       <c r="C377" s="2"/>
       <c r="D377" s="8"/>
     </row>
-    <row r="378" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="378" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B378" s="2"/>
       <c r="C378" s="2"/>
       <c r="D378" s="8"/>
     </row>
-    <row r="379" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="379" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B379" s="2"/>
       <c r="C379" s="2"/>
       <c r="D379" s="8"/>
     </row>
-    <row r="380" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="380" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B380" s="2"/>
       <c r="C380" s="2"/>
       <c r="D380" s="8"/>
     </row>
-    <row r="381" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="381" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B381" s="2"/>
       <c r="C381" s="2"/>
       <c r="D381" s="8"/>
     </row>
-    <row r="382" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="382" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B382" s="2"/>
       <c r="C382" s="2"/>
       <c r="D382" s="8"/>
     </row>
-    <row r="383" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="383" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B383" s="2"/>
       <c r="C383" s="2"/>
       <c r="D383" s="8"/>
     </row>
-    <row r="384" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="384" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B384" s="2"/>
       <c r="C384" s="2"/>
       <c r="D384" s="8"/>
     </row>
-    <row r="385" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="385" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B385" s="2"/>
       <c r="C385" s="2"/>
       <c r="D385" s="8"/>
     </row>
-    <row r="386" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="386" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B386" s="2"/>
       <c r="C386" s="2"/>
       <c r="D386" s="8"/>
     </row>
-    <row r="387" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="387" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B387" s="2"/>
       <c r="C387" s="2"/>
       <c r="D387" s="8"/>
     </row>
-    <row r="388" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="388" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B388" s="2"/>
       <c r="C388" s="2"/>
       <c r="D388" s="8"/>
     </row>
-    <row r="389" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="389" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B389" s="2"/>
       <c r="C389" s="2"/>
       <c r="D389" s="8"/>
     </row>
-    <row r="390" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="390" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B390" s="2"/>
       <c r="C390" s="2"/>
       <c r="D390" s="8"/>
     </row>
-    <row r="391" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="391" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B391" s="2"/>
       <c r="C391" s="2"/>
       <c r="D391" s="8"/>
     </row>
-    <row r="392" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="392" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B392" s="2"/>
       <c r="C392" s="2"/>
       <c r="D392" s="8"/>
     </row>
-    <row r="393" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="393" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B393" s="2"/>
       <c r="C393" s="2"/>
       <c r="D393" s="8"/>
     </row>
-    <row r="394" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="394" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B394" s="2"/>
       <c r="C394" s="2"/>
       <c r="D394" s="8"/>
     </row>
-    <row r="395" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="395" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B395" s="2"/>
       <c r="C395" s="2"/>
       <c r="D395" s="8"/>
     </row>
-    <row r="396" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="396" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B396" s="2"/>
       <c r="C396" s="2"/>
       <c r="D396" s="8"/>
     </row>
-    <row r="397" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="397" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B397" s="2"/>
       <c r="C397" s="2"/>
       <c r="D397" s="8"/>
     </row>
-    <row r="398" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="398" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B398" s="2"/>
       <c r="C398" s="2"/>
       <c r="D398" s="8"/>
     </row>
-    <row r="399" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="399" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B399" s="2"/>
       <c r="C399" s="2"/>
       <c r="D399" s="8"/>
     </row>
-    <row r="400" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="400" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B400" s="2"/>
       <c r="C400" s="2"/>
       <c r="D400" s="8"/>
     </row>
-    <row r="401" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="401" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B401" s="2"/>
       <c r="C401" s="2"/>
       <c r="D401" s="8"/>
     </row>
-    <row r="402" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="402" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B402" s="2"/>
       <c r="C402" s="2"/>
       <c r="D402" s="8"/>
     </row>
-    <row r="403" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="403" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B403" s="2"/>
       <c r="C403" s="2"/>
       <c r="D403" s="8"/>
     </row>
-    <row r="404" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="404" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D404" s="8"/>
     </row>
-    <row r="405" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="405" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D405" s="8"/>
     </row>
-    <row r="406" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="406" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D406" s="8"/>
     </row>
-    <row r="407" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="407" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D407" s="8"/>
     </row>
-    <row r="408" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="408" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D408" s="8"/>
     </row>
-    <row r="409" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="409" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D409" s="8"/>
     </row>
-    <row r="410" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="410" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D410" s="8"/>
     </row>
-    <row r="411" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="411" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D411" s="8"/>
     </row>
-    <row r="412" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="412" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D412" s="8"/>
     </row>
-    <row r="413" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="413" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D413" s="8"/>
     </row>
-    <row r="414" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="414" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D414" s="8"/>
     </row>
-    <row r="415" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="415" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D415" s="8"/>
     </row>
-    <row r="416" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="416" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D416" s="8"/>
     </row>
-    <row r="417" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="417" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D417" s="8"/>
     </row>
-    <row r="418" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="418" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D418" s="8"/>
     </row>
-    <row r="419" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="419" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D419" s="8"/>
     </row>
-    <row r="420" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="420" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D420" s="8"/>
     </row>
-    <row r="421" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="421" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D421" s="8"/>
     </row>
-    <row r="422" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="422" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D422" s="8"/>
     </row>
-    <row r="423" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="423" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D423" s="8"/>
     </row>
-    <row r="424" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="424" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D424" s="8"/>
     </row>
-    <row r="425" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="425" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D425" s="8"/>
     </row>
-    <row r="426" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="426" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D426" s="8"/>
     </row>
-    <row r="427" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="427" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D427" s="8"/>
     </row>
-    <row r="428" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="428" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D428" s="8"/>
     </row>
-    <row r="429" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="429" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D429" s="8"/>
     </row>
-    <row r="430" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="430" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D430" s="8"/>
     </row>
-    <row r="431" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="431" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D431" s="8"/>
     </row>
-    <row r="432" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="432" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D432" s="8"/>
     </row>
-    <row r="433" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="433" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D433" s="8"/>
     </row>
-    <row r="434" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="434" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D434" s="8"/>
     </row>
-    <row r="435" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="435" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D435" s="8"/>
     </row>
-    <row r="436" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="436" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D436" s="8"/>
     </row>
-    <row r="437" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="437" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D437" s="8"/>
     </row>
-    <row r="438" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="438" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D438" s="8"/>
     </row>
-    <row r="439" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="439" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D439" s="8"/>
     </row>
-    <row r="440" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="440" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D440" s="8"/>
     </row>
-    <row r="441" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="441" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D441" s="8"/>
     </row>
-    <row r="442" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="442" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D442" s="8"/>
     </row>
-    <row r="443" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="443" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D443" s="8"/>
     </row>
-    <row r="444" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="444" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D444" s="8"/>
     </row>
-    <row r="445" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="445" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D445" s="8"/>
     </row>
-    <row r="446" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="446" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D446" s="8"/>
     </row>
-    <row r="447" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="447" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D447" s="8"/>
     </row>
-    <row r="448" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="448" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D448" s="8"/>
     </row>
-    <row r="449" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="449" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D449" s="8"/>
     </row>
-    <row r="450" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="450" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D450" s="8"/>
     </row>
-    <row r="451" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="451" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D451" s="8"/>
     </row>
-    <row r="452" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="452" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D452" s="8"/>
     </row>
-    <row r="453" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="453" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D453" s="8"/>
     </row>
-    <row r="454" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="454" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D454" s="8"/>
     </row>
-    <row r="455" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="455" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D455" s="8"/>
     </row>
-    <row r="456" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="456" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D456" s="8"/>
     </row>
-    <row r="457" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="457" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D457" s="8"/>
     </row>
-    <row r="458" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="458" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D458" s="8"/>
     </row>
-    <row r="459" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="459" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D459" s="8"/>
     </row>
-    <row r="460" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="460" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D460" s="8"/>
     </row>
-    <row r="461" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="461" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D461" s="8"/>
     </row>
-    <row r="462" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="462" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D462" s="8"/>
     </row>
-    <row r="463" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="463" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D463" s="8"/>
     </row>
-    <row r="464" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="464" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D464" s="8"/>
     </row>
-    <row r="465" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="465" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D465" s="8"/>
     </row>
-    <row r="466" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="466" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D466" s="8"/>
     </row>
-    <row r="467" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="467" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D467" s="8"/>
     </row>
-    <row r="468" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="468" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D468" s="8"/>
     </row>
-    <row r="469" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="469" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D469" s="8"/>
     </row>
-    <row r="470" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="470" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D470" s="8"/>
     </row>
-    <row r="471" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="471" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D471" s="8"/>
     </row>
-    <row r="472" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="472" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D472" s="8"/>
     </row>
-    <row r="473" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="473" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D473" s="8"/>
     </row>
-    <row r="474" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="474" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D474" s="8"/>
     </row>
-    <row r="475" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="475" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D475" s="8"/>
     </row>
-    <row r="476" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="476" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D476" s="8"/>
     </row>
-    <row r="477" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="477" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D477" s="8"/>
     </row>
-    <row r="478" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="478" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D478" s="8"/>
     </row>
-    <row r="479" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="479" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D479" s="8"/>
     </row>
-    <row r="480" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="480" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D480" s="8"/>
     </row>
-    <row r="481" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="481" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D481" s="8"/>
     </row>
-    <row r="482" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="482" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D482" s="8"/>
     </row>
-    <row r="483" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="483" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D483" s="8"/>
     </row>
-    <row r="484" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="484" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D484" s="8"/>
     </row>
-    <row r="485" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="485" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D485" s="8"/>
     </row>
-    <row r="486" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="486" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D486" s="8"/>
     </row>
-    <row r="487" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="487" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D487" s="8"/>
     </row>
-    <row r="488" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="488" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D488" s="8"/>
     </row>
-    <row r="489" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="489" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D489" s="8"/>
     </row>
-    <row r="490" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="490" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D490" s="8"/>
     </row>
-    <row r="491" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="491" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D491" s="8"/>
     </row>
-    <row r="492" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="492" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D492" s="8"/>
     </row>
-    <row r="493" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="493" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D493" s="8"/>
     </row>
-    <row r="494" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="494" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D494" s="8"/>
     </row>
-    <row r="495" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="495" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D495" s="8"/>
     </row>
-    <row r="496" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="496" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D496" s="8"/>
     </row>
-    <row r="497" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="497" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D497" s="8"/>
     </row>
-    <row r="498" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="498" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D498" s="8"/>
     </row>
-    <row r="499" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="499" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D499" s="8"/>
     </row>
-    <row r="500" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="500" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D500" s="8"/>
     </row>
-    <row r="501" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="501" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D501" s="8"/>
     </row>
-    <row r="502" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="502" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D502" s="8"/>
     </row>
-    <row r="503" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="503" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D503" s="8"/>
     </row>
-    <row r="504" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="504" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D504" s="8"/>
     </row>
-    <row r="505" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="505" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D505" s="8"/>
     </row>
-    <row r="506" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="506" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D506" s="8"/>
     </row>
-    <row r="507" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="507" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D507" s="8"/>
     </row>
-    <row r="508" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="508" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D508" s="8"/>
     </row>
-    <row r="509" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="509" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D509" s="8"/>
     </row>
-    <row r="510" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="510" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D510" s="8"/>
     </row>
-    <row r="511" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="511" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D511" s="8"/>
     </row>
-    <row r="512" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="512" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D512" s="8"/>
     </row>
-    <row r="513" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="513" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D513" s="8"/>
     </row>
-    <row r="514" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="514" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D514" s="8"/>
     </row>
-    <row r="515" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="515" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D515" s="8"/>
     </row>
-    <row r="516" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="516" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D516" s="8"/>
     </row>
-    <row r="517" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="517" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D517" s="8"/>
     </row>
-    <row r="518" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="518" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D518" s="8"/>
     </row>
-    <row r="519" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="519" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D519" s="8"/>
     </row>
-    <row r="520" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="520" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D520" s="8"/>
     </row>
-    <row r="521" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="521" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D521" s="8"/>
     </row>
-    <row r="522" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="522" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D522" s="8"/>
     </row>
-    <row r="523" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="523" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D523" s="8"/>
     </row>
-    <row r="524" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="524" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D524" s="8"/>
     </row>
-    <row r="525" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="525" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D525" s="8"/>
     </row>
-    <row r="526" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="526" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D526" s="8"/>
     </row>
-    <row r="527" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="527" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D527" s="8"/>
     </row>
-    <row r="528" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="528" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D528" s="8"/>
     </row>
-    <row r="529" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="529" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D529" s="8"/>
     </row>
-    <row r="530" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="530" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D530" s="8"/>
     </row>
-    <row r="531" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="531" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D531" s="8"/>
     </row>
-    <row r="532" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="532" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D532" s="8"/>
     </row>
-    <row r="533" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="533" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D533" s="8"/>
     </row>
-    <row r="534" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="534" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D534" s="8"/>
     </row>
-    <row r="535" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="535" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D535" s="8"/>
     </row>
-    <row r="536" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="536" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D536" s="8"/>
     </row>
-    <row r="537" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="537" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D537" s="8"/>
     </row>
-    <row r="538" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="538" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D538" s="8"/>
     </row>
-    <row r="539" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="539" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D539" s="8"/>
     </row>
-    <row r="540" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="540" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D540" s="8"/>
     </row>
-    <row r="541" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="541" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D541" s="8"/>
     </row>
-    <row r="542" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="542" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D542" s="8"/>
     </row>
-    <row r="543" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="543" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D543" s="8"/>
     </row>
-    <row r="544" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="544" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D544" s="8"/>
     </row>
-    <row r="545" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="545" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D545" s="8"/>
     </row>
-    <row r="546" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="546" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D546" s="8"/>
     </row>
-    <row r="547" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="547" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D547" s="8"/>
     </row>
-    <row r="548" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="548" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D548" s="8"/>
     </row>
-    <row r="549" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="549" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D549" s="8"/>
     </row>
-    <row r="550" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="550" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D550" s="8"/>
     </row>
-    <row r="551" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="551" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D551" s="8"/>
     </row>
-    <row r="552" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="552" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D552" s="8"/>
     </row>
-    <row r="553" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="553" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D553" s="8"/>
     </row>
-    <row r="554" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="554" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D554" s="8"/>
     </row>
-    <row r="555" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="555" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D555" s="8"/>
     </row>
-    <row r="556" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="556" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D556" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
free fill box operator in excel template hs code is nullable multiline text in cargo description change container list font to courier new weight and volume number format to 2 decimal places with comma separator
</commit_message>
<xml_diff>
--- a/public/template/shipping_instruction_template.xlsx
+++ b/public/template/shipping_instruction_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\MyLaravelApps\gus-automate\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2F77B8-D023-4838-9644-411FF560B3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECC46FD-C578-474C-93AF-9647867CA658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{378D42B6-8EFA-4EF6-9C50-436D539EEED8}"/>
+    <workbookView xWindow="4560" yWindow="2310" windowWidth="23790" windowHeight="19290" xr2:uid="{378D42B6-8EFA-4EF6-9C50-436D539EEED8}"/>
   </bookViews>
   <sheets>
     <sheet name="BillOfLading" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>BOX OPERATOR</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>NOTIFY PARTY CONTACT</t>
-  </si>
-  <si>
-    <t>EVERGREEN</t>
   </si>
   <si>
     <t>GROSS WEIGHT (KGS)</t>
@@ -197,7 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -248,11 +245,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -882,7 +875,7 @@
   <dimension ref="B2:H556"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -901,9 +894,7 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>16</v>
-      </c>
+      <c r="C2" s="13"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
@@ -1000,7 +991,7 @@
         <v>12</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>7</v>
@@ -1019,56 +1010,56 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
-      <c r="E20" s="18"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="9"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="18"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="9"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="18"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="9"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="18"/>
+      <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
-      <c r="E24" s="18"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
-      <c r="E25" s="18"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="18"/>
+      <c r="E26" s="9"/>
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
-      <c r="E27" s="18"/>
+      <c r="E27" s="9"/>
       <c r="F27" s="9"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.35">
@@ -3412,14 +3403,8 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="1">
-    <mergeCell ref="E19:E27"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2" xr:uid="{B78CC3E9-3AD1-4ADD-ADE6-D3BE0B9CCE5F}">
-      <formula1>"Titanium OOCL,EVERGREEN,NAVEGACION"</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D19:D556" xr:uid="{A1576279-0AF6-4A01-B086-277E31EECE1F}">
       <formula1>"40HC, 20DC"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
update telex bill of lading template update excel template
</commit_message>
<xml_diff>
--- a/public/template/shipping_instruction_template.xlsx
+++ b/public/template/shipping_instruction_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\MyLaravelApps\gus-automate\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECC46FD-C578-474C-93AF-9647867CA658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DE7767-B062-43BD-829B-A543E2C354C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="2310" windowWidth="23790" windowHeight="19290" xr2:uid="{378D42B6-8EFA-4EF6-9C50-436D539EEED8}"/>
+    <workbookView xWindow="40820" yWindow="1200" windowWidth="23790" windowHeight="19290" xr2:uid="{378D42B6-8EFA-4EF6-9C50-436D539EEED8}"/>
   </bookViews>
   <sheets>
     <sheet name="BillOfLading" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -245,6 +245,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -875,7 +879,7 @@
   <dimension ref="B2:H556"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="E19" sqref="E19:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1010,56 +1014,56 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
-      <c r="E20" s="9"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="9"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="9"/>
+      <c r="E21" s="18"/>
       <c r="F21" s="9"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="9"/>
+      <c r="E22" s="18"/>
       <c r="F22" s="9"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="9"/>
+      <c r="E23" s="18"/>
       <c r="F23" s="9"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
-      <c r="E24" s="9"/>
+      <c r="E24" s="18"/>
       <c r="F24" s="9"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
-      <c r="E25" s="9"/>
+      <c r="E25" s="18"/>
       <c r="F25" s="9"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="9"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
-      <c r="E27" s="9"/>
+      <c r="E27" s="18"/>
       <c r="F27" s="9"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.35">
@@ -3403,6 +3407,9 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="E19:E27"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D19:D556" xr:uid="{A1576279-0AF6-4A01-B086-277E31EECE1F}">

</xml_diff>